<commit_message>
Added script for making a character array to indicate task order and saving this with other information to the task info csv
</commit_message>
<xml_diff>
--- a/PsychoPyData_ColumnKey.xlsx
+++ b/PsychoPyData_ColumnKey.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1738" documentId="8_{447AABAE-0265-45CA-9969-8E24E37FF3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECCC3420-6B50-4F27-A63C-EB751776FFE5}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{5015AFB7-EBCA-4E4E-B1B8-96F1F0B54514}"/>
+    <workbookView xWindow="8214" yWindow="168" windowWidth="14442" windowHeight="8124" xr2:uid="{5015AFB7-EBCA-4E4E-B1B8-96F1F0B54514}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2556,10 +2556,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2573,21 +2588,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2954,10 +2954,10 @@
   <dimension ref="A1:N372"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2997,12 +2997,12 @@
       <c r="H1" t="s">
         <v>335</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="23" t="s">
         <v>799</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
@@ -3020,10 +3020,10 @@
       <c r="H2" t="s">
         <v>632</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
@@ -3041,10 +3041,10 @@
       <c r="H3" t="s">
         <v>633</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -3062,10 +3062,10 @@
       <c r="H4" t="s">
         <v>632</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
@@ -3083,10 +3083,10 @@
       <c r="H5" t="s">
         <v>632</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
@@ -3104,10 +3104,10 @@
       <c r="H6" t="s">
         <v>632</v>
       </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -3125,10 +3125,10 @@
       <c r="H7" t="s">
         <v>632</v>
       </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
     </row>
     <row r="8" spans="1:12" s="12" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="12" t="s">
@@ -3147,16 +3147,16 @@
       <c r="H8" s="12" t="s">
         <v>632</v>
       </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
     </row>
     <row r="9" spans="1:12" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="19" t="s">
         <v>532</v>
       </c>
       <c r="E9" t="s">
@@ -3165,16 +3165,16 @@
       <c r="F9" t="s">
         <v>398</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="20"/>
       <c r="E10" t="s">
         <v>357</v>
       </c>
@@ -3184,16 +3184,16 @@
       <c r="H10" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="20"/>
       <c r="E11" t="s">
         <v>357</v>
       </c>
@@ -3203,16 +3203,16 @@
       <c r="H11" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="25"/>
+      <c r="C12" s="20"/>
       <c r="E12" t="s">
         <v>357</v>
       </c>
@@ -3222,16 +3222,16 @@
       <c r="H12" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="20"/>
       <c r="E13" t="s">
         <v>364</v>
       </c>
@@ -3243,7 +3243,7 @@
       <c r="A14" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="25"/>
+      <c r="C14" s="20"/>
       <c r="E14" t="s">
         <v>364</v>
       </c>
@@ -3258,7 +3258,7 @@
       <c r="A15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="25"/>
+      <c r="C15" s="20"/>
       <c r="E15" t="s">
         <v>364</v>
       </c>
@@ -3273,7 +3273,7 @@
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="25"/>
+      <c r="C16" s="20"/>
       <c r="E16" t="s">
         <v>364</v>
       </c>
@@ -3288,7 +3288,7 @@
       <c r="A17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="28"/>
+      <c r="C17" s="22"/>
       <c r="E17" s="12" t="s">
         <v>364</v>
       </c>
@@ -3303,7 +3303,7 @@
       <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="20" t="s">
         <v>533</v>
       </c>
       <c r="D18" t="s">
@@ -3323,7 +3323,7 @@
       <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="25"/>
+      <c r="C19" s="20"/>
       <c r="D19" t="s">
         <v>353</v>
       </c>
@@ -3341,7 +3341,7 @@
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="25"/>
+      <c r="C20" s="20"/>
       <c r="D20" t="s">
         <v>354</v>
       </c>
@@ -3362,7 +3362,7 @@
       <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="25"/>
+      <c r="C21" s="20"/>
       <c r="E21" t="s">
         <v>357</v>
       </c>
@@ -3374,7 +3374,7 @@
       <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="25"/>
+      <c r="C22" s="20"/>
       <c r="E22" t="s">
         <v>357</v>
       </c>
@@ -3389,7 +3389,7 @@
       <c r="A23" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="25"/>
+      <c r="C23" s="20"/>
       <c r="D23" t="s">
         <v>384</v>
       </c>
@@ -3410,7 +3410,7 @@
       <c r="A24" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="25"/>
+      <c r="C24" s="20"/>
       <c r="E24" t="s">
         <v>357</v>
       </c>
@@ -3422,7 +3422,7 @@
       <c r="A25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="26"/>
+      <c r="C25" s="21"/>
       <c r="E25" s="6" t="s">
         <v>364</v>
       </c>
@@ -3434,7 +3434,7 @@
       <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="19" t="s">
         <v>534</v>
       </c>
       <c r="D26" t="s">
@@ -3457,7 +3457,7 @@
       <c r="A27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="26"/>
+      <c r="C27" s="21"/>
       <c r="D27" s="6" t="s">
         <v>409</v>
       </c>
@@ -3478,7 +3478,7 @@
       <c r="A28" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="20" t="s">
         <v>535</v>
       </c>
       <c r="D28" t="s">
@@ -3501,7 +3501,7 @@
       <c r="A29" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="25"/>
+      <c r="C29" s="20"/>
       <c r="D29" t="s">
         <v>348</v>
       </c>
@@ -3519,7 +3519,7 @@
       <c r="A30" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="25"/>
+      <c r="C30" s="20"/>
       <c r="D30" t="s">
         <v>378</v>
       </c>
@@ -3537,7 +3537,7 @@
       <c r="A31" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="25"/>
+      <c r="C31" s="20"/>
       <c r="E31" t="s">
         <v>357</v>
       </c>
@@ -3549,7 +3549,7 @@
       <c r="A32" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="25"/>
+      <c r="C32" s="20"/>
       <c r="E32" t="s">
         <v>357</v>
       </c>
@@ -3561,7 +3561,7 @@
       <c r="A33" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="25"/>
+      <c r="C33" s="20"/>
       <c r="D33" t="s">
         <v>385</v>
       </c>
@@ -3582,7 +3582,7 @@
       <c r="A34" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="25"/>
+      <c r="C34" s="20"/>
       <c r="E34" t="s">
         <v>357</v>
       </c>
@@ -3594,7 +3594,7 @@
       <c r="A35" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="26"/>
+      <c r="C35" s="21"/>
       <c r="E35" s="6" t="s">
         <v>364</v>
       </c>
@@ -3606,7 +3606,7 @@
       <c r="A36" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="19" t="s">
         <v>536</v>
       </c>
       <c r="E36" t="s">
@@ -3620,7 +3620,7 @@
       <c r="A37" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="25"/>
+      <c r="C37" s="20"/>
       <c r="E37" t="s">
         <v>357</v>
       </c>
@@ -3632,7 +3632,7 @@
       <c r="A38" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="25"/>
+      <c r="C38" s="20"/>
       <c r="E38" t="s">
         <v>357</v>
       </c>
@@ -3644,7 +3644,7 @@
       <c r="A39" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="25"/>
+      <c r="C39" s="20"/>
       <c r="E39" t="s">
         <v>357</v>
       </c>
@@ -3656,7 +3656,7 @@
       <c r="A40" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="28"/>
+      <c r="C40" s="22"/>
       <c r="E40" s="12" t="s">
         <v>364</v>
       </c>
@@ -3668,7 +3668,7 @@
       <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="20" t="s">
         <v>537</v>
       </c>
       <c r="D41" t="s">
@@ -3691,7 +3691,7 @@
       <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="25"/>
+      <c r="C42" s="20"/>
       <c r="D42" t="s">
         <v>411</v>
       </c>
@@ -3712,7 +3712,7 @@
       <c r="A43" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="25"/>
+      <c r="C43" s="20"/>
       <c r="D43" t="s">
         <v>412</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="A44" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="25"/>
+      <c r="C44" s="20"/>
       <c r="E44" t="s">
         <v>357</v>
       </c>
@@ -3745,7 +3745,7 @@
       <c r="A45" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="25"/>
+      <c r="C45" s="20"/>
       <c r="E45" t="s">
         <v>357</v>
       </c>
@@ -3757,7 +3757,7 @@
       <c r="A46" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="25"/>
+      <c r="C46" s="20"/>
       <c r="D46" t="s">
         <v>413</v>
       </c>
@@ -3778,7 +3778,7 @@
       <c r="A47" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="25"/>
+      <c r="C47" s="20"/>
       <c r="E47" t="s">
         <v>357</v>
       </c>
@@ -3790,7 +3790,7 @@
       <c r="A48" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="26"/>
+      <c r="C48" s="21"/>
       <c r="E48" s="6" t="s">
         <v>364</v>
       </c>
@@ -3802,7 +3802,7 @@
       <c r="A49" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="19" t="s">
         <v>538</v>
       </c>
       <c r="D49" t="s">
@@ -3825,7 +3825,7 @@
       <c r="A50" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="26"/>
+      <c r="C50" s="21"/>
       <c r="D50" s="6" t="s">
         <v>422</v>
       </c>
@@ -3846,7 +3846,7 @@
       <c r="A51" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="19" t="s">
         <v>539</v>
       </c>
       <c r="D51" t="s">
@@ -3869,7 +3869,7 @@
       <c r="A52" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="25"/>
+      <c r="C52" s="20"/>
       <c r="D52" t="s">
         <v>415</v>
       </c>
@@ -3890,7 +3890,7 @@
       <c r="A53" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="25"/>
+      <c r="C53" s="20"/>
       <c r="D53" t="s">
         <v>416</v>
       </c>
@@ -3911,7 +3911,7 @@
       <c r="A54" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="25"/>
+      <c r="C54" s="20"/>
       <c r="E54" t="s">
         <v>357</v>
       </c>
@@ -3923,7 +3923,7 @@
       <c r="A55" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="25"/>
+      <c r="C55" s="20"/>
       <c r="E55" t="s">
         <v>357</v>
       </c>
@@ -3935,7 +3935,7 @@
       <c r="A56" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="25"/>
+      <c r="C56" s="20"/>
       <c r="D56" t="s">
         <v>417</v>
       </c>
@@ -3956,7 +3956,7 @@
       <c r="A57" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="25"/>
+      <c r="C57" s="20"/>
       <c r="E57" t="s">
         <v>357</v>
       </c>
@@ -3968,7 +3968,7 @@
       <c r="A58" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="26"/>
+      <c r="C58" s="21"/>
       <c r="E58" s="6" t="s">
         <v>364</v>
       </c>
@@ -3980,7 +3980,7 @@
       <c r="A59" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C59" s="19" t="s">
         <v>540</v>
       </c>
       <c r="E59" t="s">
@@ -3994,7 +3994,7 @@
       <c r="A60" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="25"/>
+      <c r="C60" s="20"/>
       <c r="E60" t="s">
         <v>357</v>
       </c>
@@ -4006,7 +4006,7 @@
       <c r="A61" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="25"/>
+      <c r="C61" s="20"/>
       <c r="E61" t="s">
         <v>357</v>
       </c>
@@ -4018,7 +4018,7 @@
       <c r="A62" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="25"/>
+      <c r="C62" s="20"/>
       <c r="E62" t="s">
         <v>357</v>
       </c>
@@ -4030,7 +4030,7 @@
       <c r="A63" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C63" s="26"/>
+      <c r="C63" s="21"/>
       <c r="E63" s="6" t="s">
         <v>364</v>
       </c>
@@ -4042,7 +4042,7 @@
       <c r="A64" t="s">
         <v>61</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C64" s="19" t="s">
         <v>541</v>
       </c>
       <c r="E64" t="s">
@@ -4056,7 +4056,7 @@
       <c r="A65" t="s">
         <v>62</v>
       </c>
-      <c r="C65" s="25"/>
+      <c r="C65" s="20"/>
       <c r="E65" t="s">
         <v>357</v>
       </c>
@@ -4068,7 +4068,7 @@
       <c r="A66" t="s">
         <v>63</v>
       </c>
-      <c r="C66" s="25"/>
+      <c r="C66" s="20"/>
       <c r="E66" t="s">
         <v>357</v>
       </c>
@@ -4083,7 +4083,7 @@
       <c r="A67" t="s">
         <v>64</v>
       </c>
-      <c r="C67" s="25"/>
+      <c r="C67" s="20"/>
       <c r="E67" t="s">
         <v>357</v>
       </c>
@@ -4098,7 +4098,7 @@
       <c r="A68" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C68" s="26"/>
+      <c r="C68" s="21"/>
       <c r="E68" s="6" t="s">
         <v>364</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="24" t="s">
+      <c r="C69" s="19" t="s">
         <v>542</v>
       </c>
       <c r="E69" t="s">
@@ -4129,7 +4129,7 @@
         <v>67</v>
       </c>
       <c r="B70" s="10"/>
-      <c r="C70" s="26"/>
+      <c r="C70" s="21"/>
       <c r="E70" s="6" t="s">
         <v>364</v>
       </c>
@@ -4144,7 +4144,7 @@
       <c r="A71" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="24" t="s">
+      <c r="C71" s="19" t="s">
         <v>543</v>
       </c>
       <c r="D71" t="s">
@@ -4167,7 +4167,7 @@
       <c r="A72" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="25"/>
+      <c r="C72" s="20"/>
       <c r="D72" t="s">
         <v>428</v>
       </c>
@@ -4188,7 +4188,7 @@
       <c r="A73" t="s">
         <v>70</v>
       </c>
-      <c r="C73" s="25"/>
+      <c r="C73" s="20"/>
       <c r="D73" t="s">
         <v>429</v>
       </c>
@@ -4209,7 +4209,7 @@
       <c r="A74" t="s">
         <v>71</v>
       </c>
-      <c r="C74" s="25"/>
+      <c r="C74" s="20"/>
       <c r="E74" t="s">
         <v>357</v>
       </c>
@@ -4221,7 +4221,7 @@
       <c r="A75" t="s">
         <v>72</v>
       </c>
-      <c r="C75" s="25"/>
+      <c r="C75" s="20"/>
       <c r="E75" t="s">
         <v>357</v>
       </c>
@@ -4233,7 +4233,7 @@
       <c r="A76" t="s">
         <v>73</v>
       </c>
-      <c r="C76" s="25"/>
+      <c r="C76" s="20"/>
       <c r="D76" t="s">
         <v>433</v>
       </c>
@@ -4254,7 +4254,7 @@
       <c r="A77" t="s">
         <v>74</v>
       </c>
-      <c r="C77" s="25"/>
+      <c r="C77" s="20"/>
       <c r="E77" t="s">
         <v>357</v>
       </c>
@@ -4266,7 +4266,7 @@
       <c r="A78" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C78" s="26"/>
+      <c r="C78" s="21"/>
       <c r="E78" s="6" t="s">
         <v>364</v>
       </c>
@@ -4278,7 +4278,7 @@
       <c r="A79" t="s">
         <v>76</v>
       </c>
-      <c r="C79" s="24" t="s">
+      <c r="C79" s="19" t="s">
         <v>544</v>
       </c>
       <c r="D79" t="s">
@@ -4301,7 +4301,7 @@
       <c r="A80" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="25"/>
+      <c r="C80" s="20"/>
       <c r="D80" t="s">
         <v>436</v>
       </c>
@@ -4322,7 +4322,7 @@
       <c r="A81" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="25"/>
+      <c r="C81" s="20"/>
       <c r="D81" t="s">
         <v>437</v>
       </c>
@@ -4343,7 +4343,7 @@
       <c r="A82" t="s">
         <v>79</v>
       </c>
-      <c r="C82" s="25"/>
+      <c r="C82" s="20"/>
       <c r="E82" t="s">
         <v>357</v>
       </c>
@@ -4355,7 +4355,7 @@
       <c r="A83" t="s">
         <v>80</v>
       </c>
-      <c r="C83" s="25"/>
+      <c r="C83" s="20"/>
       <c r="E83" t="s">
         <v>357</v>
       </c>
@@ -4367,7 +4367,7 @@
       <c r="A84" t="s">
         <v>81</v>
       </c>
-      <c r="C84" s="25"/>
+      <c r="C84" s="20"/>
       <c r="D84" t="s">
         <v>435</v>
       </c>
@@ -4388,7 +4388,7 @@
       <c r="A85" t="s">
         <v>82</v>
       </c>
-      <c r="C85" s="25"/>
+      <c r="C85" s="20"/>
       <c r="E85" t="s">
         <v>357</v>
       </c>
@@ -4400,7 +4400,7 @@
       <c r="A86" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C86" s="26"/>
+      <c r="C86" s="21"/>
       <c r="E86" s="6" t="s">
         <v>364</v>
       </c>
@@ -4412,7 +4412,7 @@
       <c r="A87" t="s">
         <v>84</v>
       </c>
-      <c r="C87" s="24" t="s">
+      <c r="C87" s="19" t="s">
         <v>545</v>
       </c>
       <c r="E87" t="s">
@@ -4426,7 +4426,7 @@
       <c r="A88" t="s">
         <v>85</v>
       </c>
-      <c r="C88" s="25"/>
+      <c r="C88" s="20"/>
       <c r="E88" t="s">
         <v>357</v>
       </c>
@@ -4438,7 +4438,7 @@
       <c r="A89" t="s">
         <v>86</v>
       </c>
-      <c r="C89" s="25"/>
+      <c r="C89" s="20"/>
       <c r="E89" t="s">
         <v>357</v>
       </c>
@@ -4450,7 +4450,7 @@
       <c r="A90" t="s">
         <v>87</v>
       </c>
-      <c r="C90" s="25"/>
+      <c r="C90" s="20"/>
       <c r="E90" t="s">
         <v>357</v>
       </c>
@@ -4462,7 +4462,7 @@
       <c r="A91" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="26"/>
+      <c r="C91" s="21"/>
       <c r="E91" s="6" t="s">
         <v>364</v>
       </c>
@@ -4474,7 +4474,7 @@
       <c r="A92" t="s">
         <v>89</v>
       </c>
-      <c r="C92" s="24" t="s">
+      <c r="C92" s="19" t="s">
         <v>546</v>
       </c>
       <c r="D92" t="s">
@@ -4497,7 +4497,7 @@
       <c r="A93" t="s">
         <v>90</v>
       </c>
-      <c r="C93" s="25"/>
+      <c r="C93" s="20"/>
       <c r="D93" t="s">
         <v>448</v>
       </c>
@@ -4518,7 +4518,7 @@
       <c r="A94" t="s">
         <v>91</v>
       </c>
-      <c r="C94" s="25"/>
+      <c r="C94" s="20"/>
       <c r="D94" t="s">
         <v>450</v>
       </c>
@@ -4539,7 +4539,7 @@
       <c r="A95" t="s">
         <v>92</v>
       </c>
-      <c r="C95" s="25"/>
+      <c r="C95" s="20"/>
       <c r="D95" t="s">
         <v>453</v>
       </c>
@@ -4560,7 +4560,7 @@
       <c r="A96" t="s">
         <v>93</v>
       </c>
-      <c r="C96" s="25"/>
+      <c r="C96" s="20"/>
       <c r="D96" t="s">
         <v>454</v>
       </c>
@@ -4581,7 +4581,7 @@
       <c r="A97" t="s">
         <v>94</v>
       </c>
-      <c r="C97" s="25"/>
+      <c r="C97" s="20"/>
       <c r="D97" t="s">
         <v>455</v>
       </c>
@@ -4602,7 +4602,7 @@
       <c r="A98" t="s">
         <v>95</v>
       </c>
-      <c r="C98" s="25"/>
+      <c r="C98" s="20"/>
       <c r="D98" t="s">
         <v>456</v>
       </c>
@@ -4623,7 +4623,7 @@
       <c r="A99" t="s">
         <v>96</v>
       </c>
-      <c r="C99" s="25"/>
+      <c r="C99" s="20"/>
       <c r="D99" t="s">
         <v>459</v>
       </c>
@@ -4644,7 +4644,7 @@
       <c r="A100" t="s">
         <v>97</v>
       </c>
-      <c r="C100" s="25"/>
+      <c r="C100" s="20"/>
       <c r="D100" t="s">
         <v>460</v>
       </c>
@@ -4665,7 +4665,7 @@
       <c r="A101" t="s">
         <v>98</v>
       </c>
-      <c r="C101" s="25"/>
+      <c r="C101" s="20"/>
       <c r="D101" t="s">
         <v>461</v>
       </c>
@@ -4686,7 +4686,7 @@
       <c r="A102" t="s">
         <v>99</v>
       </c>
-      <c r="C102" s="25"/>
+      <c r="C102" s="20"/>
       <c r="D102" t="s">
         <v>465</v>
       </c>
@@ -4707,7 +4707,7 @@
       <c r="A103" t="s">
         <v>100</v>
       </c>
-      <c r="C103" s="25"/>
+      <c r="C103" s="20"/>
       <c r="D103" t="s">
         <v>466</v>
       </c>
@@ -4728,7 +4728,7 @@
       <c r="A104" t="s">
         <v>101</v>
       </c>
-      <c r="C104" s="25"/>
+      <c r="C104" s="20"/>
       <c r="D104" t="s">
         <v>467</v>
       </c>
@@ -4749,7 +4749,7 @@
       <c r="A105" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="25"/>
+      <c r="C105" s="20"/>
       <c r="D105" t="s">
         <v>468</v>
       </c>
@@ -4770,7 +4770,7 @@
       <c r="A106" t="s">
         <v>103</v>
       </c>
-      <c r="C106" s="25"/>
+      <c r="C106" s="20"/>
       <c r="E106" t="s">
         <v>357</v>
       </c>
@@ -4782,7 +4782,7 @@
       <c r="A107" t="s">
         <v>104</v>
       </c>
-      <c r="C107" s="25"/>
+      <c r="C107" s="20"/>
       <c r="E107" t="s">
         <v>357</v>
       </c>
@@ -4794,7 +4794,7 @@
       <c r="A108" t="s">
         <v>105</v>
       </c>
-      <c r="C108" s="25"/>
+      <c r="C108" s="20"/>
       <c r="D108" t="s">
         <v>472</v>
       </c>
@@ -4815,7 +4815,7 @@
       <c r="A109" t="s">
         <v>106</v>
       </c>
-      <c r="C109" s="25"/>
+      <c r="C109" s="20"/>
       <c r="E109" t="s">
         <v>357</v>
       </c>
@@ -4827,7 +4827,7 @@
       <c r="A110" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C110" s="26"/>
+      <c r="C110" s="21"/>
       <c r="E110" s="6" t="s">
         <v>364</v>
       </c>
@@ -4853,7 +4853,7 @@
       <c r="A112" t="s">
         <v>109</v>
       </c>
-      <c r="C112" s="24" t="s">
+      <c r="C112" s="19" t="s">
         <v>548</v>
       </c>
       <c r="D112" t="s">
@@ -4873,7 +4873,7 @@
       <c r="A113" t="s">
         <v>110</v>
       </c>
-      <c r="C113" s="25"/>
+      <c r="C113" s="20"/>
       <c r="D113" t="s">
         <v>477</v>
       </c>
@@ -4891,7 +4891,7 @@
       <c r="A114" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="25"/>
+      <c r="C114" s="20"/>
       <c r="D114" t="s">
         <v>478</v>
       </c>
@@ -4909,7 +4909,7 @@
       <c r="A115" t="s">
         <v>112</v>
       </c>
-      <c r="C115" s="25"/>
+      <c r="C115" s="20"/>
       <c r="D115" t="s">
         <v>479</v>
       </c>
@@ -4927,7 +4927,7 @@
       <c r="A116" t="s">
         <v>113</v>
       </c>
-      <c r="C116" s="25"/>
+      <c r="C116" s="20"/>
       <c r="D116" t="s">
         <v>480</v>
       </c>
@@ -4948,7 +4948,7 @@
       <c r="A117" t="s">
         <v>114</v>
       </c>
-      <c r="C117" s="25"/>
+      <c r="C117" s="20"/>
       <c r="D117" t="s">
         <v>481</v>
       </c>
@@ -4969,7 +4969,7 @@
       <c r="A118" t="s">
         <v>115</v>
       </c>
-      <c r="C118" s="25"/>
+      <c r="C118" s="20"/>
       <c r="D118" t="s">
         <v>488</v>
       </c>
@@ -4990,7 +4990,7 @@
       <c r="A119" t="s">
         <v>116</v>
       </c>
-      <c r="C119" s="25"/>
+      <c r="C119" s="20"/>
       <c r="D119" t="s">
         <v>442</v>
       </c>
@@ -5011,7 +5011,7 @@
       <c r="A120" t="s">
         <v>117</v>
       </c>
-      <c r="C120" s="25"/>
+      <c r="C120" s="20"/>
       <c r="D120" t="s">
         <v>483</v>
       </c>
@@ -5032,7 +5032,7 @@
       <c r="A121" t="s">
         <v>118</v>
       </c>
-      <c r="C121" s="25"/>
+      <c r="C121" s="20"/>
       <c r="D121" t="s">
         <v>487</v>
       </c>
@@ -5053,7 +5053,7 @@
       <c r="A122" t="s">
         <v>119</v>
       </c>
-      <c r="C122" s="25"/>
+      <c r="C122" s="20"/>
       <c r="D122" t="s">
         <v>484</v>
       </c>
@@ -5074,7 +5074,7 @@
       <c r="A123" t="s">
         <v>120</v>
       </c>
-      <c r="C123" s="25"/>
+      <c r="C123" s="20"/>
       <c r="D123" t="s">
         <v>485</v>
       </c>
@@ -5095,7 +5095,7 @@
       <c r="A124" t="s">
         <v>121</v>
       </c>
-      <c r="C124" s="25"/>
+      <c r="C124" s="20"/>
       <c r="D124" t="s">
         <v>486</v>
       </c>
@@ -5116,7 +5116,7 @@
       <c r="A125" t="s">
         <v>122</v>
       </c>
-      <c r="C125" s="25"/>
+      <c r="C125" s="20"/>
       <c r="D125" t="s">
         <v>482</v>
       </c>
@@ -5137,7 +5137,7 @@
       <c r="A126" t="s">
         <v>123</v>
       </c>
-      <c r="C126" s="25"/>
+      <c r="C126" s="20"/>
       <c r="E126" t="s">
         <v>357</v>
       </c>
@@ -5149,7 +5149,7 @@
       <c r="A127" t="s">
         <v>124</v>
       </c>
-      <c r="C127" s="25"/>
+      <c r="C127" s="20"/>
       <c r="E127" t="s">
         <v>357</v>
       </c>
@@ -5161,7 +5161,7 @@
       <c r="A128" t="s">
         <v>125</v>
       </c>
-      <c r="C128" s="25"/>
+      <c r="C128" s="20"/>
       <c r="D128" t="s">
         <v>491</v>
       </c>
@@ -5182,7 +5182,7 @@
       <c r="A129" t="s">
         <v>126</v>
       </c>
-      <c r="C129" s="25"/>
+      <c r="C129" s="20"/>
       <c r="E129" t="s">
         <v>357</v>
       </c>
@@ -5194,7 +5194,7 @@
       <c r="A130" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C130" s="26"/>
+      <c r="C130" s="21"/>
       <c r="E130" s="6" t="s">
         <v>364</v>
       </c>
@@ -5206,7 +5206,7 @@
       <c r="A131" t="s">
         <v>128</v>
       </c>
-      <c r="C131" s="24" t="s">
+      <c r="C131" s="19" t="s">
         <v>549</v>
       </c>
       <c r="E131" t="s">
@@ -5220,7 +5220,7 @@
       <c r="A132" t="s">
         <v>129</v>
       </c>
-      <c r="C132" s="25"/>
+      <c r="C132" s="20"/>
       <c r="E132" t="s">
         <v>357</v>
       </c>
@@ -5232,7 +5232,7 @@
       <c r="A133" t="s">
         <v>130</v>
       </c>
-      <c r="C133" s="25"/>
+      <c r="C133" s="20"/>
       <c r="E133" t="s">
         <v>357</v>
       </c>
@@ -5244,7 +5244,7 @@
       <c r="A134" t="s">
         <v>131</v>
       </c>
-      <c r="C134" s="25"/>
+      <c r="C134" s="20"/>
       <c r="E134" t="s">
         <v>357</v>
       </c>
@@ -5256,7 +5256,7 @@
       <c r="A135" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C135" s="28"/>
+      <c r="C135" s="22"/>
       <c r="E135" s="12" t="s">
         <v>364</v>
       </c>
@@ -5268,7 +5268,7 @@
       <c r="A136" t="s">
         <v>133</v>
       </c>
-      <c r="C136" s="25" t="s">
+      <c r="C136" s="20" t="s">
         <v>550</v>
       </c>
       <c r="D136" t="s">
@@ -5291,7 +5291,7 @@
       <c r="A137" t="s">
         <v>134</v>
       </c>
-      <c r="C137" s="25"/>
+      <c r="C137" s="20"/>
       <c r="D137" t="s">
         <v>501</v>
       </c>
@@ -5312,7 +5312,7 @@
       <c r="A138" t="s">
         <v>135</v>
       </c>
-      <c r="C138" s="25"/>
+      <c r="C138" s="20"/>
       <c r="E138" t="s">
         <v>497</v>
       </c>
@@ -5327,7 +5327,7 @@
       <c r="A139" t="s">
         <v>136</v>
       </c>
-      <c r="C139" s="25"/>
+      <c r="C139" s="20"/>
       <c r="D139" t="s">
         <v>502</v>
       </c>
@@ -5348,7 +5348,7 @@
       <c r="A140" t="s">
         <v>637</v>
       </c>
-      <c r="C140" s="25"/>
+      <c r="C140" s="20"/>
       <c r="E140" t="s">
         <v>623</v>
       </c>
@@ -5366,7 +5366,7 @@
       <c r="A141" t="s">
         <v>638</v>
       </c>
-      <c r="C141" s="25"/>
+      <c r="C141" s="20"/>
       <c r="E141" t="s">
         <v>623</v>
       </c>
@@ -5384,7 +5384,7 @@
       <c r="A142" t="s">
         <v>639</v>
       </c>
-      <c r="C142" s="25"/>
+      <c r="C142" s="20"/>
       <c r="E142" t="s">
         <v>629</v>
       </c>
@@ -5402,7 +5402,7 @@
       <c r="A143" t="s">
         <v>640</v>
       </c>
-      <c r="C143" s="25"/>
+      <c r="C143" s="20"/>
       <c r="E143" t="s">
         <v>629</v>
       </c>
@@ -5420,7 +5420,7 @@
       <c r="A144" t="s">
         <v>641</v>
       </c>
-      <c r="C144" s="25"/>
+      <c r="C144" s="20"/>
       <c r="E144" t="s">
         <v>629</v>
       </c>
@@ -5438,7 +5438,7 @@
       <c r="A145" t="s">
         <v>642</v>
       </c>
-      <c r="C145" s="25"/>
+      <c r="C145" s="20"/>
       <c r="D145" t="s">
         <v>656</v>
       </c>
@@ -5462,7 +5462,7 @@
       <c r="A146" t="s">
         <v>137</v>
       </c>
-      <c r="C146" s="25"/>
+      <c r="C146" s="20"/>
       <c r="D146" t="s">
         <v>503</v>
       </c>
@@ -5483,7 +5483,7 @@
       <c r="A147" t="s">
         <v>138</v>
       </c>
-      <c r="C147" s="25"/>
+      <c r="C147" s="20"/>
       <c r="E147" t="s">
         <v>357</v>
       </c>
@@ -5495,7 +5495,7 @@
       <c r="A148" t="s">
         <v>139</v>
       </c>
-      <c r="C148" s="25"/>
+      <c r="C148" s="20"/>
       <c r="E148" t="s">
         <v>357</v>
       </c>
@@ -5507,7 +5507,7 @@
       <c r="A149" t="s">
         <v>140</v>
       </c>
-      <c r="C149" s="25"/>
+      <c r="C149" s="20"/>
       <c r="D149" t="s">
         <v>504</v>
       </c>
@@ -5528,7 +5528,7 @@
       <c r="A150" t="s">
         <v>141</v>
       </c>
-      <c r="C150" s="25"/>
+      <c r="C150" s="20"/>
       <c r="E150" t="s">
         <v>357</v>
       </c>
@@ -5540,7 +5540,7 @@
       <c r="A151" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C151" s="26"/>
+      <c r="C151" s="21"/>
       <c r="E151" s="6" t="s">
         <v>364</v>
       </c>
@@ -5566,7 +5566,7 @@
       <c r="A153" t="s">
         <v>144</v>
       </c>
-      <c r="C153" s="24" t="s">
+      <c r="C153" s="19" t="s">
         <v>551</v>
       </c>
       <c r="E153" t="s">
@@ -5580,7 +5580,7 @@
       <c r="A154" t="s">
         <v>145</v>
       </c>
-      <c r="C154" s="25"/>
+      <c r="C154" s="20"/>
       <c r="E154" t="s">
         <v>357</v>
       </c>
@@ -5592,7 +5592,7 @@
       <c r="A155" t="s">
         <v>146</v>
       </c>
-      <c r="C155" s="25"/>
+      <c r="C155" s="20"/>
       <c r="E155" t="s">
         <v>357</v>
       </c>
@@ -5604,7 +5604,7 @@
       <c r="A156" t="s">
         <v>147</v>
       </c>
-      <c r="C156" s="25"/>
+      <c r="C156" s="20"/>
       <c r="E156" t="s">
         <v>357</v>
       </c>
@@ -5616,7 +5616,7 @@
       <c r="A157" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C157" s="26"/>
+      <c r="C157" s="21"/>
       <c r="E157" s="6" t="s">
         <v>364</v>
       </c>
@@ -5628,7 +5628,7 @@
       <c r="A158" t="s">
         <v>149</v>
       </c>
-      <c r="C158" s="24" t="s">
+      <c r="C158" s="19" t="s">
         <v>552</v>
       </c>
       <c r="E158" t="s">
@@ -5642,7 +5642,7 @@
       <c r="A159" t="s">
         <v>150</v>
       </c>
-      <c r="C159" s="25"/>
+      <c r="C159" s="20"/>
       <c r="E159" t="s">
         <v>357</v>
       </c>
@@ -5654,7 +5654,7 @@
       <c r="A160" t="s">
         <v>151</v>
       </c>
-      <c r="C160" s="25"/>
+      <c r="C160" s="20"/>
       <c r="E160" t="s">
         <v>357</v>
       </c>
@@ -5669,7 +5669,7 @@
       <c r="A161" t="s">
         <v>152</v>
       </c>
-      <c r="C161" s="25"/>
+      <c r="C161" s="20"/>
       <c r="E161" t="s">
         <v>357</v>
       </c>
@@ -5684,7 +5684,7 @@
       <c r="A162" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C162" s="26"/>
+      <c r="C162" s="21"/>
       <c r="E162" s="6" t="s">
         <v>364</v>
       </c>
@@ -5696,7 +5696,7 @@
       <c r="A163" t="s">
         <v>154</v>
       </c>
-      <c r="C163" s="24" t="s">
+      <c r="C163" s="19" t="s">
         <v>553</v>
       </c>
       <c r="D163" t="s">
@@ -5719,7 +5719,7 @@
       <c r="A164" t="s">
         <v>155</v>
       </c>
-      <c r="C164" s="25"/>
+      <c r="C164" s="20"/>
       <c r="E164" t="s">
         <v>357</v>
       </c>
@@ -5731,26 +5731,26 @@
       <c r="A165" t="s">
         <v>156</v>
       </c>
-      <c r="C165" s="25"/>
+      <c r="C165" s="20"/>
       <c r="E165" t="s">
         <v>357</v>
       </c>
       <c r="F165" t="s">
         <v>522</v>
       </c>
-      <c r="I165" s="27" t="s">
+      <c r="I165" s="18" t="s">
         <v>601</v>
       </c>
-      <c r="J165" s="27"/>
-      <c r="K165" s="27"/>
-      <c r="L165" s="27"/>
-      <c r="M165" s="27"/>
+      <c r="J165" s="18"/>
+      <c r="K165" s="18"/>
+      <c r="L165" s="18"/>
+      <c r="M165" s="18"/>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
         <v>157</v>
       </c>
-      <c r="C166" s="25"/>
+      <c r="C166" s="20"/>
       <c r="D166" t="s">
         <v>511</v>
       </c>
@@ -5766,51 +5766,51 @@
       <c r="H166" t="s">
         <v>634</v>
       </c>
-      <c r="I166" s="27"/>
-      <c r="J166" s="27"/>
-      <c r="K166" s="27"/>
-      <c r="L166" s="27"/>
-      <c r="M166" s="27"/>
+      <c r="I166" s="18"/>
+      <c r="J166" s="18"/>
+      <c r="K166" s="18"/>
+      <c r="L166" s="18"/>
+      <c r="M166" s="18"/>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="s">
         <v>158</v>
       </c>
-      <c r="C167" s="25"/>
+      <c r="C167" s="20"/>
       <c r="E167" t="s">
         <v>357</v>
       </c>
       <c r="F167" t="s">
         <v>492</v>
       </c>
-      <c r="I167" s="27"/>
-      <c r="J167" s="27"/>
-      <c r="K167" s="27"/>
-      <c r="L167" s="27"/>
-      <c r="M167" s="27"/>
+      <c r="I167" s="18"/>
+      <c r="J167" s="18"/>
+      <c r="K167" s="18"/>
+      <c r="L167" s="18"/>
+      <c r="M167" s="18"/>
     </row>
     <row r="168" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C168" s="26"/>
+      <c r="C168" s="21"/>
       <c r="E168" s="6" t="s">
         <v>364</v>
       </c>
       <c r="F168" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="I168" s="27"/>
-      <c r="J168" s="27"/>
-      <c r="K168" s="27"/>
-      <c r="L168" s="27"/>
-      <c r="M168" s="27"/>
+      <c r="I168" s="18"/>
+      <c r="J168" s="18"/>
+      <c r="K168" s="18"/>
+      <c r="L168" s="18"/>
+      <c r="M168" s="18"/>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
         <v>160</v>
       </c>
-      <c r="C169" s="24" t="s">
+      <c r="C169" s="19" t="s">
         <v>555</v>
       </c>
       <c r="E169" t="s">
@@ -5827,7 +5827,7 @@
       <c r="A170" t="s">
         <v>161</v>
       </c>
-      <c r="C170" s="25"/>
+      <c r="C170" s="20"/>
       <c r="D170" t="s">
         <v>520</v>
       </c>
@@ -5848,7 +5848,7 @@
       <c r="A171" t="s">
         <v>620</v>
       </c>
-      <c r="C171" s="25"/>
+      <c r="C171" s="20"/>
       <c r="E171" t="s">
         <v>623</v>
       </c>
@@ -5866,7 +5866,7 @@
       <c r="A172" t="s">
         <v>621</v>
       </c>
-      <c r="C172" s="25"/>
+      <c r="C172" s="20"/>
       <c r="E172" t="s">
         <v>623</v>
       </c>
@@ -5884,7 +5884,7 @@
       <c r="A173" t="s">
         <v>625</v>
       </c>
-      <c r="C173" s="25"/>
+      <c r="C173" s="20"/>
       <c r="E173" t="s">
         <v>629</v>
       </c>
@@ -5902,7 +5902,7 @@
       <c r="A174" t="s">
         <v>626</v>
       </c>
-      <c r="C174" s="25"/>
+      <c r="C174" s="20"/>
       <c r="E174" t="s">
         <v>629</v>
       </c>
@@ -5920,7 +5920,7 @@
       <c r="A175" t="s">
         <v>627</v>
       </c>
-      <c r="C175" s="25"/>
+      <c r="C175" s="20"/>
       <c r="E175" t="s">
         <v>629</v>
       </c>
@@ -5938,7 +5938,7 @@
       <c r="A176" t="s">
         <v>628</v>
       </c>
-      <c r="C176" s="25"/>
+      <c r="C176" s="20"/>
       <c r="D176" t="s">
         <v>657</v>
       </c>
@@ -5962,7 +5962,7 @@
       <c r="A177" t="s">
         <v>162</v>
       </c>
-      <c r="C177" s="25"/>
+      <c r="C177" s="20"/>
       <c r="D177" t="s">
         <v>521</v>
       </c>
@@ -5983,7 +5983,7 @@
       <c r="A178" t="s">
         <v>163</v>
       </c>
-      <c r="C178" s="25"/>
+      <c r="C178" s="20"/>
       <c r="E178" t="s">
         <v>357</v>
       </c>
@@ -5995,7 +5995,7 @@
       <c r="A179" t="s">
         <v>164</v>
       </c>
-      <c r="C179" s="25"/>
+      <c r="C179" s="20"/>
       <c r="E179" t="s">
         <v>357</v>
       </c>
@@ -6007,7 +6007,7 @@
       <c r="A180" t="s">
         <v>165</v>
       </c>
-      <c r="C180" s="25"/>
+      <c r="C180" s="20"/>
       <c r="E180" t="s">
         <v>357</v>
       </c>
@@ -6019,7 +6019,7 @@
       <c r="A181" t="s">
         <v>166</v>
       </c>
-      <c r="C181" s="25"/>
+      <c r="C181" s="20"/>
       <c r="E181" t="s">
         <v>357</v>
       </c>
@@ -6031,7 +6031,7 @@
       <c r="A182" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C182" s="26"/>
+      <c r="C182" s="21"/>
       <c r="E182" s="6" t="s">
         <v>364</v>
       </c>
@@ -6043,7 +6043,7 @@
       <c r="A183" t="s">
         <v>168</v>
       </c>
-      <c r="C183" s="24" t="s">
+      <c r="C183" s="19" t="s">
         <v>556</v>
       </c>
       <c r="E183" t="s">
@@ -6057,7 +6057,7 @@
       <c r="A184" t="s">
         <v>169</v>
       </c>
-      <c r="C184" s="25"/>
+      <c r="C184" s="20"/>
       <c r="E184" t="s">
         <v>357</v>
       </c>
@@ -6069,7 +6069,7 @@
       <c r="A185" t="s">
         <v>170</v>
       </c>
-      <c r="C185" s="25"/>
+      <c r="C185" s="20"/>
       <c r="D185" t="s">
         <v>524</v>
       </c>
@@ -6090,7 +6090,7 @@
       <c r="A186" t="s">
         <v>171</v>
       </c>
-      <c r="C186" s="25"/>
+      <c r="C186" s="20"/>
       <c r="E186" t="s">
         <v>357</v>
       </c>
@@ -6102,7 +6102,7 @@
       <c r="A187" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C187" s="26"/>
+      <c r="C187" s="21"/>
       <c r="E187" s="6" t="s">
         <v>364</v>
       </c>
@@ -6114,7 +6114,7 @@
       <c r="A188" t="s">
         <v>173</v>
       </c>
-      <c r="C188" s="24" t="s">
+      <c r="C188" s="19" t="s">
         <v>557</v>
       </c>
       <c r="E188" t="s">
@@ -6128,7 +6128,7 @@
       <c r="A189" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C189" s="26"/>
+      <c r="C189" s="21"/>
       <c r="D189" s="6" t="s">
         <v>530</v>
       </c>
@@ -6149,7 +6149,7 @@
       <c r="A190" t="s">
         <v>175</v>
       </c>
-      <c r="C190" s="24" t="s">
+      <c r="C190" s="19" t="s">
         <v>558</v>
       </c>
       <c r="E190" t="s">
@@ -6163,7 +6163,7 @@
       <c r="A191" t="s">
         <v>176</v>
       </c>
-      <c r="C191" s="25"/>
+      <c r="C191" s="20"/>
       <c r="E191" t="s">
         <v>357</v>
       </c>
@@ -6175,7 +6175,7 @@
       <c r="A192" t="s">
         <v>177</v>
       </c>
-      <c r="C192" s="25"/>
+      <c r="C192" s="20"/>
       <c r="E192" t="s">
         <v>357</v>
       </c>
@@ -6187,7 +6187,7 @@
       <c r="A193" t="s">
         <v>178</v>
       </c>
-      <c r="C193" s="25"/>
+      <c r="C193" s="20"/>
       <c r="E193" t="s">
         <v>357</v>
       </c>
@@ -6199,7 +6199,7 @@
       <c r="A194" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C194" s="26"/>
+      <c r="C194" s="21"/>
       <c r="E194" s="6" t="s">
         <v>364</v>
       </c>
@@ -6211,7 +6211,7 @@
       <c r="A195" t="s">
         <v>180</v>
       </c>
-      <c r="C195" s="24" t="s">
+      <c r="C195" s="19" t="s">
         <v>559</v>
       </c>
       <c r="E195" t="s">
@@ -6225,7 +6225,7 @@
       <c r="A196" t="s">
         <v>181</v>
       </c>
-      <c r="C196" s="25"/>
+      <c r="C196" s="20"/>
       <c r="E196" t="s">
         <v>357</v>
       </c>
@@ -6237,7 +6237,7 @@
       <c r="A197" t="s">
         <v>182</v>
       </c>
-      <c r="C197" s="25"/>
+      <c r="C197" s="20"/>
       <c r="D197" t="s">
         <v>596</v>
       </c>
@@ -6258,7 +6258,7 @@
       <c r="A198" t="s">
         <v>183</v>
       </c>
-      <c r="C198" s="25"/>
+      <c r="C198" s="20"/>
       <c r="E198" t="s">
         <v>357</v>
       </c>
@@ -6270,7 +6270,7 @@
       <c r="A199" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C199" s="26"/>
+      <c r="C199" s="21"/>
       <c r="E199" s="6" t="s">
         <v>364</v>
       </c>
@@ -6282,7 +6282,7 @@
       <c r="A200" t="s">
         <v>185</v>
       </c>
-      <c r="C200" s="24" t="s">
+      <c r="C200" s="19" t="s">
         <v>560</v>
       </c>
       <c r="E200" t="s">
@@ -6296,7 +6296,7 @@
       <c r="A201" t="s">
         <v>186</v>
       </c>
-      <c r="C201" s="25"/>
+      <c r="C201" s="20"/>
       <c r="E201" t="s">
         <v>357</v>
       </c>
@@ -6308,7 +6308,7 @@
       <c r="A202" t="s">
         <v>187</v>
       </c>
-      <c r="C202" s="25"/>
+      <c r="C202" s="20"/>
       <c r="D202" t="s">
         <v>595</v>
       </c>
@@ -6329,7 +6329,7 @@
       <c r="A203" t="s">
         <v>188</v>
       </c>
-      <c r="C203" s="25"/>
+      <c r="C203" s="20"/>
       <c r="E203" t="s">
         <v>357</v>
       </c>
@@ -6341,7 +6341,7 @@
       <c r="A204" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C204" s="26"/>
+      <c r="C204" s="21"/>
       <c r="E204" s="6" t="s">
         <v>364</v>
       </c>
@@ -6353,7 +6353,7 @@
       <c r="A205" t="s">
         <v>190</v>
       </c>
-      <c r="C205" s="24" t="s">
+      <c r="C205" s="19" t="s">
         <v>563</v>
       </c>
       <c r="E205" t="s">
@@ -6367,7 +6367,7 @@
       <c r="A206" t="s">
         <v>191</v>
       </c>
-      <c r="C206" s="25"/>
+      <c r="C206" s="20"/>
       <c r="E206" t="s">
         <v>357</v>
       </c>
@@ -6379,7 +6379,7 @@
       <c r="A207" t="s">
         <v>192</v>
       </c>
-      <c r="C207" s="25"/>
+      <c r="C207" s="20"/>
       <c r="D207" t="s">
         <v>600</v>
       </c>
@@ -6400,7 +6400,7 @@
       <c r="A208" t="s">
         <v>193</v>
       </c>
-      <c r="C208" s="25"/>
+      <c r="C208" s="20"/>
       <c r="E208" t="s">
         <v>357</v>
       </c>
@@ -6412,7 +6412,7 @@
       <c r="A209" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C209" s="26"/>
+      <c r="C209" s="21"/>
       <c r="E209" s="6" t="s">
         <v>364</v>
       </c>
@@ -6424,7 +6424,7 @@
       <c r="A210" t="s">
         <v>195</v>
       </c>
-      <c r="C210" s="24" t="s">
+      <c r="C210" s="19" t="s">
         <v>561</v>
       </c>
       <c r="D210" t="s">
@@ -6450,7 +6450,7 @@
       <c r="A211" t="s">
         <v>196</v>
       </c>
-      <c r="C211" s="25"/>
+      <c r="C211" s="20"/>
       <c r="D211" t="s">
         <v>609</v>
       </c>
@@ -6471,7 +6471,7 @@
       <c r="A212" t="s">
         <v>197</v>
       </c>
-      <c r="C212" s="25"/>
+      <c r="C212" s="20"/>
       <c r="D212" t="s">
         <v>610</v>
       </c>
@@ -6489,7 +6489,7 @@
       <c r="A213" t="s">
         <v>198</v>
       </c>
-      <c r="C213" s="25"/>
+      <c r="C213" s="20"/>
       <c r="D213" t="s">
         <v>611</v>
       </c>
@@ -6510,7 +6510,7 @@
       <c r="A214" t="s">
         <v>643</v>
       </c>
-      <c r="C214" s="25"/>
+      <c r="C214" s="20"/>
       <c r="E214" t="s">
         <v>623</v>
       </c>
@@ -6525,7 +6525,7 @@
       <c r="A215" t="s">
         <v>644</v>
       </c>
-      <c r="C215" s="25"/>
+      <c r="C215" s="20"/>
       <c r="E215" t="s">
         <v>623</v>
       </c>
@@ -6540,7 +6540,7 @@
       <c r="A216" t="s">
         <v>645</v>
       </c>
-      <c r="C216" s="25"/>
+      <c r="C216" s="20"/>
       <c r="E216" t="s">
         <v>629</v>
       </c>
@@ -6555,7 +6555,7 @@
       <c r="A217" t="s">
         <v>646</v>
       </c>
-      <c r="C217" s="25"/>
+      <c r="C217" s="20"/>
       <c r="E217" t="s">
         <v>629</v>
       </c>
@@ -6570,7 +6570,7 @@
       <c r="A218" t="s">
         <v>647</v>
       </c>
-      <c r="C218" s="25"/>
+      <c r="C218" s="20"/>
       <c r="E218" t="s">
         <v>629</v>
       </c>
@@ -6585,7 +6585,7 @@
       <c r="A219" t="s">
         <v>648</v>
       </c>
-      <c r="C219" s="25"/>
+      <c r="C219" s="20"/>
       <c r="D219" t="s">
         <v>658</v>
       </c>
@@ -6606,7 +6606,7 @@
       <c r="A220" t="s">
         <v>199</v>
       </c>
-      <c r="C220" s="25"/>
+      <c r="C220" s="20"/>
       <c r="E220" t="s">
         <v>612</v>
       </c>
@@ -6618,7 +6618,7 @@
       <c r="A221" t="s">
         <v>200</v>
       </c>
-      <c r="C221" s="25"/>
+      <c r="C221" s="20"/>
       <c r="D221" t="s">
         <v>614</v>
       </c>
@@ -6636,7 +6636,7 @@
       <c r="A222" t="s">
         <v>201</v>
       </c>
-      <c r="C222" s="25"/>
+      <c r="C222" s="20"/>
       <c r="E222" t="s">
         <v>357</v>
       </c>
@@ -6648,7 +6648,7 @@
       <c r="A223" t="s">
         <v>202</v>
       </c>
-      <c r="C223" s="25"/>
+      <c r="C223" s="20"/>
       <c r="D223" t="s">
         <v>665</v>
       </c>
@@ -6672,7 +6672,7 @@
       <c r="A224" t="s">
         <v>203</v>
       </c>
-      <c r="C224" s="25"/>
+      <c r="C224" s="20"/>
       <c r="E224" t="s">
         <v>357</v>
       </c>
@@ -6684,7 +6684,7 @@
       <c r="A225" t="s">
         <v>204</v>
       </c>
-      <c r="C225" s="25"/>
+      <c r="C225" s="20"/>
       <c r="E225" t="s">
         <v>357</v>
       </c>
@@ -6696,7 +6696,7 @@
       <c r="A226" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C226" s="26"/>
+      <c r="C226" s="21"/>
       <c r="E226" s="6" t="s">
         <v>364</v>
       </c>
@@ -6708,7 +6708,7 @@
       <c r="A227" t="s">
         <v>206</v>
       </c>
-      <c r="C227" s="24" t="s">
+      <c r="C227" s="19" t="s">
         <v>562</v>
       </c>
       <c r="E227" t="s">
@@ -6722,7 +6722,7 @@
       <c r="A228" t="s">
         <v>207</v>
       </c>
-      <c r="C228" s="25"/>
+      <c r="C228" s="20"/>
       <c r="D228" t="s">
         <v>617</v>
       </c>
@@ -6740,7 +6740,7 @@
       <c r="A229" t="s">
         <v>650</v>
       </c>
-      <c r="C229" s="25"/>
+      <c r="C229" s="20"/>
       <c r="E229" t="s">
         <v>623</v>
       </c>
@@ -6755,7 +6755,7 @@
       <c r="A230" t="s">
         <v>651</v>
       </c>
-      <c r="C230" s="25"/>
+      <c r="C230" s="20"/>
       <c r="E230" t="s">
         <v>623</v>
       </c>
@@ -6770,7 +6770,7 @@
       <c r="A231" t="s">
         <v>652</v>
       </c>
-      <c r="C231" s="25"/>
+      <c r="C231" s="20"/>
       <c r="E231" t="s">
         <v>629</v>
       </c>
@@ -6785,7 +6785,7 @@
       <c r="A232" t="s">
         <v>653</v>
       </c>
-      <c r="C232" s="25"/>
+      <c r="C232" s="20"/>
       <c r="E232" t="s">
         <v>629</v>
       </c>
@@ -6800,7 +6800,7 @@
       <c r="A233" t="s">
         <v>654</v>
       </c>
-      <c r="C233" s="25"/>
+      <c r="C233" s="20"/>
       <c r="E233" t="s">
         <v>629</v>
       </c>
@@ -6815,7 +6815,7 @@
       <c r="A234" t="s">
         <v>655</v>
       </c>
-      <c r="C234" s="25"/>
+      <c r="C234" s="20"/>
       <c r="D234" t="s">
         <v>659</v>
       </c>
@@ -6836,7 +6836,7 @@
       <c r="A235" t="s">
         <v>208</v>
       </c>
-      <c r="C235" s="25"/>
+      <c r="C235" s="20"/>
       <c r="D235" t="s">
         <v>616</v>
       </c>
@@ -6854,7 +6854,7 @@
       <c r="A236" t="s">
         <v>209</v>
       </c>
-      <c r="C236" s="25"/>
+      <c r="C236" s="20"/>
       <c r="E236" t="s">
         <v>357</v>
       </c>
@@ -6866,7 +6866,7 @@
       <c r="A237" t="s">
         <v>210</v>
       </c>
-      <c r="C237" s="25"/>
+      <c r="C237" s="20"/>
       <c r="E237" t="s">
         <v>357</v>
       </c>
@@ -6878,7 +6878,7 @@
       <c r="A238" t="s">
         <v>211</v>
       </c>
-      <c r="C238" s="25"/>
+      <c r="C238" s="20"/>
       <c r="D238" t="s">
         <v>664</v>
       </c>
@@ -6899,7 +6899,7 @@
       <c r="A239" t="s">
         <v>212</v>
       </c>
-      <c r="C239" s="25"/>
+      <c r="C239" s="20"/>
       <c r="E239" t="s">
         <v>357</v>
       </c>
@@ -6911,7 +6911,7 @@
       <c r="A240" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="C240" s="26"/>
+      <c r="C240" s="21"/>
       <c r="E240" s="6" t="s">
         <v>364</v>
       </c>
@@ -6923,7 +6923,7 @@
       <c r="A241" t="s">
         <v>214</v>
       </c>
-      <c r="C241" s="24" t="s">
+      <c r="C241" s="19" t="s">
         <v>564</v>
       </c>
       <c r="E241" t="s">
@@ -6937,7 +6937,7 @@
       <c r="A242" t="s">
         <v>215</v>
       </c>
-      <c r="C242" s="25"/>
+      <c r="C242" s="20"/>
       <c r="E242" t="s">
         <v>357</v>
       </c>
@@ -6949,7 +6949,7 @@
       <c r="A243" t="s">
         <v>216</v>
       </c>
-      <c r="C243" s="25"/>
+      <c r="C243" s="20"/>
       <c r="D243" t="s">
         <v>669</v>
       </c>
@@ -6970,7 +6970,7 @@
       <c r="A244" t="s">
         <v>217</v>
       </c>
-      <c r="C244" s="25"/>
+      <c r="C244" s="20"/>
       <c r="E244" t="s">
         <v>357</v>
       </c>
@@ -6982,7 +6982,7 @@
       <c r="A245" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C245" s="26"/>
+      <c r="C245" s="21"/>
       <c r="E245" s="6" t="s">
         <v>364</v>
       </c>
@@ -6994,7 +6994,7 @@
       <c r="A246" t="s">
         <v>219</v>
       </c>
-      <c r="C246" s="24" t="s">
+      <c r="C246" s="19" t="s">
         <v>565</v>
       </c>
       <c r="E246" t="s">
@@ -7008,7 +7008,7 @@
       <c r="A247" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C247" s="26"/>
+      <c r="C247" s="21"/>
       <c r="E247" s="6" t="s">
         <v>379</v>
       </c>
@@ -7023,7 +7023,7 @@
       <c r="A248" t="s">
         <v>221</v>
       </c>
-      <c r="C248" s="24" t="s">
+      <c r="C248" s="19" t="s">
         <v>566</v>
       </c>
       <c r="E248" t="s">
@@ -7037,7 +7037,7 @@
       <c r="A249" t="s">
         <v>222</v>
       </c>
-      <c r="C249" s="25"/>
+      <c r="C249" s="20"/>
       <c r="E249" t="s">
         <v>357</v>
       </c>
@@ -7049,7 +7049,7 @@
       <c r="A250" t="s">
         <v>223</v>
       </c>
-      <c r="C250" s="25"/>
+      <c r="C250" s="20"/>
       <c r="E250" t="s">
         <v>357</v>
       </c>
@@ -7061,7 +7061,7 @@
       <c r="A251" t="s">
         <v>224</v>
       </c>
-      <c r="C251" s="25"/>
+      <c r="C251" s="20"/>
       <c r="E251" t="s">
         <v>357</v>
       </c>
@@ -7073,7 +7073,7 @@
       <c r="A252" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="C252" s="28"/>
+      <c r="C252" s="22"/>
       <c r="E252" s="12" t="s">
         <v>364</v>
       </c>
@@ -7085,7 +7085,7 @@
       <c r="A253" t="s">
         <v>226</v>
       </c>
-      <c r="C253" s="25" t="s">
+      <c r="C253" s="20" t="s">
         <v>567</v>
       </c>
       <c r="D253" t="s">
@@ -7105,7 +7105,7 @@
       <c r="A254" t="s">
         <v>227</v>
       </c>
-      <c r="C254" s="25"/>
+      <c r="C254" s="20"/>
       <c r="D254" t="s">
         <v>683</v>
       </c>
@@ -7123,7 +7123,7 @@
       <c r="A255" t="s">
         <v>228</v>
       </c>
-      <c r="C255" s="25"/>
+      <c r="C255" s="20"/>
       <c r="E255" t="s">
         <v>357</v>
       </c>
@@ -7135,7 +7135,7 @@
       <c r="A256" t="s">
         <v>229</v>
       </c>
-      <c r="C256" s="25"/>
+      <c r="C256" s="20"/>
       <c r="D256" t="s">
         <v>682</v>
       </c>
@@ -7156,7 +7156,7 @@
       <c r="A257" t="s">
         <v>230</v>
       </c>
-      <c r="C257" s="25"/>
+      <c r="C257" s="20"/>
       <c r="E257" t="s">
         <v>357</v>
       </c>
@@ -7168,7 +7168,7 @@
       <c r="A258" t="s">
         <v>231</v>
       </c>
-      <c r="C258" s="25"/>
+      <c r="C258" s="20"/>
       <c r="E258" t="s">
         <v>357</v>
       </c>
@@ -7180,7 +7180,7 @@
       <c r="A259" t="s">
         <v>232</v>
       </c>
-      <c r="C259" s="25"/>
+      <c r="C259" s="20"/>
       <c r="E259" t="s">
         <v>364</v>
       </c>
@@ -7192,7 +7192,7 @@
       <c r="A260" t="s">
         <v>233</v>
       </c>
-      <c r="C260" s="25"/>
+      <c r="C260" s="20"/>
       <c r="D260" t="s">
         <v>684</v>
       </c>
@@ -7213,7 +7213,7 @@
       <c r="A261" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C261" s="25"/>
+      <c r="C261" s="20"/>
       <c r="D261" s="6" t="s">
         <v>687</v>
       </c>
@@ -7231,7 +7231,7 @@
       <c r="A262" t="s">
         <v>235</v>
       </c>
-      <c r="C262" s="25" t="s">
+      <c r="C262" s="20" t="s">
         <v>569</v>
       </c>
       <c r="D262" t="s">
@@ -7249,17 +7249,17 @@
       <c r="H262" t="s">
         <v>636</v>
       </c>
-      <c r="I262" s="19" t="s">
+      <c r="I262" s="23" t="s">
         <v>704</v>
       </c>
-      <c r="J262" s="19"/>
-      <c r="K262" s="19"/>
+      <c r="J262" s="23"/>
+      <c r="K262" s="23"/>
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" t="s">
         <v>236</v>
       </c>
-      <c r="C263" s="25"/>
+      <c r="C263" s="20"/>
       <c r="D263" t="s">
         <v>694</v>
       </c>
@@ -7272,15 +7272,15 @@
       <c r="H263" t="s">
         <v>636</v>
       </c>
-      <c r="I263" s="19"/>
-      <c r="J263" s="19"/>
-      <c r="K263" s="19"/>
+      <c r="I263" s="23"/>
+      <c r="J263" s="23"/>
+      <c r="K263" s="23"/>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" t="s">
         <v>237</v>
       </c>
-      <c r="C264" s="25"/>
+      <c r="C264" s="20"/>
       <c r="D264" t="s">
         <v>698</v>
       </c>
@@ -7293,15 +7293,15 @@
       <c r="H264" t="s">
         <v>636</v>
       </c>
-      <c r="I264" s="19"/>
-      <c r="J264" s="19"/>
-      <c r="K264" s="19"/>
+      <c r="I264" s="23"/>
+      <c r="J264" s="23"/>
+      <c r="K264" s="23"/>
     </row>
     <row r="265" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" t="s">
         <v>238</v>
       </c>
-      <c r="C265" s="25"/>
+      <c r="C265" s="20"/>
       <c r="D265" t="s">
         <v>697</v>
       </c>
@@ -7311,15 +7311,15 @@
       <c r="F265" t="s">
         <v>674</v>
       </c>
-      <c r="I265" s="19"/>
-      <c r="J265" s="19"/>
-      <c r="K265" s="19"/>
+      <c r="I265" s="23"/>
+      <c r="J265" s="23"/>
+      <c r="K265" s="23"/>
     </row>
     <row r="266" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" t="s">
         <v>239</v>
       </c>
-      <c r="C266" s="25"/>
+      <c r="C266" s="20"/>
       <c r="E266" t="s">
         <v>357</v>
       </c>
@@ -7337,7 +7337,7 @@
       <c r="A267" t="s">
         <v>240</v>
       </c>
-      <c r="C267" s="25"/>
+      <c r="C267" s="20"/>
       <c r="E267" t="s">
         <v>357</v>
       </c>
@@ -7349,7 +7349,7 @@
       <c r="A268" t="s">
         <v>241</v>
       </c>
-      <c r="C268" s="25"/>
+      <c r="C268" s="20"/>
       <c r="E268" t="s">
         <v>357</v>
       </c>
@@ -7361,7 +7361,7 @@
       <c r="A269" t="s">
         <v>242</v>
       </c>
-      <c r="C269" s="25"/>
+      <c r="C269" s="20"/>
       <c r="E269" t="s">
         <v>364</v>
       </c>
@@ -7373,7 +7373,7 @@
       <c r="A270" t="s">
         <v>243</v>
       </c>
-      <c r="C270" s="25"/>
+      <c r="C270" s="20"/>
       <c r="D270" t="s">
         <v>699</v>
       </c>
@@ -7391,7 +7391,7 @@
       <c r="A271" t="s">
         <v>244</v>
       </c>
-      <c r="C271" s="25"/>
+      <c r="C271" s="20"/>
       <c r="D271" t="s">
         <v>701</v>
       </c>
@@ -7409,7 +7409,7 @@
       <c r="A272" t="s">
         <v>245</v>
       </c>
-      <c r="C272" s="25"/>
+      <c r="C272" s="20"/>
       <c r="D272" t="s">
         <v>695</v>
       </c>
@@ -7427,7 +7427,7 @@
       <c r="A273" t="s">
         <v>246</v>
       </c>
-      <c r="C273" s="25"/>
+      <c r="C273" s="20"/>
       <c r="D273" t="s">
         <v>708</v>
       </c>
@@ -7448,7 +7448,7 @@
       <c r="A274" t="s">
         <v>247</v>
       </c>
-      <c r="C274" s="25"/>
+      <c r="C274" s="20"/>
       <c r="E274" t="s">
         <v>357</v>
       </c>
@@ -7460,7 +7460,7 @@
       <c r="A275" t="s">
         <v>248</v>
       </c>
-      <c r="C275" s="25"/>
+      <c r="C275" s="20"/>
       <c r="D275" t="s">
         <v>696</v>
       </c>
@@ -7481,7 +7481,7 @@
       <c r="A276" t="s">
         <v>249</v>
       </c>
-      <c r="C276" s="25"/>
+      <c r="C276" s="20"/>
       <c r="E276" t="s">
         <v>357</v>
       </c>
@@ -7493,7 +7493,7 @@
       <c r="A277" t="s">
         <v>250</v>
       </c>
-      <c r="C277" s="25"/>
+      <c r="C277" s="20"/>
       <c r="E277" t="s">
         <v>357</v>
       </c>
@@ -7505,7 +7505,7 @@
       <c r="A278" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="C278" s="26"/>
+      <c r="C278" s="21"/>
       <c r="E278" s="6" t="s">
         <v>364</v>
       </c>
@@ -7537,7 +7537,7 @@
       <c r="A280" t="s">
         <v>253</v>
       </c>
-      <c r="C280" s="24" t="s">
+      <c r="C280" s="19" t="s">
         <v>571</v>
       </c>
       <c r="D280" t="s">
@@ -7557,7 +7557,7 @@
       <c r="A281" t="s">
         <v>254</v>
       </c>
-      <c r="C281" s="25"/>
+      <c r="C281" s="20"/>
       <c r="D281" t="s">
         <v>715</v>
       </c>
@@ -7575,7 +7575,7 @@
       <c r="A282" t="s">
         <v>255</v>
       </c>
-      <c r="C282" s="25"/>
+      <c r="C282" s="20"/>
       <c r="E282" t="s">
         <v>357</v>
       </c>
@@ -7587,7 +7587,7 @@
       <c r="A283" t="s">
         <v>256</v>
       </c>
-      <c r="C283" s="25"/>
+      <c r="C283" s="20"/>
       <c r="D283" t="s">
         <v>716</v>
       </c>
@@ -7608,7 +7608,7 @@
       <c r="A284" t="s">
         <v>257</v>
       </c>
-      <c r="C284" s="25"/>
+      <c r="C284" s="20"/>
       <c r="E284" t="s">
         <v>357</v>
       </c>
@@ -7620,7 +7620,7 @@
       <c r="A285" t="s">
         <v>258</v>
       </c>
-      <c r="C285" s="25"/>
+      <c r="C285" s="20"/>
       <c r="E285" t="s">
         <v>357</v>
       </c>
@@ -7632,7 +7632,7 @@
       <c r="A286" t="s">
         <v>259</v>
       </c>
-      <c r="C286" s="25"/>
+      <c r="C286" s="20"/>
       <c r="E286" t="s">
         <v>364</v>
       </c>
@@ -7644,7 +7644,7 @@
       <c r="A287" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C287" s="26"/>
+      <c r="C287" s="21"/>
       <c r="D287" s="6" t="s">
         <v>717</v>
       </c>
@@ -7662,7 +7662,7 @@
       <c r="A288" t="s">
         <v>261</v>
       </c>
-      <c r="C288" s="24" t="s">
+      <c r="C288" s="19" t="s">
         <v>572</v>
       </c>
       <c r="D288" t="s">
@@ -7685,7 +7685,7 @@
       <c r="A289" t="s">
         <v>262</v>
       </c>
-      <c r="C289" s="25"/>
+      <c r="C289" s="20"/>
       <c r="D289" t="s">
         <v>721</v>
       </c>
@@ -7703,7 +7703,7 @@
       <c r="A290" t="s">
         <v>263</v>
       </c>
-      <c r="C290" s="25"/>
+      <c r="C290" s="20"/>
       <c r="D290" t="s">
         <v>722</v>
       </c>
@@ -7721,7 +7721,7 @@
       <c r="A291" t="s">
         <v>264</v>
       </c>
-      <c r="C291" s="25"/>
+      <c r="C291" s="20"/>
       <c r="D291" t="s">
         <v>723</v>
       </c>
@@ -7736,7 +7736,7 @@
       <c r="A292" t="s">
         <v>265</v>
       </c>
-      <c r="C292" s="25"/>
+      <c r="C292" s="20"/>
       <c r="E292" t="s">
         <v>357</v>
       </c>
@@ -7754,7 +7754,7 @@
       <c r="A293" t="s">
         <v>266</v>
       </c>
-      <c r="C293" s="25"/>
+      <c r="C293" s="20"/>
       <c r="E293" t="s">
         <v>357</v>
       </c>
@@ -7766,7 +7766,7 @@
       <c r="A294" t="s">
         <v>267</v>
       </c>
-      <c r="C294" s="25"/>
+      <c r="C294" s="20"/>
       <c r="E294" t="s">
         <v>357</v>
       </c>
@@ -7778,7 +7778,7 @@
       <c r="A295" t="s">
         <v>268</v>
       </c>
-      <c r="C295" s="25"/>
+      <c r="C295" s="20"/>
       <c r="E295" t="s">
         <v>364</v>
       </c>
@@ -7790,7 +7790,7 @@
       <c r="A296" t="s">
         <v>269</v>
       </c>
-      <c r="C296" s="25"/>
+      <c r="C296" s="20"/>
       <c r="D296" t="s">
         <v>724</v>
       </c>
@@ -7808,7 +7808,7 @@
       <c r="A297" t="s">
         <v>270</v>
       </c>
-      <c r="C297" s="25"/>
+      <c r="C297" s="20"/>
       <c r="D297" t="s">
         <v>727</v>
       </c>
@@ -7826,7 +7826,7 @@
       <c r="A298" t="s">
         <v>271</v>
       </c>
-      <c r="C298" s="25"/>
+      <c r="C298" s="20"/>
       <c r="D298" t="s">
         <v>728</v>
       </c>
@@ -7844,7 +7844,7 @@
       <c r="A299" t="s">
         <v>272</v>
       </c>
-      <c r="C299" s="25"/>
+      <c r="C299" s="20"/>
       <c r="E299" t="s">
         <v>357</v>
       </c>
@@ -7856,7 +7856,7 @@
       <c r="A300" t="s">
         <v>273</v>
       </c>
-      <c r="C300" s="25"/>
+      <c r="C300" s="20"/>
       <c r="D300" t="s">
         <v>729</v>
       </c>
@@ -7877,7 +7877,7 @@
       <c r="A301" t="s">
         <v>274</v>
       </c>
-      <c r="C301" s="25"/>
+      <c r="C301" s="20"/>
       <c r="E301" t="s">
         <v>357</v>
       </c>
@@ -7889,7 +7889,7 @@
       <c r="A302" t="s">
         <v>275</v>
       </c>
-      <c r="C302" s="25"/>
+      <c r="C302" s="20"/>
       <c r="E302" t="s">
         <v>357</v>
       </c>
@@ -7901,7 +7901,7 @@
       <c r="A303" t="s">
         <v>276</v>
       </c>
-      <c r="C303" s="25"/>
+      <c r="C303" s="20"/>
       <c r="E303" t="s">
         <v>364</v>
       </c>
@@ -7913,7 +7913,7 @@
       <c r="A304" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C304" s="26"/>
+      <c r="C304" s="21"/>
       <c r="D304" s="6" t="s">
         <v>730</v>
       </c>
@@ -7934,7 +7934,7 @@
       <c r="A305" t="s">
         <v>278</v>
       </c>
-      <c r="C305" s="24" t="s">
+      <c r="C305" s="19" t="s">
         <v>573</v>
       </c>
       <c r="E305" t="s">
@@ -7948,7 +7948,7 @@
       <c r="A306" t="s">
         <v>279</v>
       </c>
-      <c r="C306" s="25"/>
+      <c r="C306" s="20"/>
       <c r="E306" t="s">
         <v>357</v>
       </c>
@@ -7960,7 +7960,7 @@
       <c r="A307" t="s">
         <v>280</v>
       </c>
-      <c r="C307" s="25"/>
+      <c r="C307" s="20"/>
       <c r="E307" t="s">
         <v>357</v>
       </c>
@@ -7972,7 +7972,7 @@
       <c r="A308" t="s">
         <v>281</v>
       </c>
-      <c r="C308" s="25"/>
+      <c r="C308" s="20"/>
       <c r="E308" t="s">
         <v>357</v>
       </c>
@@ -7984,7 +7984,7 @@
       <c r="A309" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="C309" s="28"/>
+      <c r="C309" s="22"/>
       <c r="E309" s="12" t="s">
         <v>364</v>
       </c>
@@ -7996,7 +7996,7 @@
       <c r="A310" t="s">
         <v>283</v>
       </c>
-      <c r="C310" s="25" t="s">
+      <c r="C310" s="20" t="s">
         <v>574</v>
       </c>
       <c r="D310" t="s">
@@ -8016,7 +8016,7 @@
       <c r="A311" t="s">
         <v>284</v>
       </c>
-      <c r="C311" s="25"/>
+      <c r="C311" s="20"/>
       <c r="D311" t="s">
         <v>732</v>
       </c>
@@ -8034,7 +8034,7 @@
       <c r="A312" t="s">
         <v>285</v>
       </c>
-      <c r="C312" s="25"/>
+      <c r="C312" s="20"/>
       <c r="D312" t="s">
         <v>735</v>
       </c>
@@ -8052,7 +8052,7 @@
       <c r="A313" t="s">
         <v>286</v>
       </c>
-      <c r="C313" s="25"/>
+      <c r="C313" s="20"/>
       <c r="D313" t="s">
         <v>736</v>
       </c>
@@ -8070,7 +8070,7 @@
       <c r="A314" t="s">
         <v>287</v>
       </c>
-      <c r="C314" s="25"/>
+      <c r="C314" s="20"/>
       <c r="D314" t="s">
         <v>737</v>
       </c>
@@ -8088,7 +8088,7 @@
       <c r="A315" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C315" s="25"/>
+      <c r="C315" s="20"/>
       <c r="D315" s="6" t="s">
         <v>738</v>
       </c>
@@ -8137,7 +8137,7 @@
       <c r="A318" t="s">
         <v>291</v>
       </c>
-      <c r="C318" s="24" t="s">
+      <c r="C318" s="19" t="s">
         <v>577</v>
       </c>
       <c r="D318" t="s">
@@ -8152,22 +8152,22 @@
       <c r="H318" t="s">
         <v>634</v>
       </c>
-      <c r="I318" s="18" t="s">
+      <c r="I318" s="24" t="s">
         <v>783</v>
       </c>
-      <c r="J318" s="18"/>
-      <c r="K318" s="18"/>
-      <c r="L318" s="18"/>
-      <c r="M318" s="21" t="s">
+      <c r="J318" s="24"/>
+      <c r="K318" s="24"/>
+      <c r="L318" s="24"/>
+      <c r="M318" s="26" t="s">
         <v>785</v>
       </c>
-      <c r="N318" s="21"/>
+      <c r="N318" s="26"/>
     </row>
     <row r="319" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" t="s">
         <v>292</v>
       </c>
-      <c r="C319" s="25"/>
+      <c r="C319" s="20"/>
       <c r="D319" t="s">
         <v>744</v>
       </c>
@@ -8180,18 +8180,18 @@
       <c r="H319" t="s">
         <v>634</v>
       </c>
-      <c r="I319" s="19"/>
-      <c r="J319" s="19"/>
-      <c r="K319" s="19"/>
-      <c r="L319" s="19"/>
-      <c r="M319" s="22"/>
-      <c r="N319" s="22"/>
+      <c r="I319" s="23"/>
+      <c r="J319" s="23"/>
+      <c r="K319" s="23"/>
+      <c r="L319" s="23"/>
+      <c r="M319" s="27"/>
+      <c r="N319" s="27"/>
     </row>
     <row r="320" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" t="s">
         <v>293</v>
       </c>
-      <c r="C320" s="25"/>
+      <c r="C320" s="20"/>
       <c r="D320" t="s">
         <v>751</v>
       </c>
@@ -8207,84 +8207,84 @@
       <c r="H320" t="s">
         <v>634</v>
       </c>
-      <c r="I320" s="19"/>
-      <c r="J320" s="19"/>
-      <c r="K320" s="19"/>
-      <c r="L320" s="19"/>
-      <c r="M320" s="22"/>
-      <c r="N320" s="22"/>
+      <c r="I320" s="23"/>
+      <c r="J320" s="23"/>
+      <c r="K320" s="23"/>
+      <c r="L320" s="23"/>
+      <c r="M320" s="27"/>
+      <c r="N320" s="27"/>
     </row>
     <row r="321" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" t="s">
         <v>294</v>
       </c>
-      <c r="C321" s="25"/>
+      <c r="C321" s="20"/>
       <c r="E321" t="s">
         <v>357</v>
       </c>
       <c r="F321" t="s">
         <v>749</v>
       </c>
-      <c r="I321" s="19"/>
-      <c r="J321" s="19"/>
-      <c r="K321" s="19"/>
-      <c r="L321" s="19"/>
-      <c r="M321" s="22"/>
-      <c r="N321" s="22"/>
+      <c r="I321" s="23"/>
+      <c r="J321" s="23"/>
+      <c r="K321" s="23"/>
+      <c r="L321" s="23"/>
+      <c r="M321" s="27"/>
+      <c r="N321" s="27"/>
     </row>
     <row r="322" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" t="s">
         <v>295</v>
       </c>
-      <c r="C322" s="25"/>
+      <c r="C322" s="20"/>
       <c r="E322" t="s">
         <v>357</v>
       </c>
       <c r="F322" t="s">
         <v>750</v>
       </c>
-      <c r="I322" s="19"/>
-      <c r="J322" s="19"/>
-      <c r="K322" s="19"/>
-      <c r="L322" s="19"/>
-      <c r="M322" s="22"/>
-      <c r="N322" s="22"/>
+      <c r="I322" s="23"/>
+      <c r="J322" s="23"/>
+      <c r="K322" s="23"/>
+      <c r="L322" s="23"/>
+      <c r="M322" s="27"/>
+      <c r="N322" s="27"/>
     </row>
     <row r="323" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" t="s">
         <v>296</v>
       </c>
-      <c r="C323" s="25"/>
+      <c r="C323" s="20"/>
       <c r="E323" t="s">
         <v>357</v>
       </c>
       <c r="F323" t="s">
         <v>663</v>
       </c>
-      <c r="I323" s="19"/>
-      <c r="J323" s="19"/>
-      <c r="K323" s="19"/>
-      <c r="L323" s="19"/>
-      <c r="M323" s="22"/>
-      <c r="N323" s="22"/>
+      <c r="I323" s="23"/>
+      <c r="J323" s="23"/>
+      <c r="K323" s="23"/>
+      <c r="L323" s="23"/>
+      <c r="M323" s="27"/>
+      <c r="N323" s="27"/>
     </row>
     <row r="324" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="C324" s="26"/>
+      <c r="C324" s="21"/>
       <c r="E324" s="6" t="s">
         <v>364</v>
       </c>
       <c r="F324" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="I324" s="20"/>
-      <c r="J324" s="20"/>
-      <c r="K324" s="20"/>
-      <c r="L324" s="20"/>
-      <c r="M324" s="23"/>
-      <c r="N324" s="23"/>
+      <c r="I324" s="25"/>
+      <c r="J324" s="25"/>
+      <c r="K324" s="25"/>
+      <c r="L324" s="25"/>
+      <c r="M324" s="28"/>
+      <c r="N324" s="28"/>
     </row>
     <row r="325" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" s="17" t="s">
@@ -8310,7 +8310,7 @@
       <c r="A326" t="s">
         <v>582</v>
       </c>
-      <c r="C326" s="24" t="s">
+      <c r="C326" s="19" t="s">
         <v>759</v>
       </c>
       <c r="D326" t="s">
@@ -8325,16 +8325,16 @@
       <c r="H326" t="s">
         <v>634</v>
       </c>
-      <c r="M326" s="21" t="s">
+      <c r="M326" s="26" t="s">
         <v>785</v>
       </c>
-      <c r="N326" s="21"/>
+      <c r="N326" s="26"/>
     </row>
     <row r="327" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" t="s">
         <v>583</v>
       </c>
-      <c r="C327" s="25"/>
+      <c r="C327" s="20"/>
       <c r="D327" t="s">
         <v>763</v>
       </c>
@@ -8347,14 +8347,14 @@
       <c r="H327" t="s">
         <v>634</v>
       </c>
-      <c r="M327" s="22"/>
-      <c r="N327" s="22"/>
+      <c r="M327" s="27"/>
+      <c r="N327" s="27"/>
     </row>
     <row r="328" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" t="s">
         <v>301</v>
       </c>
-      <c r="C328" s="25"/>
+      <c r="C328" s="20"/>
       <c r="D328" t="s">
         <v>764</v>
       </c>
@@ -8367,14 +8367,14 @@
       <c r="H328" t="s">
         <v>634</v>
       </c>
-      <c r="M328" s="22"/>
-      <c r="N328" s="22"/>
+      <c r="M328" s="27"/>
+      <c r="N328" s="27"/>
     </row>
     <row r="329" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" t="s">
         <v>302</v>
       </c>
-      <c r="C329" s="25"/>
+      <c r="C329" s="20"/>
       <c r="D329" t="s">
         <v>765</v>
       </c>
@@ -8387,14 +8387,14 @@
       <c r="H329" t="s">
         <v>634</v>
       </c>
-      <c r="M329" s="22"/>
-      <c r="N329" s="22"/>
+      <c r="M329" s="27"/>
+      <c r="N329" s="27"/>
     </row>
     <row r="330" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" t="s">
         <v>303</v>
       </c>
-      <c r="C330" s="25"/>
+      <c r="C330" s="20"/>
       <c r="D330" t="s">
         <v>766</v>
       </c>
@@ -8407,14 +8407,14 @@
       <c r="H330" t="s">
         <v>634</v>
       </c>
-      <c r="M330" s="22"/>
-      <c r="N330" s="22"/>
+      <c r="M330" s="27"/>
+      <c r="N330" s="27"/>
     </row>
     <row r="331" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" t="s">
         <v>304</v>
       </c>
-      <c r="C331" s="25"/>
+      <c r="C331" s="20"/>
       <c r="D331" t="s">
         <v>767</v>
       </c>
@@ -8427,18 +8427,18 @@
       <c r="H331" t="s">
         <v>634</v>
       </c>
-      <c r="I331" s="27" t="s">
+      <c r="I331" s="18" t="s">
         <v>779</v>
       </c>
-      <c r="J331" s="27"/>
-      <c r="M331" s="22"/>
-      <c r="N331" s="22"/>
+      <c r="J331" s="18"/>
+      <c r="M331" s="27"/>
+      <c r="N331" s="27"/>
     </row>
     <row r="332" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" t="s">
         <v>584</v>
       </c>
-      <c r="C332" s="25"/>
+      <c r="C332" s="20"/>
       <c r="D332" t="s">
         <v>768</v>
       </c>
@@ -8451,16 +8451,16 @@
       <c r="H332" t="s">
         <v>634</v>
       </c>
-      <c r="I332" s="27"/>
-      <c r="J332" s="27"/>
-      <c r="M332" s="23"/>
-      <c r="N332" s="23"/>
+      <c r="I332" s="18"/>
+      <c r="J332" s="18"/>
+      <c r="M332" s="28"/>
+      <c r="N332" s="28"/>
     </row>
     <row r="333" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" s="6" t="s">
         <v>585</v>
       </c>
-      <c r="C333" s="26"/>
+      <c r="C333" s="21"/>
       <c r="D333" s="6" t="s">
         <v>769</v>
       </c>
@@ -8473,14 +8473,14 @@
       <c r="H333" s="6" t="s">
         <v>634</v>
       </c>
-      <c r="I333" s="27"/>
-      <c r="J333" s="27"/>
+      <c r="I333" s="18"/>
+      <c r="J333" s="18"/>
     </row>
     <row r="334" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" t="s">
         <v>752</v>
       </c>
-      <c r="C334" s="24" t="s">
+      <c r="C334" s="19" t="s">
         <v>758</v>
       </c>
       <c r="E334" t="s">
@@ -8489,64 +8489,64 @@
       <c r="F334" t="s">
         <v>674</v>
       </c>
-      <c r="I334" s="27"/>
-      <c r="J334" s="27"/>
+      <c r="I334" s="18"/>
+      <c r="J334" s="18"/>
     </row>
     <row r="335" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" t="s">
         <v>753</v>
       </c>
-      <c r="C335" s="25"/>
+      <c r="C335" s="20"/>
       <c r="E335" t="s">
         <v>357</v>
       </c>
       <c r="F335" t="s">
         <v>675</v>
       </c>
-      <c r="I335" s="27"/>
-      <c r="J335" s="27"/>
+      <c r="I335" s="18"/>
+      <c r="J335" s="18"/>
     </row>
     <row r="336" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" t="s">
         <v>754</v>
       </c>
-      <c r="C336" s="25"/>
+      <c r="C336" s="20"/>
       <c r="E336" t="s">
         <v>357</v>
       </c>
       <c r="F336" t="s">
         <v>778</v>
       </c>
-      <c r="I336" s="27"/>
-      <c r="J336" s="27"/>
+      <c r="I336" s="18"/>
+      <c r="J336" s="18"/>
     </row>
     <row r="337" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" t="s">
         <v>755</v>
       </c>
-      <c r="C337" s="25"/>
+      <c r="C337" s="20"/>
       <c r="E337" t="s">
         <v>357</v>
       </c>
       <c r="F337" t="s">
         <v>663</v>
       </c>
-      <c r="I337" s="27"/>
-      <c r="J337" s="27"/>
+      <c r="I337" s="18"/>
+      <c r="J337" s="18"/>
     </row>
     <row r="338" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" s="6" t="s">
         <v>756</v>
       </c>
-      <c r="C338" s="26"/>
+      <c r="C338" s="21"/>
       <c r="E338" s="6" t="s">
         <v>364</v>
       </c>
       <c r="F338" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="I338" s="27"/>
-      <c r="J338" s="27"/>
+      <c r="I338" s="18"/>
+      <c r="J338" s="18"/>
     </row>
     <row r="339" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" t="s">
@@ -8555,7 +8555,7 @@
       <c r="B339" t="s">
         <v>582</v>
       </c>
-      <c r="C339" s="24" t="s">
+      <c r="C339" s="19" t="s">
         <v>757</v>
       </c>
       <c r="D339" t="s">
@@ -8570,12 +8570,12 @@
       <c r="H339" t="s">
         <v>634</v>
       </c>
-      <c r="I339" s="27"/>
-      <c r="J339" s="27"/>
-      <c r="M339" s="21" t="s">
+      <c r="I339" s="18"/>
+      <c r="J339" s="18"/>
+      <c r="M339" s="26" t="s">
         <v>785</v>
       </c>
-      <c r="N339" s="21"/>
+      <c r="N339" s="26"/>
     </row>
     <row r="340" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" t="s">
@@ -8584,7 +8584,7 @@
       <c r="B340" t="s">
         <v>583</v>
       </c>
-      <c r="C340" s="25"/>
+      <c r="C340" s="20"/>
       <c r="D340" t="s">
         <v>763</v>
       </c>
@@ -8597,16 +8597,16 @@
       <c r="H340" t="s">
         <v>634</v>
       </c>
-      <c r="I340" s="27"/>
-      <c r="J340" s="27"/>
-      <c r="M340" s="22"/>
-      <c r="N340" s="22"/>
+      <c r="I340" s="18"/>
+      <c r="J340" s="18"/>
+      <c r="M340" s="27"/>
+      <c r="N340" s="27"/>
     </row>
     <row r="341" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" t="s">
         <v>301</v>
       </c>
-      <c r="C341" s="25"/>
+      <c r="C341" s="20"/>
       <c r="D341" t="s">
         <v>764</v>
       </c>
@@ -8619,16 +8619,16 @@
       <c r="H341" t="s">
         <v>634</v>
       </c>
-      <c r="I341" s="27"/>
-      <c r="J341" s="27"/>
-      <c r="M341" s="22"/>
-      <c r="N341" s="22"/>
+      <c r="I341" s="18"/>
+      <c r="J341" s="18"/>
+      <c r="M341" s="27"/>
+      <c r="N341" s="27"/>
     </row>
     <row r="342" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" t="s">
         <v>302</v>
       </c>
-      <c r="C342" s="25"/>
+      <c r="C342" s="20"/>
       <c r="D342" t="s">
         <v>765</v>
       </c>
@@ -8641,14 +8641,14 @@
       <c r="H342" t="s">
         <v>634</v>
       </c>
-      <c r="M342" s="22"/>
-      <c r="N342" s="22"/>
+      <c r="M342" s="27"/>
+      <c r="N342" s="27"/>
     </row>
     <row r="343" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" t="s">
         <v>303</v>
       </c>
-      <c r="C343" s="25"/>
+      <c r="C343" s="20"/>
       <c r="D343" t="s">
         <v>766</v>
       </c>
@@ -8661,14 +8661,14 @@
       <c r="H343" t="s">
         <v>634</v>
       </c>
-      <c r="M343" s="22"/>
-      <c r="N343" s="22"/>
+      <c r="M343" s="27"/>
+      <c r="N343" s="27"/>
     </row>
     <row r="344" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" t="s">
         <v>304</v>
       </c>
-      <c r="C344" s="25"/>
+      <c r="C344" s="20"/>
       <c r="D344" t="s">
         <v>767</v>
       </c>
@@ -8681,8 +8681,8 @@
       <c r="H344" t="s">
         <v>634</v>
       </c>
-      <c r="M344" s="22"/>
-      <c r="N344" s="22"/>
+      <c r="M344" s="27"/>
+      <c r="N344" s="27"/>
     </row>
     <row r="345" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" t="s">
@@ -8691,7 +8691,7 @@
       <c r="B345" t="s">
         <v>584</v>
       </c>
-      <c r="C345" s="25"/>
+      <c r="C345" s="20"/>
       <c r="D345" t="s">
         <v>768</v>
       </c>
@@ -8704,8 +8704,8 @@
       <c r="H345" t="s">
         <v>634</v>
       </c>
-      <c r="M345" s="23"/>
-      <c r="N345" s="23"/>
+      <c r="M345" s="28"/>
+      <c r="N345" s="28"/>
     </row>
     <row r="346" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" s="6" t="s">
@@ -8714,7 +8714,7 @@
       <c r="B346" s="6" t="s">
         <v>585</v>
       </c>
-      <c r="C346" s="26"/>
+      <c r="C346" s="21"/>
       <c r="D346" s="6" t="s">
         <v>769</v>
       </c>
@@ -8732,7 +8732,7 @@
       <c r="A347" t="s">
         <v>307</v>
       </c>
-      <c r="C347" s="24" t="s">
+      <c r="C347" s="19" t="s">
         <v>578</v>
       </c>
       <c r="E347" t="s">
@@ -8746,7 +8746,7 @@
       <c r="A348" t="s">
         <v>308</v>
       </c>
-      <c r="C348" s="25"/>
+      <c r="C348" s="20"/>
       <c r="E348" t="s">
         <v>357</v>
       </c>
@@ -8758,7 +8758,7 @@
       <c r="A349" t="s">
         <v>309</v>
       </c>
-      <c r="C349" s="25"/>
+      <c r="C349" s="20"/>
       <c r="E349" t="s">
         <v>357</v>
       </c>
@@ -8770,7 +8770,7 @@
       <c r="A350" t="s">
         <v>310</v>
       </c>
-      <c r="C350" s="25"/>
+      <c r="C350" s="20"/>
       <c r="E350" t="s">
         <v>357</v>
       </c>
@@ -8782,7 +8782,7 @@
       <c r="A351" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="C351" s="26"/>
+      <c r="C351" s="21"/>
       <c r="E351" s="6" t="s">
         <v>364</v>
       </c>
@@ -8794,7 +8794,7 @@
       <c r="A352" t="s">
         <v>312</v>
       </c>
-      <c r="C352" s="25" t="s">
+      <c r="C352" s="20" t="s">
         <v>579</v>
       </c>
       <c r="D352" t="s">
@@ -8809,22 +8809,22 @@
       <c r="H352" t="s">
         <v>636</v>
       </c>
-      <c r="I352" s="18" t="s">
+      <c r="I352" s="24" t="s">
         <v>783</v>
       </c>
-      <c r="J352" s="18"/>
-      <c r="K352" s="18"/>
-      <c r="L352" s="18"/>
-      <c r="M352" s="21" t="s">
+      <c r="J352" s="24"/>
+      <c r="K352" s="24"/>
+      <c r="L352" s="24"/>
+      <c r="M352" s="26" t="s">
         <v>785</v>
       </c>
-      <c r="N352" s="21"/>
+      <c r="N352" s="26"/>
     </row>
     <row r="353" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" t="s">
         <v>313</v>
       </c>
-      <c r="C353" s="25"/>
+      <c r="C353" s="20"/>
       <c r="D353" t="s">
         <v>781</v>
       </c>
@@ -8837,18 +8837,18 @@
       <c r="H353" t="s">
         <v>636</v>
       </c>
-      <c r="I353" s="19"/>
-      <c r="J353" s="19"/>
-      <c r="K353" s="19"/>
-      <c r="L353" s="19"/>
-      <c r="M353" s="22"/>
-      <c r="N353" s="22"/>
+      <c r="I353" s="23"/>
+      <c r="J353" s="23"/>
+      <c r="K353" s="23"/>
+      <c r="L353" s="23"/>
+      <c r="M353" s="27"/>
+      <c r="N353" s="27"/>
     </row>
     <row r="354" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" t="s">
         <v>314</v>
       </c>
-      <c r="C354" s="25"/>
+      <c r="C354" s="20"/>
       <c r="D354" t="s">
         <v>782</v>
       </c>
@@ -8864,18 +8864,18 @@
       <c r="H354" t="s">
         <v>636</v>
       </c>
-      <c r="I354" s="19"/>
-      <c r="J354" s="19"/>
-      <c r="K354" s="19"/>
-      <c r="L354" s="19"/>
-      <c r="M354" s="22"/>
-      <c r="N354" s="22"/>
+      <c r="I354" s="23"/>
+      <c r="J354" s="23"/>
+      <c r="K354" s="23"/>
+      <c r="L354" s="23"/>
+      <c r="M354" s="27"/>
+      <c r="N354" s="27"/>
     </row>
     <row r="355" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" t="s">
         <v>315</v>
       </c>
-      <c r="C355" s="25"/>
+      <c r="C355" s="20"/>
       <c r="E355" t="s">
         <v>357</v>
       </c>
@@ -8885,18 +8885,18 @@
       <c r="H355" t="s">
         <v>636</v>
       </c>
-      <c r="I355" s="19"/>
-      <c r="J355" s="19"/>
-      <c r="K355" s="19"/>
-      <c r="L355" s="19"/>
-      <c r="M355" s="22"/>
-      <c r="N355" s="22"/>
+      <c r="I355" s="23"/>
+      <c r="J355" s="23"/>
+      <c r="K355" s="23"/>
+      <c r="L355" s="23"/>
+      <c r="M355" s="27"/>
+      <c r="N355" s="27"/>
     </row>
     <row r="356" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" t="s">
         <v>316</v>
       </c>
-      <c r="C356" s="25"/>
+      <c r="C356" s="20"/>
       <c r="E356" t="s">
         <v>357</v>
       </c>
@@ -8906,18 +8906,18 @@
       <c r="H356" t="s">
         <v>636</v>
       </c>
-      <c r="I356" s="19"/>
-      <c r="J356" s="19"/>
-      <c r="K356" s="19"/>
-      <c r="L356" s="19"/>
-      <c r="M356" s="22"/>
-      <c r="N356" s="22"/>
+      <c r="I356" s="23"/>
+      <c r="J356" s="23"/>
+      <c r="K356" s="23"/>
+      <c r="L356" s="23"/>
+      <c r="M356" s="27"/>
+      <c r="N356" s="27"/>
     </row>
     <row r="357" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" t="s">
         <v>317</v>
       </c>
-      <c r="C357" s="25"/>
+      <c r="C357" s="20"/>
       <c r="E357" t="s">
         <v>357</v>
       </c>
@@ -8927,18 +8927,18 @@
       <c r="H357" t="s">
         <v>636</v>
       </c>
-      <c r="I357" s="19"/>
-      <c r="J357" s="19"/>
-      <c r="K357" s="19"/>
-      <c r="L357" s="19"/>
-      <c r="M357" s="22"/>
-      <c r="N357" s="22"/>
+      <c r="I357" s="23"/>
+      <c r="J357" s="23"/>
+      <c r="K357" s="23"/>
+      <c r="L357" s="23"/>
+      <c r="M357" s="27"/>
+      <c r="N357" s="27"/>
     </row>
     <row r="358" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A358" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="C358" s="26"/>
+      <c r="C358" s="21"/>
       <c r="E358" s="6" t="s">
         <v>364</v>
       </c>
@@ -8948,18 +8948,18 @@
       <c r="H358" s="6" t="s">
         <v>636</v>
       </c>
-      <c r="I358" s="20"/>
-      <c r="J358" s="20"/>
-      <c r="K358" s="20"/>
-      <c r="L358" s="20"/>
-      <c r="M358" s="23"/>
-      <c r="N358" s="23"/>
+      <c r="I358" s="25"/>
+      <c r="J358" s="25"/>
+      <c r="K358" s="25"/>
+      <c r="L358" s="25"/>
+      <c r="M358" s="28"/>
+      <c r="N358" s="28"/>
     </row>
     <row r="359" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" t="s">
         <v>319</v>
       </c>
-      <c r="C359" s="25" t="s">
+      <c r="C359" s="20" t="s">
         <v>580</v>
       </c>
       <c r="D359" t="s">
@@ -8979,7 +8979,7 @@
       <c r="A360" t="s">
         <v>320</v>
       </c>
-      <c r="C360" s="25"/>
+      <c r="C360" s="20"/>
       <c r="D360" t="s">
         <v>788</v>
       </c>
@@ -8997,7 +8997,7 @@
       <c r="A361" t="s">
         <v>321</v>
       </c>
-      <c r="C361" s="25"/>
+      <c r="C361" s="20"/>
       <c r="D361" t="s">
         <v>789</v>
       </c>
@@ -9015,7 +9015,7 @@
       <c r="A362" t="s">
         <v>322</v>
       </c>
-      <c r="C362" s="25"/>
+      <c r="C362" s="20"/>
       <c r="D362" t="s">
         <v>790</v>
       </c>
@@ -9033,7 +9033,7 @@
       <c r="A363" t="s">
         <v>323</v>
       </c>
-      <c r="C363" s="25"/>
+      <c r="C363" s="20"/>
       <c r="D363" t="s">
         <v>791</v>
       </c>
@@ -9051,7 +9051,7 @@
       <c r="A364" t="s">
         <v>324</v>
       </c>
-      <c r="C364" s="25"/>
+      <c r="C364" s="20"/>
       <c r="D364" t="s">
         <v>792</v>
       </c>
@@ -9069,7 +9069,7 @@
       <c r="A365" t="s">
         <v>325</v>
       </c>
-      <c r="C365" s="25"/>
+      <c r="C365" s="20"/>
       <c r="D365" t="s">
         <v>793</v>
       </c>
@@ -9087,7 +9087,7 @@
       <c r="A366" t="s">
         <v>326</v>
       </c>
-      <c r="C366" s="25"/>
+      <c r="C366" s="20"/>
       <c r="D366" t="s">
         <v>794</v>
       </c>
@@ -9105,7 +9105,7 @@
       <c r="A367" t="s">
         <v>327</v>
       </c>
-      <c r="C367" s="25"/>
+      <c r="C367" s="20"/>
       <c r="E367" t="s">
         <v>357</v>
       </c>
@@ -9117,7 +9117,7 @@
       <c r="A368" t="s">
         <v>328</v>
       </c>
-      <c r="C368" s="25"/>
+      <c r="C368" s="20"/>
       <c r="E368" t="s">
         <v>357</v>
       </c>
@@ -9129,7 +9129,7 @@
       <c r="A369" t="s">
         <v>329</v>
       </c>
-      <c r="C369" s="25"/>
+      <c r="C369" s="20"/>
       <c r="E369" t="s">
         <v>357</v>
       </c>
@@ -9141,7 +9141,7 @@
       <c r="A370" t="s">
         <v>330</v>
       </c>
-      <c r="C370" s="25"/>
+      <c r="C370" s="20"/>
       <c r="E370" t="s">
         <v>357</v>
       </c>
@@ -9153,7 +9153,7 @@
       <c r="A371" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C371" s="28"/>
+      <c r="C371" s="22"/>
       <c r="E371" s="12" t="s">
         <v>364</v>
       </c>
@@ -9164,6 +9164,46 @@
     <row r="372" spans="1:6" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="I352:L358"/>
+    <mergeCell ref="I318:L324"/>
+    <mergeCell ref="M318:N324"/>
+    <mergeCell ref="M326:N332"/>
+    <mergeCell ref="M339:N345"/>
+    <mergeCell ref="M352:N358"/>
+    <mergeCell ref="I262:K265"/>
+    <mergeCell ref="C326:C333"/>
+    <mergeCell ref="C334:C338"/>
+    <mergeCell ref="I331:J341"/>
+    <mergeCell ref="I1:L12"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C41:C48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C51:C58"/>
+    <mergeCell ref="C59:C63"/>
+    <mergeCell ref="C64:C68"/>
+    <mergeCell ref="C9:C17"/>
+    <mergeCell ref="C18:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="C28:C35"/>
+    <mergeCell ref="C112:C130"/>
+    <mergeCell ref="C131:C135"/>
+    <mergeCell ref="C136:C151"/>
+    <mergeCell ref="C153:C157"/>
+    <mergeCell ref="C71:C78"/>
+    <mergeCell ref="C79:C86"/>
+    <mergeCell ref="C87:C91"/>
+    <mergeCell ref="C92:C110"/>
+    <mergeCell ref="C158:C162"/>
+    <mergeCell ref="C163:C168"/>
+    <mergeCell ref="C169:C182"/>
+    <mergeCell ref="C183:C187"/>
+    <mergeCell ref="C188:C189"/>
+    <mergeCell ref="C190:C194"/>
+    <mergeCell ref="C195:C199"/>
+    <mergeCell ref="C200:C204"/>
+    <mergeCell ref="C205:C209"/>
+    <mergeCell ref="C210:C226"/>
     <mergeCell ref="I165:M168"/>
     <mergeCell ref="C318:C324"/>
     <mergeCell ref="C347:C351"/>
@@ -9180,46 +9220,6 @@
     <mergeCell ref="C246:C247"/>
     <mergeCell ref="C248:C252"/>
     <mergeCell ref="C253:C261"/>
-    <mergeCell ref="C190:C194"/>
-    <mergeCell ref="C195:C199"/>
-    <mergeCell ref="C200:C204"/>
-    <mergeCell ref="C205:C209"/>
-    <mergeCell ref="C210:C226"/>
-    <mergeCell ref="C158:C162"/>
-    <mergeCell ref="C163:C168"/>
-    <mergeCell ref="C169:C182"/>
-    <mergeCell ref="C183:C187"/>
-    <mergeCell ref="C188:C189"/>
-    <mergeCell ref="C112:C130"/>
-    <mergeCell ref="C131:C135"/>
-    <mergeCell ref="C136:C151"/>
-    <mergeCell ref="C153:C157"/>
-    <mergeCell ref="C71:C78"/>
-    <mergeCell ref="C79:C86"/>
-    <mergeCell ref="C87:C91"/>
-    <mergeCell ref="C92:C110"/>
-    <mergeCell ref="I262:K265"/>
-    <mergeCell ref="C326:C333"/>
-    <mergeCell ref="C334:C338"/>
-    <mergeCell ref="I331:J341"/>
-    <mergeCell ref="I1:L12"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C41:C48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C51:C58"/>
-    <mergeCell ref="C59:C63"/>
-    <mergeCell ref="C64:C68"/>
-    <mergeCell ref="C9:C17"/>
-    <mergeCell ref="C18:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="C28:C35"/>
-    <mergeCell ref="I352:L358"/>
-    <mergeCell ref="I318:L324"/>
-    <mergeCell ref="M318:N324"/>
-    <mergeCell ref="M326:N332"/>
-    <mergeCell ref="M339:N345"/>
-    <mergeCell ref="M352:N358"/>
   </mergeCells>
   <conditionalFormatting sqref="I262 H1:H264 H266:H290 H292:H304 H306:H1048576">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">

</xml_diff>

<commit_message>
Added code to separate SART into practice and actual tasks, removed extra rows and columns, renamed columns, increased counters to start at 1.
</commit_message>
<xml_diff>
--- a/PsychoPyData_ColumnKey.xlsx
+++ b/PsychoPyData_ColumnKey.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1738" documentId="8_{447AABAE-0265-45CA-9969-8E24E37FF3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECCC3420-6B50-4F27-A63C-EB751776FFE5}"/>
   <bookViews>
-    <workbookView xWindow="8214" yWindow="168" windowWidth="14442" windowHeight="8124" xr2:uid="{5015AFB7-EBCA-4E4E-B1B8-96F1F0B54514}"/>
+    <workbookView xWindow="228" yWindow="2592" windowWidth="10800" windowHeight="10608" xr2:uid="{5015AFB7-EBCA-4E4E-B1B8-96F1F0B54514}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2556,25 +2556,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2588,6 +2573,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2954,10 +2954,10 @@
   <dimension ref="A1:N372"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2997,12 +2997,12 @@
       <c r="H1" t="s">
         <v>335</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="19" t="s">
         <v>799</v>
       </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
@@ -3020,10 +3020,10 @@
       <c r="H2" t="s">
         <v>632</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
@@ -3041,10 +3041,10 @@
       <c r="H3" t="s">
         <v>633</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -3062,10 +3062,10 @@
       <c r="H4" t="s">
         <v>632</v>
       </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
@@ -3083,10 +3083,10 @@
       <c r="H5" t="s">
         <v>632</v>
       </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
@@ -3104,10 +3104,10 @@
       <c r="H6" t="s">
         <v>632</v>
       </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -3125,10 +3125,10 @@
       <c r="H7" t="s">
         <v>632</v>
       </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:12" s="12" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="12" t="s">
@@ -3147,16 +3147,16 @@
       <c r="H8" s="12" t="s">
         <v>632</v>
       </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
     </row>
     <row r="9" spans="1:12" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="24" t="s">
         <v>532</v>
       </c>
       <c r="E9" t="s">
@@ -3165,16 +3165,16 @@
       <c r="F9" t="s">
         <v>398</v>
       </c>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="25"/>
       <c r="E10" t="s">
         <v>357</v>
       </c>
@@ -3184,16 +3184,16 @@
       <c r="H10" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="20"/>
+      <c r="C11" s="25"/>
       <c r="E11" t="s">
         <v>357</v>
       </c>
@@ -3203,16 +3203,16 @@
       <c r="H11" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="25"/>
       <c r="E12" t="s">
         <v>357</v>
       </c>
@@ -3222,16 +3222,16 @@
       <c r="H12" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="20"/>
+      <c r="C13" s="25"/>
       <c r="E13" t="s">
         <v>364</v>
       </c>
@@ -3243,7 +3243,7 @@
       <c r="A14" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="25"/>
       <c r="E14" t="s">
         <v>364</v>
       </c>
@@ -3258,7 +3258,7 @@
       <c r="A15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="20"/>
+      <c r="C15" s="25"/>
       <c r="E15" t="s">
         <v>364</v>
       </c>
@@ -3273,7 +3273,7 @@
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="25"/>
       <c r="E16" t="s">
         <v>364</v>
       </c>
@@ -3288,7 +3288,7 @@
       <c r="A17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="28"/>
       <c r="E17" s="12" t="s">
         <v>364</v>
       </c>
@@ -3303,7 +3303,7 @@
       <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="25" t="s">
         <v>533</v>
       </c>
       <c r="D18" t="s">
@@ -3323,7 +3323,7 @@
       <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="20"/>
+      <c r="C19" s="25"/>
       <c r="D19" t="s">
         <v>353</v>
       </c>
@@ -3341,7 +3341,7 @@
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="20"/>
+      <c r="C20" s="25"/>
       <c r="D20" t="s">
         <v>354</v>
       </c>
@@ -3362,7 +3362,7 @@
       <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="25"/>
       <c r="E21" t="s">
         <v>357</v>
       </c>
@@ -3374,7 +3374,7 @@
       <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="20"/>
+      <c r="C22" s="25"/>
       <c r="E22" t="s">
         <v>357</v>
       </c>
@@ -3389,7 +3389,7 @@
       <c r="A23" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="20"/>
+      <c r="C23" s="25"/>
       <c r="D23" t="s">
         <v>384</v>
       </c>
@@ -3410,7 +3410,7 @@
       <c r="A24" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="20"/>
+      <c r="C24" s="25"/>
       <c r="E24" t="s">
         <v>357</v>
       </c>
@@ -3422,7 +3422,7 @@
       <c r="A25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="21"/>
+      <c r="C25" s="26"/>
       <c r="E25" s="6" t="s">
         <v>364</v>
       </c>
@@ -3434,7 +3434,7 @@
       <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="24" t="s">
         <v>534</v>
       </c>
       <c r="D26" t="s">
@@ -3457,7 +3457,7 @@
       <c r="A27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="21"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="6" t="s">
         <v>409</v>
       </c>
@@ -3478,7 +3478,7 @@
       <c r="A28" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="25" t="s">
         <v>535</v>
       </c>
       <c r="D28" t="s">
@@ -3501,7 +3501,7 @@
       <c r="A29" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="20"/>
+      <c r="C29" s="25"/>
       <c r="D29" t="s">
         <v>348</v>
       </c>
@@ -3519,7 +3519,7 @@
       <c r="A30" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="20"/>
+      <c r="C30" s="25"/>
       <c r="D30" t="s">
         <v>378</v>
       </c>
@@ -3537,7 +3537,7 @@
       <c r="A31" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="20"/>
+      <c r="C31" s="25"/>
       <c r="E31" t="s">
         <v>357</v>
       </c>
@@ -3549,7 +3549,7 @@
       <c r="A32" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="20"/>
+      <c r="C32" s="25"/>
       <c r="E32" t="s">
         <v>357</v>
       </c>
@@ -3561,7 +3561,7 @@
       <c r="A33" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="20"/>
+      <c r="C33" s="25"/>
       <c r="D33" t="s">
         <v>385</v>
       </c>
@@ -3582,7 +3582,7 @@
       <c r="A34" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="20"/>
+      <c r="C34" s="25"/>
       <c r="E34" t="s">
         <v>357</v>
       </c>
@@ -3594,7 +3594,7 @@
       <c r="A35" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="21"/>
+      <c r="C35" s="26"/>
       <c r="E35" s="6" t="s">
         <v>364</v>
       </c>
@@ -3606,7 +3606,7 @@
       <c r="A36" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="24" t="s">
         <v>536</v>
       </c>
       <c r="E36" t="s">
@@ -3620,7 +3620,7 @@
       <c r="A37" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="20"/>
+      <c r="C37" s="25"/>
       <c r="E37" t="s">
         <v>357</v>
       </c>
@@ -3632,7 +3632,7 @@
       <c r="A38" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="20"/>
+      <c r="C38" s="25"/>
       <c r="E38" t="s">
         <v>357</v>
       </c>
@@ -3644,7 +3644,7 @@
       <c r="A39" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="20"/>
+      <c r="C39" s="25"/>
       <c r="E39" t="s">
         <v>357</v>
       </c>
@@ -3656,7 +3656,7 @@
       <c r="A40" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="22"/>
+      <c r="C40" s="28"/>
       <c r="E40" s="12" t="s">
         <v>364</v>
       </c>
@@ -3668,7 +3668,7 @@
       <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="25" t="s">
         <v>537</v>
       </c>
       <c r="D41" t="s">
@@ -3691,7 +3691,7 @@
       <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="20"/>
+      <c r="C42" s="25"/>
       <c r="D42" t="s">
         <v>411</v>
       </c>
@@ -3712,7 +3712,7 @@
       <c r="A43" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="20"/>
+      <c r="C43" s="25"/>
       <c r="D43" t="s">
         <v>412</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="A44" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="20"/>
+      <c r="C44" s="25"/>
       <c r="E44" t="s">
         <v>357</v>
       </c>
@@ -3745,7 +3745,7 @@
       <c r="A45" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="20"/>
+      <c r="C45" s="25"/>
       <c r="E45" t="s">
         <v>357</v>
       </c>
@@ -3757,7 +3757,7 @@
       <c r="A46" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="20"/>
+      <c r="C46" s="25"/>
       <c r="D46" t="s">
         <v>413</v>
       </c>
@@ -3778,7 +3778,7 @@
       <c r="A47" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="20"/>
+      <c r="C47" s="25"/>
       <c r="E47" t="s">
         <v>357</v>
       </c>
@@ -3790,7 +3790,7 @@
       <c r="A48" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="21"/>
+      <c r="C48" s="26"/>
       <c r="E48" s="6" t="s">
         <v>364</v>
       </c>
@@ -3802,7 +3802,7 @@
       <c r="A49" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="24" t="s">
         <v>538</v>
       </c>
       <c r="D49" t="s">
@@ -3825,7 +3825,7 @@
       <c r="A50" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="21"/>
+      <c r="C50" s="26"/>
       <c r="D50" s="6" t="s">
         <v>422</v>
       </c>
@@ -3846,7 +3846,7 @@
       <c r="A51" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="24" t="s">
         <v>539</v>
       </c>
       <c r="D51" t="s">
@@ -3869,7 +3869,7 @@
       <c r="A52" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="20"/>
+      <c r="C52" s="25"/>
       <c r="D52" t="s">
         <v>415</v>
       </c>
@@ -3890,7 +3890,7 @@
       <c r="A53" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="20"/>
+      <c r="C53" s="25"/>
       <c r="D53" t="s">
         <v>416</v>
       </c>
@@ -3911,7 +3911,7 @@
       <c r="A54" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="20"/>
+      <c r="C54" s="25"/>
       <c r="E54" t="s">
         <v>357</v>
       </c>
@@ -3923,7 +3923,7 @@
       <c r="A55" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="20"/>
+      <c r="C55" s="25"/>
       <c r="E55" t="s">
         <v>357</v>
       </c>
@@ -3935,7 +3935,7 @@
       <c r="A56" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="20"/>
+      <c r="C56" s="25"/>
       <c r="D56" t="s">
         <v>417</v>
       </c>
@@ -3956,7 +3956,7 @@
       <c r="A57" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="20"/>
+      <c r="C57" s="25"/>
       <c r="E57" t="s">
         <v>357</v>
       </c>
@@ -3968,7 +3968,7 @@
       <c r="A58" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="21"/>
+      <c r="C58" s="26"/>
       <c r="E58" s="6" t="s">
         <v>364</v>
       </c>
@@ -3980,7 +3980,7 @@
       <c r="A59" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="C59" s="24" t="s">
         <v>540</v>
       </c>
       <c r="E59" t="s">
@@ -3994,7 +3994,7 @@
       <c r="A60" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="20"/>
+      <c r="C60" s="25"/>
       <c r="E60" t="s">
         <v>357</v>
       </c>
@@ -4006,7 +4006,7 @@
       <c r="A61" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="20"/>
+      <c r="C61" s="25"/>
       <c r="E61" t="s">
         <v>357</v>
       </c>
@@ -4018,7 +4018,7 @@
       <c r="A62" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="20"/>
+      <c r="C62" s="25"/>
       <c r="E62" t="s">
         <v>357</v>
       </c>
@@ -4030,7 +4030,7 @@
       <c r="A63" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C63" s="21"/>
+      <c r="C63" s="26"/>
       <c r="E63" s="6" t="s">
         <v>364</v>
       </c>
@@ -4042,7 +4042,7 @@
       <c r="A64" t="s">
         <v>61</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="24" t="s">
         <v>541</v>
       </c>
       <c r="E64" t="s">
@@ -4056,7 +4056,7 @@
       <c r="A65" t="s">
         <v>62</v>
       </c>
-      <c r="C65" s="20"/>
+      <c r="C65" s="25"/>
       <c r="E65" t="s">
         <v>357</v>
       </c>
@@ -4068,7 +4068,7 @@
       <c r="A66" t="s">
         <v>63</v>
       </c>
-      <c r="C66" s="20"/>
+      <c r="C66" s="25"/>
       <c r="E66" t="s">
         <v>357</v>
       </c>
@@ -4083,7 +4083,7 @@
       <c r="A67" t="s">
         <v>64</v>
       </c>
-      <c r="C67" s="20"/>
+      <c r="C67" s="25"/>
       <c r="E67" t="s">
         <v>357</v>
       </c>
@@ -4098,7 +4098,7 @@
       <c r="A68" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C68" s="21"/>
+      <c r="C68" s="26"/>
       <c r="E68" s="6" t="s">
         <v>364</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="24" t="s">
         <v>542</v>
       </c>
       <c r="E69" t="s">
@@ -4129,7 +4129,7 @@
         <v>67</v>
       </c>
       <c r="B70" s="10"/>
-      <c r="C70" s="21"/>
+      <c r="C70" s="26"/>
       <c r="E70" s="6" t="s">
         <v>364</v>
       </c>
@@ -4144,7 +4144,7 @@
       <c r="A71" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="24" t="s">
         <v>543</v>
       </c>
       <c r="D71" t="s">
@@ -4167,7 +4167,7 @@
       <c r="A72" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="20"/>
+      <c r="C72" s="25"/>
       <c r="D72" t="s">
         <v>428</v>
       </c>
@@ -4188,7 +4188,7 @@
       <c r="A73" t="s">
         <v>70</v>
       </c>
-      <c r="C73" s="20"/>
+      <c r="C73" s="25"/>
       <c r="D73" t="s">
         <v>429</v>
       </c>
@@ -4209,7 +4209,7 @@
       <c r="A74" t="s">
         <v>71</v>
       </c>
-      <c r="C74" s="20"/>
+      <c r="C74" s="25"/>
       <c r="E74" t="s">
         <v>357</v>
       </c>
@@ -4221,7 +4221,7 @@
       <c r="A75" t="s">
         <v>72</v>
       </c>
-      <c r="C75" s="20"/>
+      <c r="C75" s="25"/>
       <c r="E75" t="s">
         <v>357</v>
       </c>
@@ -4233,7 +4233,7 @@
       <c r="A76" t="s">
         <v>73</v>
       </c>
-      <c r="C76" s="20"/>
+      <c r="C76" s="25"/>
       <c r="D76" t="s">
         <v>433</v>
       </c>
@@ -4254,7 +4254,7 @@
       <c r="A77" t="s">
         <v>74</v>
       </c>
-      <c r="C77" s="20"/>
+      <c r="C77" s="25"/>
       <c r="E77" t="s">
         <v>357</v>
       </c>
@@ -4266,7 +4266,7 @@
       <c r="A78" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C78" s="21"/>
+      <c r="C78" s="26"/>
       <c r="E78" s="6" t="s">
         <v>364</v>
       </c>
@@ -4278,7 +4278,7 @@
       <c r="A79" t="s">
         <v>76</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="C79" s="24" t="s">
         <v>544</v>
       </c>
       <c r="D79" t="s">
@@ -4301,7 +4301,7 @@
       <c r="A80" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="20"/>
+      <c r="C80" s="25"/>
       <c r="D80" t="s">
         <v>436</v>
       </c>
@@ -4322,7 +4322,7 @@
       <c r="A81" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="20"/>
+      <c r="C81" s="25"/>
       <c r="D81" t="s">
         <v>437</v>
       </c>
@@ -4343,7 +4343,7 @@
       <c r="A82" t="s">
         <v>79</v>
       </c>
-      <c r="C82" s="20"/>
+      <c r="C82" s="25"/>
       <c r="E82" t="s">
         <v>357</v>
       </c>
@@ -4355,7 +4355,7 @@
       <c r="A83" t="s">
         <v>80</v>
       </c>
-      <c r="C83" s="20"/>
+      <c r="C83" s="25"/>
       <c r="E83" t="s">
         <v>357</v>
       </c>
@@ -4367,7 +4367,7 @@
       <c r="A84" t="s">
         <v>81</v>
       </c>
-      <c r="C84" s="20"/>
+      <c r="C84" s="25"/>
       <c r="D84" t="s">
         <v>435</v>
       </c>
@@ -4388,7 +4388,7 @@
       <c r="A85" t="s">
         <v>82</v>
       </c>
-      <c r="C85" s="20"/>
+      <c r="C85" s="25"/>
       <c r="E85" t="s">
         <v>357</v>
       </c>
@@ -4400,7 +4400,7 @@
       <c r="A86" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C86" s="21"/>
+      <c r="C86" s="26"/>
       <c r="E86" s="6" t="s">
         <v>364</v>
       </c>
@@ -4412,7 +4412,7 @@
       <c r="A87" t="s">
         <v>84</v>
       </c>
-      <c r="C87" s="19" t="s">
+      <c r="C87" s="24" t="s">
         <v>545</v>
       </c>
       <c r="E87" t="s">
@@ -4426,7 +4426,7 @@
       <c r="A88" t="s">
         <v>85</v>
       </c>
-      <c r="C88" s="20"/>
+      <c r="C88" s="25"/>
       <c r="E88" t="s">
         <v>357</v>
       </c>
@@ -4438,7 +4438,7 @@
       <c r="A89" t="s">
         <v>86</v>
       </c>
-      <c r="C89" s="20"/>
+      <c r="C89" s="25"/>
       <c r="E89" t="s">
         <v>357</v>
       </c>
@@ -4450,7 +4450,7 @@
       <c r="A90" t="s">
         <v>87</v>
       </c>
-      <c r="C90" s="20"/>
+      <c r="C90" s="25"/>
       <c r="E90" t="s">
         <v>357</v>
       </c>
@@ -4462,7 +4462,7 @@
       <c r="A91" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="21"/>
+      <c r="C91" s="26"/>
       <c r="E91" s="6" t="s">
         <v>364</v>
       </c>
@@ -4474,7 +4474,7 @@
       <c r="A92" t="s">
         <v>89</v>
       </c>
-      <c r="C92" s="19" t="s">
+      <c r="C92" s="24" t="s">
         <v>546</v>
       </c>
       <c r="D92" t="s">
@@ -4497,7 +4497,7 @@
       <c r="A93" t="s">
         <v>90</v>
       </c>
-      <c r="C93" s="20"/>
+      <c r="C93" s="25"/>
       <c r="D93" t="s">
         <v>448</v>
       </c>
@@ -4518,7 +4518,7 @@
       <c r="A94" t="s">
         <v>91</v>
       </c>
-      <c r="C94" s="20"/>
+      <c r="C94" s="25"/>
       <c r="D94" t="s">
         <v>450</v>
       </c>
@@ -4539,7 +4539,7 @@
       <c r="A95" t="s">
         <v>92</v>
       </c>
-      <c r="C95" s="20"/>
+      <c r="C95" s="25"/>
       <c r="D95" t="s">
         <v>453</v>
       </c>
@@ -4560,7 +4560,7 @@
       <c r="A96" t="s">
         <v>93</v>
       </c>
-      <c r="C96" s="20"/>
+      <c r="C96" s="25"/>
       <c r="D96" t="s">
         <v>454</v>
       </c>
@@ -4581,7 +4581,7 @@
       <c r="A97" t="s">
         <v>94</v>
       </c>
-      <c r="C97" s="20"/>
+      <c r="C97" s="25"/>
       <c r="D97" t="s">
         <v>455</v>
       </c>
@@ -4602,7 +4602,7 @@
       <c r="A98" t="s">
         <v>95</v>
       </c>
-      <c r="C98" s="20"/>
+      <c r="C98" s="25"/>
       <c r="D98" t="s">
         <v>456</v>
       </c>
@@ -4623,7 +4623,7 @@
       <c r="A99" t="s">
         <v>96</v>
       </c>
-      <c r="C99" s="20"/>
+      <c r="C99" s="25"/>
       <c r="D99" t="s">
         <v>459</v>
       </c>
@@ -4644,7 +4644,7 @@
       <c r="A100" t="s">
         <v>97</v>
       </c>
-      <c r="C100" s="20"/>
+      <c r="C100" s="25"/>
       <c r="D100" t="s">
         <v>460</v>
       </c>
@@ -4665,7 +4665,7 @@
       <c r="A101" t="s">
         <v>98</v>
       </c>
-      <c r="C101" s="20"/>
+      <c r="C101" s="25"/>
       <c r="D101" t="s">
         <v>461</v>
       </c>
@@ -4686,7 +4686,7 @@
       <c r="A102" t="s">
         <v>99</v>
       </c>
-      <c r="C102" s="20"/>
+      <c r="C102" s="25"/>
       <c r="D102" t="s">
         <v>465</v>
       </c>
@@ -4707,7 +4707,7 @@
       <c r="A103" t="s">
         <v>100</v>
       </c>
-      <c r="C103" s="20"/>
+      <c r="C103" s="25"/>
       <c r="D103" t="s">
         <v>466</v>
       </c>
@@ -4728,7 +4728,7 @@
       <c r="A104" t="s">
         <v>101</v>
       </c>
-      <c r="C104" s="20"/>
+      <c r="C104" s="25"/>
       <c r="D104" t="s">
         <v>467</v>
       </c>
@@ -4749,7 +4749,7 @@
       <c r="A105" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="20"/>
+      <c r="C105" s="25"/>
       <c r="D105" t="s">
         <v>468</v>
       </c>
@@ -4770,7 +4770,7 @@
       <c r="A106" t="s">
         <v>103</v>
       </c>
-      <c r="C106" s="20"/>
+      <c r="C106" s="25"/>
       <c r="E106" t="s">
         <v>357</v>
       </c>
@@ -4782,7 +4782,7 @@
       <c r="A107" t="s">
         <v>104</v>
       </c>
-      <c r="C107" s="20"/>
+      <c r="C107" s="25"/>
       <c r="E107" t="s">
         <v>357</v>
       </c>
@@ -4794,7 +4794,7 @@
       <c r="A108" t="s">
         <v>105</v>
       </c>
-      <c r="C108" s="20"/>
+      <c r="C108" s="25"/>
       <c r="D108" t="s">
         <v>472</v>
       </c>
@@ -4815,7 +4815,7 @@
       <c r="A109" t="s">
         <v>106</v>
       </c>
-      <c r="C109" s="20"/>
+      <c r="C109" s="25"/>
       <c r="E109" t="s">
         <v>357</v>
       </c>
@@ -4827,7 +4827,7 @@
       <c r="A110" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C110" s="21"/>
+      <c r="C110" s="26"/>
       <c r="E110" s="6" t="s">
         <v>364</v>
       </c>
@@ -4853,7 +4853,7 @@
       <c r="A112" t="s">
         <v>109</v>
       </c>
-      <c r="C112" s="19" t="s">
+      <c r="C112" s="24" t="s">
         <v>548</v>
       </c>
       <c r="D112" t="s">
@@ -4873,7 +4873,7 @@
       <c r="A113" t="s">
         <v>110</v>
       </c>
-      <c r="C113" s="20"/>
+      <c r="C113" s="25"/>
       <c r="D113" t="s">
         <v>477</v>
       </c>
@@ -4891,7 +4891,7 @@
       <c r="A114" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="20"/>
+      <c r="C114" s="25"/>
       <c r="D114" t="s">
         <v>478</v>
       </c>
@@ -4909,7 +4909,7 @@
       <c r="A115" t="s">
         <v>112</v>
       </c>
-      <c r="C115" s="20"/>
+      <c r="C115" s="25"/>
       <c r="D115" t="s">
         <v>479</v>
       </c>
@@ -4927,7 +4927,7 @@
       <c r="A116" t="s">
         <v>113</v>
       </c>
-      <c r="C116" s="20"/>
+      <c r="C116" s="25"/>
       <c r="D116" t="s">
         <v>480</v>
       </c>
@@ -4948,7 +4948,7 @@
       <c r="A117" t="s">
         <v>114</v>
       </c>
-      <c r="C117" s="20"/>
+      <c r="C117" s="25"/>
       <c r="D117" t="s">
         <v>481</v>
       </c>
@@ -4969,7 +4969,7 @@
       <c r="A118" t="s">
         <v>115</v>
       </c>
-      <c r="C118" s="20"/>
+      <c r="C118" s="25"/>
       <c r="D118" t="s">
         <v>488</v>
       </c>
@@ -4990,7 +4990,7 @@
       <c r="A119" t="s">
         <v>116</v>
       </c>
-      <c r="C119" s="20"/>
+      <c r="C119" s="25"/>
       <c r="D119" t="s">
         <v>442</v>
       </c>
@@ -5011,7 +5011,7 @@
       <c r="A120" t="s">
         <v>117</v>
       </c>
-      <c r="C120" s="20"/>
+      <c r="C120" s="25"/>
       <c r="D120" t="s">
         <v>483</v>
       </c>
@@ -5032,7 +5032,7 @@
       <c r="A121" t="s">
         <v>118</v>
       </c>
-      <c r="C121" s="20"/>
+      <c r="C121" s="25"/>
       <c r="D121" t="s">
         <v>487</v>
       </c>
@@ -5053,7 +5053,7 @@
       <c r="A122" t="s">
         <v>119</v>
       </c>
-      <c r="C122" s="20"/>
+      <c r="C122" s="25"/>
       <c r="D122" t="s">
         <v>484</v>
       </c>
@@ -5074,7 +5074,7 @@
       <c r="A123" t="s">
         <v>120</v>
       </c>
-      <c r="C123" s="20"/>
+      <c r="C123" s="25"/>
       <c r="D123" t="s">
         <v>485</v>
       </c>
@@ -5095,7 +5095,7 @@
       <c r="A124" t="s">
         <v>121</v>
       </c>
-      <c r="C124" s="20"/>
+      <c r="C124" s="25"/>
       <c r="D124" t="s">
         <v>486</v>
       </c>
@@ -5116,7 +5116,7 @@
       <c r="A125" t="s">
         <v>122</v>
       </c>
-      <c r="C125" s="20"/>
+      <c r="C125" s="25"/>
       <c r="D125" t="s">
         <v>482</v>
       </c>
@@ -5137,7 +5137,7 @@
       <c r="A126" t="s">
         <v>123</v>
       </c>
-      <c r="C126" s="20"/>
+      <c r="C126" s="25"/>
       <c r="E126" t="s">
         <v>357</v>
       </c>
@@ -5149,7 +5149,7 @@
       <c r="A127" t="s">
         <v>124</v>
       </c>
-      <c r="C127" s="20"/>
+      <c r="C127" s="25"/>
       <c r="E127" t="s">
         <v>357</v>
       </c>
@@ -5161,7 +5161,7 @@
       <c r="A128" t="s">
         <v>125</v>
       </c>
-      <c r="C128" s="20"/>
+      <c r="C128" s="25"/>
       <c r="D128" t="s">
         <v>491</v>
       </c>
@@ -5182,7 +5182,7 @@
       <c r="A129" t="s">
         <v>126</v>
       </c>
-      <c r="C129" s="20"/>
+      <c r="C129" s="25"/>
       <c r="E129" t="s">
         <v>357</v>
       </c>
@@ -5194,7 +5194,7 @@
       <c r="A130" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C130" s="21"/>
+      <c r="C130" s="26"/>
       <c r="E130" s="6" t="s">
         <v>364</v>
       </c>
@@ -5206,7 +5206,7 @@
       <c r="A131" t="s">
         <v>128</v>
       </c>
-      <c r="C131" s="19" t="s">
+      <c r="C131" s="24" t="s">
         <v>549</v>
       </c>
       <c r="E131" t="s">
@@ -5220,7 +5220,7 @@
       <c r="A132" t="s">
         <v>129</v>
       </c>
-      <c r="C132" s="20"/>
+      <c r="C132" s="25"/>
       <c r="E132" t="s">
         <v>357</v>
       </c>
@@ -5232,7 +5232,7 @@
       <c r="A133" t="s">
         <v>130</v>
       </c>
-      <c r="C133" s="20"/>
+      <c r="C133" s="25"/>
       <c r="E133" t="s">
         <v>357</v>
       </c>
@@ -5244,7 +5244,7 @@
       <c r="A134" t="s">
         <v>131</v>
       </c>
-      <c r="C134" s="20"/>
+      <c r="C134" s="25"/>
       <c r="E134" t="s">
         <v>357</v>
       </c>
@@ -5256,7 +5256,7 @@
       <c r="A135" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C135" s="22"/>
+      <c r="C135" s="28"/>
       <c r="E135" s="12" t="s">
         <v>364</v>
       </c>
@@ -5268,7 +5268,7 @@
       <c r="A136" t="s">
         <v>133</v>
       </c>
-      <c r="C136" s="20" t="s">
+      <c r="C136" s="25" t="s">
         <v>550</v>
       </c>
       <c r="D136" t="s">
@@ -5291,7 +5291,7 @@
       <c r="A137" t="s">
         <v>134</v>
       </c>
-      <c r="C137" s="20"/>
+      <c r="C137" s="25"/>
       <c r="D137" t="s">
         <v>501</v>
       </c>
@@ -5312,7 +5312,7 @@
       <c r="A138" t="s">
         <v>135</v>
       </c>
-      <c r="C138" s="20"/>
+      <c r="C138" s="25"/>
       <c r="E138" t="s">
         <v>497</v>
       </c>
@@ -5327,7 +5327,7 @@
       <c r="A139" t="s">
         <v>136</v>
       </c>
-      <c r="C139" s="20"/>
+      <c r="C139" s="25"/>
       <c r="D139" t="s">
         <v>502</v>
       </c>
@@ -5348,7 +5348,7 @@
       <c r="A140" t="s">
         <v>637</v>
       </c>
-      <c r="C140" s="20"/>
+      <c r="C140" s="25"/>
       <c r="E140" t="s">
         <v>623</v>
       </c>
@@ -5366,7 +5366,7 @@
       <c r="A141" t="s">
         <v>638</v>
       </c>
-      <c r="C141" s="20"/>
+      <c r="C141" s="25"/>
       <c r="E141" t="s">
         <v>623</v>
       </c>
@@ -5384,7 +5384,7 @@
       <c r="A142" t="s">
         <v>639</v>
       </c>
-      <c r="C142" s="20"/>
+      <c r="C142" s="25"/>
       <c r="E142" t="s">
         <v>629</v>
       </c>
@@ -5402,7 +5402,7 @@
       <c r="A143" t="s">
         <v>640</v>
       </c>
-      <c r="C143" s="20"/>
+      <c r="C143" s="25"/>
       <c r="E143" t="s">
         <v>629</v>
       </c>
@@ -5420,7 +5420,7 @@
       <c r="A144" t="s">
         <v>641</v>
       </c>
-      <c r="C144" s="20"/>
+      <c r="C144" s="25"/>
       <c r="E144" t="s">
         <v>629</v>
       </c>
@@ -5438,7 +5438,7 @@
       <c r="A145" t="s">
         <v>642</v>
       </c>
-      <c r="C145" s="20"/>
+      <c r="C145" s="25"/>
       <c r="D145" t="s">
         <v>656</v>
       </c>
@@ -5462,7 +5462,7 @@
       <c r="A146" t="s">
         <v>137</v>
       </c>
-      <c r="C146" s="20"/>
+      <c r="C146" s="25"/>
       <c r="D146" t="s">
         <v>503</v>
       </c>
@@ -5483,7 +5483,7 @@
       <c r="A147" t="s">
         <v>138</v>
       </c>
-      <c r="C147" s="20"/>
+      <c r="C147" s="25"/>
       <c r="E147" t="s">
         <v>357</v>
       </c>
@@ -5495,7 +5495,7 @@
       <c r="A148" t="s">
         <v>139</v>
       </c>
-      <c r="C148" s="20"/>
+      <c r="C148" s="25"/>
       <c r="E148" t="s">
         <v>357</v>
       </c>
@@ -5507,7 +5507,7 @@
       <c r="A149" t="s">
         <v>140</v>
       </c>
-      <c r="C149" s="20"/>
+      <c r="C149" s="25"/>
       <c r="D149" t="s">
         <v>504</v>
       </c>
@@ -5528,7 +5528,7 @@
       <c r="A150" t="s">
         <v>141</v>
       </c>
-      <c r="C150" s="20"/>
+      <c r="C150" s="25"/>
       <c r="E150" t="s">
         <v>357</v>
       </c>
@@ -5540,7 +5540,7 @@
       <c r="A151" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C151" s="21"/>
+      <c r="C151" s="26"/>
       <c r="E151" s="6" t="s">
         <v>364</v>
       </c>
@@ -5566,7 +5566,7 @@
       <c r="A153" t="s">
         <v>144</v>
       </c>
-      <c r="C153" s="19" t="s">
+      <c r="C153" s="24" t="s">
         <v>551</v>
       </c>
       <c r="E153" t="s">
@@ -5580,7 +5580,7 @@
       <c r="A154" t="s">
         <v>145</v>
       </c>
-      <c r="C154" s="20"/>
+      <c r="C154" s="25"/>
       <c r="E154" t="s">
         <v>357</v>
       </c>
@@ -5592,7 +5592,7 @@
       <c r="A155" t="s">
         <v>146</v>
       </c>
-      <c r="C155" s="20"/>
+      <c r="C155" s="25"/>
       <c r="E155" t="s">
         <v>357</v>
       </c>
@@ -5604,7 +5604,7 @@
       <c r="A156" t="s">
         <v>147</v>
       </c>
-      <c r="C156" s="20"/>
+      <c r="C156" s="25"/>
       <c r="E156" t="s">
         <v>357</v>
       </c>
@@ -5616,7 +5616,7 @@
       <c r="A157" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C157" s="21"/>
+      <c r="C157" s="26"/>
       <c r="E157" s="6" t="s">
         <v>364</v>
       </c>
@@ -5628,7 +5628,7 @@
       <c r="A158" t="s">
         <v>149</v>
       </c>
-      <c r="C158" s="19" t="s">
+      <c r="C158" s="24" t="s">
         <v>552</v>
       </c>
       <c r="E158" t="s">
@@ -5642,7 +5642,7 @@
       <c r="A159" t="s">
         <v>150</v>
       </c>
-      <c r="C159" s="20"/>
+      <c r="C159" s="25"/>
       <c r="E159" t="s">
         <v>357</v>
       </c>
@@ -5654,7 +5654,7 @@
       <c r="A160" t="s">
         <v>151</v>
       </c>
-      <c r="C160" s="20"/>
+      <c r="C160" s="25"/>
       <c r="E160" t="s">
         <v>357</v>
       </c>
@@ -5669,7 +5669,7 @@
       <c r="A161" t="s">
         <v>152</v>
       </c>
-      <c r="C161" s="20"/>
+      <c r="C161" s="25"/>
       <c r="E161" t="s">
         <v>357</v>
       </c>
@@ -5684,7 +5684,7 @@
       <c r="A162" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C162" s="21"/>
+      <c r="C162" s="26"/>
       <c r="E162" s="6" t="s">
         <v>364</v>
       </c>
@@ -5696,7 +5696,7 @@
       <c r="A163" t="s">
         <v>154</v>
       </c>
-      <c r="C163" s="19" t="s">
+      <c r="C163" s="24" t="s">
         <v>553</v>
       </c>
       <c r="D163" t="s">
@@ -5719,7 +5719,7 @@
       <c r="A164" t="s">
         <v>155</v>
       </c>
-      <c r="C164" s="20"/>
+      <c r="C164" s="25"/>
       <c r="E164" t="s">
         <v>357</v>
       </c>
@@ -5731,26 +5731,26 @@
       <c r="A165" t="s">
         <v>156</v>
       </c>
-      <c r="C165" s="20"/>
+      <c r="C165" s="25"/>
       <c r="E165" t="s">
         <v>357</v>
       </c>
       <c r="F165" t="s">
         <v>522</v>
       </c>
-      <c r="I165" s="18" t="s">
+      <c r="I165" s="27" t="s">
         <v>601</v>
       </c>
-      <c r="J165" s="18"/>
-      <c r="K165" s="18"/>
-      <c r="L165" s="18"/>
-      <c r="M165" s="18"/>
+      <c r="J165" s="27"/>
+      <c r="K165" s="27"/>
+      <c r="L165" s="27"/>
+      <c r="M165" s="27"/>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
         <v>157</v>
       </c>
-      <c r="C166" s="20"/>
+      <c r="C166" s="25"/>
       <c r="D166" t="s">
         <v>511</v>
       </c>
@@ -5766,51 +5766,51 @@
       <c r="H166" t="s">
         <v>634</v>
       </c>
-      <c r="I166" s="18"/>
-      <c r="J166" s="18"/>
-      <c r="K166" s="18"/>
-      <c r="L166" s="18"/>
-      <c r="M166" s="18"/>
+      <c r="I166" s="27"/>
+      <c r="J166" s="27"/>
+      <c r="K166" s="27"/>
+      <c r="L166" s="27"/>
+      <c r="M166" s="27"/>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="s">
         <v>158</v>
       </c>
-      <c r="C167" s="20"/>
+      <c r="C167" s="25"/>
       <c r="E167" t="s">
         <v>357</v>
       </c>
       <c r="F167" t="s">
         <v>492</v>
       </c>
-      <c r="I167" s="18"/>
-      <c r="J167" s="18"/>
-      <c r="K167" s="18"/>
-      <c r="L167" s="18"/>
-      <c r="M167" s="18"/>
+      <c r="I167" s="27"/>
+      <c r="J167" s="27"/>
+      <c r="K167" s="27"/>
+      <c r="L167" s="27"/>
+      <c r="M167" s="27"/>
     </row>
     <row r="168" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C168" s="21"/>
+      <c r="C168" s="26"/>
       <c r="E168" s="6" t="s">
         <v>364</v>
       </c>
       <c r="F168" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="I168" s="18"/>
-      <c r="J168" s="18"/>
-      <c r="K168" s="18"/>
-      <c r="L168" s="18"/>
-      <c r="M168" s="18"/>
+      <c r="I168" s="27"/>
+      <c r="J168" s="27"/>
+      <c r="K168" s="27"/>
+      <c r="L168" s="27"/>
+      <c r="M168" s="27"/>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
         <v>160</v>
       </c>
-      <c r="C169" s="19" t="s">
+      <c r="C169" s="24" t="s">
         <v>555</v>
       </c>
       <c r="E169" t="s">
@@ -5827,7 +5827,7 @@
       <c r="A170" t="s">
         <v>161</v>
       </c>
-      <c r="C170" s="20"/>
+      <c r="C170" s="25"/>
       <c r="D170" t="s">
         <v>520</v>
       </c>
@@ -5848,7 +5848,7 @@
       <c r="A171" t="s">
         <v>620</v>
       </c>
-      <c r="C171" s="20"/>
+      <c r="C171" s="25"/>
       <c r="E171" t="s">
         <v>623</v>
       </c>
@@ -5866,7 +5866,7 @@
       <c r="A172" t="s">
         <v>621</v>
       </c>
-      <c r="C172" s="20"/>
+      <c r="C172" s="25"/>
       <c r="E172" t="s">
         <v>623</v>
       </c>
@@ -5884,7 +5884,7 @@
       <c r="A173" t="s">
         <v>625</v>
       </c>
-      <c r="C173" s="20"/>
+      <c r="C173" s="25"/>
       <c r="E173" t="s">
         <v>629</v>
       </c>
@@ -5902,7 +5902,7 @@
       <c r="A174" t="s">
         <v>626</v>
       </c>
-      <c r="C174" s="20"/>
+      <c r="C174" s="25"/>
       <c r="E174" t="s">
         <v>629</v>
       </c>
@@ -5920,7 +5920,7 @@
       <c r="A175" t="s">
         <v>627</v>
       </c>
-      <c r="C175" s="20"/>
+      <c r="C175" s="25"/>
       <c r="E175" t="s">
         <v>629</v>
       </c>
@@ -5938,7 +5938,7 @@
       <c r="A176" t="s">
         <v>628</v>
       </c>
-      <c r="C176" s="20"/>
+      <c r="C176" s="25"/>
       <c r="D176" t="s">
         <v>657</v>
       </c>
@@ -5962,7 +5962,7 @@
       <c r="A177" t="s">
         <v>162</v>
       </c>
-      <c r="C177" s="20"/>
+      <c r="C177" s="25"/>
       <c r="D177" t="s">
         <v>521</v>
       </c>
@@ -5983,7 +5983,7 @@
       <c r="A178" t="s">
         <v>163</v>
       </c>
-      <c r="C178" s="20"/>
+      <c r="C178" s="25"/>
       <c r="E178" t="s">
         <v>357</v>
       </c>
@@ -5995,7 +5995,7 @@
       <c r="A179" t="s">
         <v>164</v>
       </c>
-      <c r="C179" s="20"/>
+      <c r="C179" s="25"/>
       <c r="E179" t="s">
         <v>357</v>
       </c>
@@ -6007,7 +6007,7 @@
       <c r="A180" t="s">
         <v>165</v>
       </c>
-      <c r="C180" s="20"/>
+      <c r="C180" s="25"/>
       <c r="E180" t="s">
         <v>357</v>
       </c>
@@ -6019,7 +6019,7 @@
       <c r="A181" t="s">
         <v>166</v>
       </c>
-      <c r="C181" s="20"/>
+      <c r="C181" s="25"/>
       <c r="E181" t="s">
         <v>357</v>
       </c>
@@ -6031,7 +6031,7 @@
       <c r="A182" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C182" s="21"/>
+      <c r="C182" s="26"/>
       <c r="E182" s="6" t="s">
         <v>364</v>
       </c>
@@ -6043,7 +6043,7 @@
       <c r="A183" t="s">
         <v>168</v>
       </c>
-      <c r="C183" s="19" t="s">
+      <c r="C183" s="24" t="s">
         <v>556</v>
       </c>
       <c r="E183" t="s">
@@ -6057,7 +6057,7 @@
       <c r="A184" t="s">
         <v>169</v>
       </c>
-      <c r="C184" s="20"/>
+      <c r="C184" s="25"/>
       <c r="E184" t="s">
         <v>357</v>
       </c>
@@ -6069,7 +6069,7 @@
       <c r="A185" t="s">
         <v>170</v>
       </c>
-      <c r="C185" s="20"/>
+      <c r="C185" s="25"/>
       <c r="D185" t="s">
         <v>524</v>
       </c>
@@ -6090,7 +6090,7 @@
       <c r="A186" t="s">
         <v>171</v>
       </c>
-      <c r="C186" s="20"/>
+      <c r="C186" s="25"/>
       <c r="E186" t="s">
         <v>357</v>
       </c>
@@ -6102,7 +6102,7 @@
       <c r="A187" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C187" s="21"/>
+      <c r="C187" s="26"/>
       <c r="E187" s="6" t="s">
         <v>364</v>
       </c>
@@ -6114,7 +6114,7 @@
       <c r="A188" t="s">
         <v>173</v>
       </c>
-      <c r="C188" s="19" t="s">
+      <c r="C188" s="24" t="s">
         <v>557</v>
       </c>
       <c r="E188" t="s">
@@ -6128,7 +6128,7 @@
       <c r="A189" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C189" s="21"/>
+      <c r="C189" s="26"/>
       <c r="D189" s="6" t="s">
         <v>530</v>
       </c>
@@ -6149,7 +6149,7 @@
       <c r="A190" t="s">
         <v>175</v>
       </c>
-      <c r="C190" s="19" t="s">
+      <c r="C190" s="24" t="s">
         <v>558</v>
       </c>
       <c r="E190" t="s">
@@ -6163,7 +6163,7 @@
       <c r="A191" t="s">
         <v>176</v>
       </c>
-      <c r="C191" s="20"/>
+      <c r="C191" s="25"/>
       <c r="E191" t="s">
         <v>357</v>
       </c>
@@ -6175,7 +6175,7 @@
       <c r="A192" t="s">
         <v>177</v>
       </c>
-      <c r="C192" s="20"/>
+      <c r="C192" s="25"/>
       <c r="E192" t="s">
         <v>357</v>
       </c>
@@ -6187,7 +6187,7 @@
       <c r="A193" t="s">
         <v>178</v>
       </c>
-      <c r="C193" s="20"/>
+      <c r="C193" s="25"/>
       <c r="E193" t="s">
         <v>357</v>
       </c>
@@ -6199,7 +6199,7 @@
       <c r="A194" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C194" s="21"/>
+      <c r="C194" s="26"/>
       <c r="E194" s="6" t="s">
         <v>364</v>
       </c>
@@ -6211,7 +6211,7 @@
       <c r="A195" t="s">
         <v>180</v>
       </c>
-      <c r="C195" s="19" t="s">
+      <c r="C195" s="24" t="s">
         <v>559</v>
       </c>
       <c r="E195" t="s">
@@ -6225,7 +6225,7 @@
       <c r="A196" t="s">
         <v>181</v>
       </c>
-      <c r="C196" s="20"/>
+      <c r="C196" s="25"/>
       <c r="E196" t="s">
         <v>357</v>
       </c>
@@ -6237,7 +6237,7 @@
       <c r="A197" t="s">
         <v>182</v>
       </c>
-      <c r="C197" s="20"/>
+      <c r="C197" s="25"/>
       <c r="D197" t="s">
         <v>596</v>
       </c>
@@ -6258,7 +6258,7 @@
       <c r="A198" t="s">
         <v>183</v>
       </c>
-      <c r="C198" s="20"/>
+      <c r="C198" s="25"/>
       <c r="E198" t="s">
         <v>357</v>
       </c>
@@ -6270,7 +6270,7 @@
       <c r="A199" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C199" s="21"/>
+      <c r="C199" s="26"/>
       <c r="E199" s="6" t="s">
         <v>364</v>
       </c>
@@ -6282,7 +6282,7 @@
       <c r="A200" t="s">
         <v>185</v>
       </c>
-      <c r="C200" s="19" t="s">
+      <c r="C200" s="24" t="s">
         <v>560</v>
       </c>
       <c r="E200" t="s">
@@ -6296,7 +6296,7 @@
       <c r="A201" t="s">
         <v>186</v>
       </c>
-      <c r="C201" s="20"/>
+      <c r="C201" s="25"/>
       <c r="E201" t="s">
         <v>357</v>
       </c>
@@ -6308,7 +6308,7 @@
       <c r="A202" t="s">
         <v>187</v>
       </c>
-      <c r="C202" s="20"/>
+      <c r="C202" s="25"/>
       <c r="D202" t="s">
         <v>595</v>
       </c>
@@ -6329,7 +6329,7 @@
       <c r="A203" t="s">
         <v>188</v>
       </c>
-      <c r="C203" s="20"/>
+      <c r="C203" s="25"/>
       <c r="E203" t="s">
         <v>357</v>
       </c>
@@ -6341,7 +6341,7 @@
       <c r="A204" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C204" s="21"/>
+      <c r="C204" s="26"/>
       <c r="E204" s="6" t="s">
         <v>364</v>
       </c>
@@ -6353,7 +6353,7 @@
       <c r="A205" t="s">
         <v>190</v>
       </c>
-      <c r="C205" s="19" t="s">
+      <c r="C205" s="24" t="s">
         <v>563</v>
       </c>
       <c r="E205" t="s">
@@ -6367,7 +6367,7 @@
       <c r="A206" t="s">
         <v>191</v>
       </c>
-      <c r="C206" s="20"/>
+      <c r="C206" s="25"/>
       <c r="E206" t="s">
         <v>357</v>
       </c>
@@ -6379,7 +6379,7 @@
       <c r="A207" t="s">
         <v>192</v>
       </c>
-      <c r="C207" s="20"/>
+      <c r="C207" s="25"/>
       <c r="D207" t="s">
         <v>600</v>
       </c>
@@ -6400,7 +6400,7 @@
       <c r="A208" t="s">
         <v>193</v>
       </c>
-      <c r="C208" s="20"/>
+      <c r="C208" s="25"/>
       <c r="E208" t="s">
         <v>357</v>
       </c>
@@ -6412,7 +6412,7 @@
       <c r="A209" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C209" s="21"/>
+      <c r="C209" s="26"/>
       <c r="E209" s="6" t="s">
         <v>364</v>
       </c>
@@ -6424,7 +6424,7 @@
       <c r="A210" t="s">
         <v>195</v>
       </c>
-      <c r="C210" s="19" t="s">
+      <c r="C210" s="24" t="s">
         <v>561</v>
       </c>
       <c r="D210" t="s">
@@ -6450,7 +6450,7 @@
       <c r="A211" t="s">
         <v>196</v>
       </c>
-      <c r="C211" s="20"/>
+      <c r="C211" s="25"/>
       <c r="D211" t="s">
         <v>609</v>
       </c>
@@ -6471,7 +6471,7 @@
       <c r="A212" t="s">
         <v>197</v>
       </c>
-      <c r="C212" s="20"/>
+      <c r="C212" s="25"/>
       <c r="D212" t="s">
         <v>610</v>
       </c>
@@ -6489,7 +6489,7 @@
       <c r="A213" t="s">
         <v>198</v>
       </c>
-      <c r="C213" s="20"/>
+      <c r="C213" s="25"/>
       <c r="D213" t="s">
         <v>611</v>
       </c>
@@ -6510,7 +6510,7 @@
       <c r="A214" t="s">
         <v>643</v>
       </c>
-      <c r="C214" s="20"/>
+      <c r="C214" s="25"/>
       <c r="E214" t="s">
         <v>623</v>
       </c>
@@ -6525,7 +6525,7 @@
       <c r="A215" t="s">
         <v>644</v>
       </c>
-      <c r="C215" s="20"/>
+      <c r="C215" s="25"/>
       <c r="E215" t="s">
         <v>623</v>
       </c>
@@ -6540,7 +6540,7 @@
       <c r="A216" t="s">
         <v>645</v>
       </c>
-      <c r="C216" s="20"/>
+      <c r="C216" s="25"/>
       <c r="E216" t="s">
         <v>629</v>
       </c>
@@ -6555,7 +6555,7 @@
       <c r="A217" t="s">
         <v>646</v>
       </c>
-      <c r="C217" s="20"/>
+      <c r="C217" s="25"/>
       <c r="E217" t="s">
         <v>629</v>
       </c>
@@ -6570,7 +6570,7 @@
       <c r="A218" t="s">
         <v>647</v>
       </c>
-      <c r="C218" s="20"/>
+      <c r="C218" s="25"/>
       <c r="E218" t="s">
         <v>629</v>
       </c>
@@ -6585,7 +6585,7 @@
       <c r="A219" t="s">
         <v>648</v>
       </c>
-      <c r="C219" s="20"/>
+      <c r="C219" s="25"/>
       <c r="D219" t="s">
         <v>658</v>
       </c>
@@ -6606,7 +6606,7 @@
       <c r="A220" t="s">
         <v>199</v>
       </c>
-      <c r="C220" s="20"/>
+      <c r="C220" s="25"/>
       <c r="E220" t="s">
         <v>612</v>
       </c>
@@ -6618,7 +6618,7 @@
       <c r="A221" t="s">
         <v>200</v>
       </c>
-      <c r="C221" s="20"/>
+      <c r="C221" s="25"/>
       <c r="D221" t="s">
         <v>614</v>
       </c>
@@ -6636,7 +6636,7 @@
       <c r="A222" t="s">
         <v>201</v>
       </c>
-      <c r="C222" s="20"/>
+      <c r="C222" s="25"/>
       <c r="E222" t="s">
         <v>357</v>
       </c>
@@ -6648,7 +6648,7 @@
       <c r="A223" t="s">
         <v>202</v>
       </c>
-      <c r="C223" s="20"/>
+      <c r="C223" s="25"/>
       <c r="D223" t="s">
         <v>665</v>
       </c>
@@ -6672,7 +6672,7 @@
       <c r="A224" t="s">
         <v>203</v>
       </c>
-      <c r="C224" s="20"/>
+      <c r="C224" s="25"/>
       <c r="E224" t="s">
         <v>357</v>
       </c>
@@ -6684,7 +6684,7 @@
       <c r="A225" t="s">
         <v>204</v>
       </c>
-      <c r="C225" s="20"/>
+      <c r="C225" s="25"/>
       <c r="E225" t="s">
         <v>357</v>
       </c>
@@ -6696,7 +6696,7 @@
       <c r="A226" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C226" s="21"/>
+      <c r="C226" s="26"/>
       <c r="E226" s="6" t="s">
         <v>364</v>
       </c>
@@ -6708,7 +6708,7 @@
       <c r="A227" t="s">
         <v>206</v>
       </c>
-      <c r="C227" s="19" t="s">
+      <c r="C227" s="24" t="s">
         <v>562</v>
       </c>
       <c r="E227" t="s">
@@ -6722,7 +6722,7 @@
       <c r="A228" t="s">
         <v>207</v>
       </c>
-      <c r="C228" s="20"/>
+      <c r="C228" s="25"/>
       <c r="D228" t="s">
         <v>617</v>
       </c>
@@ -6740,7 +6740,7 @@
       <c r="A229" t="s">
         <v>650</v>
       </c>
-      <c r="C229" s="20"/>
+      <c r="C229" s="25"/>
       <c r="E229" t="s">
         <v>623</v>
       </c>
@@ -6755,7 +6755,7 @@
       <c r="A230" t="s">
         <v>651</v>
       </c>
-      <c r="C230" s="20"/>
+      <c r="C230" s="25"/>
       <c r="E230" t="s">
         <v>623</v>
       </c>
@@ -6770,7 +6770,7 @@
       <c r="A231" t="s">
         <v>652</v>
       </c>
-      <c r="C231" s="20"/>
+      <c r="C231" s="25"/>
       <c r="E231" t="s">
         <v>629</v>
       </c>
@@ -6785,7 +6785,7 @@
       <c r="A232" t="s">
         <v>653</v>
       </c>
-      <c r="C232" s="20"/>
+      <c r="C232" s="25"/>
       <c r="E232" t="s">
         <v>629</v>
       </c>
@@ -6800,7 +6800,7 @@
       <c r="A233" t="s">
         <v>654</v>
       </c>
-      <c r="C233" s="20"/>
+      <c r="C233" s="25"/>
       <c r="E233" t="s">
         <v>629</v>
       </c>
@@ -6815,7 +6815,7 @@
       <c r="A234" t="s">
         <v>655</v>
       </c>
-      <c r="C234" s="20"/>
+      <c r="C234" s="25"/>
       <c r="D234" t="s">
         <v>659</v>
       </c>
@@ -6836,7 +6836,7 @@
       <c r="A235" t="s">
         <v>208</v>
       </c>
-      <c r="C235" s="20"/>
+      <c r="C235" s="25"/>
       <c r="D235" t="s">
         <v>616</v>
       </c>
@@ -6854,7 +6854,7 @@
       <c r="A236" t="s">
         <v>209</v>
       </c>
-      <c r="C236" s="20"/>
+      <c r="C236" s="25"/>
       <c r="E236" t="s">
         <v>357</v>
       </c>
@@ -6866,7 +6866,7 @@
       <c r="A237" t="s">
         <v>210</v>
       </c>
-      <c r="C237" s="20"/>
+      <c r="C237" s="25"/>
       <c r="E237" t="s">
         <v>357</v>
       </c>
@@ -6878,7 +6878,7 @@
       <c r="A238" t="s">
         <v>211</v>
       </c>
-      <c r="C238" s="20"/>
+      <c r="C238" s="25"/>
       <c r="D238" t="s">
         <v>664</v>
       </c>
@@ -6899,7 +6899,7 @@
       <c r="A239" t="s">
         <v>212</v>
       </c>
-      <c r="C239" s="20"/>
+      <c r="C239" s="25"/>
       <c r="E239" t="s">
         <v>357</v>
       </c>
@@ -6911,7 +6911,7 @@
       <c r="A240" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="C240" s="21"/>
+      <c r="C240" s="26"/>
       <c r="E240" s="6" t="s">
         <v>364</v>
       </c>
@@ -6923,7 +6923,7 @@
       <c r="A241" t="s">
         <v>214</v>
       </c>
-      <c r="C241" s="19" t="s">
+      <c r="C241" s="24" t="s">
         <v>564</v>
       </c>
       <c r="E241" t="s">
@@ -6937,7 +6937,7 @@
       <c r="A242" t="s">
         <v>215</v>
       </c>
-      <c r="C242" s="20"/>
+      <c r="C242" s="25"/>
       <c r="E242" t="s">
         <v>357</v>
       </c>
@@ -6949,7 +6949,7 @@
       <c r="A243" t="s">
         <v>216</v>
       </c>
-      <c r="C243" s="20"/>
+      <c r="C243" s="25"/>
       <c r="D243" t="s">
         <v>669</v>
       </c>
@@ -6970,7 +6970,7 @@
       <c r="A244" t="s">
         <v>217</v>
       </c>
-      <c r="C244" s="20"/>
+      <c r="C244" s="25"/>
       <c r="E244" t="s">
         <v>357</v>
       </c>
@@ -6982,7 +6982,7 @@
       <c r="A245" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C245" s="21"/>
+      <c r="C245" s="26"/>
       <c r="E245" s="6" t="s">
         <v>364</v>
       </c>
@@ -6994,7 +6994,7 @@
       <c r="A246" t="s">
         <v>219</v>
       </c>
-      <c r="C246" s="19" t="s">
+      <c r="C246" s="24" t="s">
         <v>565</v>
       </c>
       <c r="E246" t="s">
@@ -7008,7 +7008,7 @@
       <c r="A247" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C247" s="21"/>
+      <c r="C247" s="26"/>
       <c r="E247" s="6" t="s">
         <v>379</v>
       </c>
@@ -7023,7 +7023,7 @@
       <c r="A248" t="s">
         <v>221</v>
       </c>
-      <c r="C248" s="19" t="s">
+      <c r="C248" s="24" t="s">
         <v>566</v>
       </c>
       <c r="E248" t="s">
@@ -7037,7 +7037,7 @@
       <c r="A249" t="s">
         <v>222</v>
       </c>
-      <c r="C249" s="20"/>
+      <c r="C249" s="25"/>
       <c r="E249" t="s">
         <v>357</v>
       </c>
@@ -7049,7 +7049,7 @@
       <c r="A250" t="s">
         <v>223</v>
       </c>
-      <c r="C250" s="20"/>
+      <c r="C250" s="25"/>
       <c r="E250" t="s">
         <v>357</v>
       </c>
@@ -7061,7 +7061,7 @@
       <c r="A251" t="s">
         <v>224</v>
       </c>
-      <c r="C251" s="20"/>
+      <c r="C251" s="25"/>
       <c r="E251" t="s">
         <v>357</v>
       </c>
@@ -7073,7 +7073,7 @@
       <c r="A252" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="C252" s="22"/>
+      <c r="C252" s="28"/>
       <c r="E252" s="12" t="s">
         <v>364</v>
       </c>
@@ -7085,7 +7085,7 @@
       <c r="A253" t="s">
         <v>226</v>
       </c>
-      <c r="C253" s="20" t="s">
+      <c r="C253" s="25" t="s">
         <v>567</v>
       </c>
       <c r="D253" t="s">
@@ -7105,7 +7105,7 @@
       <c r="A254" t="s">
         <v>227</v>
       </c>
-      <c r="C254" s="20"/>
+      <c r="C254" s="25"/>
       <c r="D254" t="s">
         <v>683</v>
       </c>
@@ -7123,7 +7123,7 @@
       <c r="A255" t="s">
         <v>228</v>
       </c>
-      <c r="C255" s="20"/>
+      <c r="C255" s="25"/>
       <c r="E255" t="s">
         <v>357</v>
       </c>
@@ -7135,7 +7135,7 @@
       <c r="A256" t="s">
         <v>229</v>
       </c>
-      <c r="C256" s="20"/>
+      <c r="C256" s="25"/>
       <c r="D256" t="s">
         <v>682</v>
       </c>
@@ -7156,7 +7156,7 @@
       <c r="A257" t="s">
         <v>230</v>
       </c>
-      <c r="C257" s="20"/>
+      <c r="C257" s="25"/>
       <c r="E257" t="s">
         <v>357</v>
       </c>
@@ -7168,7 +7168,7 @@
       <c r="A258" t="s">
         <v>231</v>
       </c>
-      <c r="C258" s="20"/>
+      <c r="C258" s="25"/>
       <c r="E258" t="s">
         <v>357</v>
       </c>
@@ -7180,7 +7180,7 @@
       <c r="A259" t="s">
         <v>232</v>
       </c>
-      <c r="C259" s="20"/>
+      <c r="C259" s="25"/>
       <c r="E259" t="s">
         <v>364</v>
       </c>
@@ -7192,7 +7192,7 @@
       <c r="A260" t="s">
         <v>233</v>
       </c>
-      <c r="C260" s="20"/>
+      <c r="C260" s="25"/>
       <c r="D260" t="s">
         <v>684</v>
       </c>
@@ -7213,7 +7213,7 @@
       <c r="A261" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C261" s="20"/>
+      <c r="C261" s="25"/>
       <c r="D261" s="6" t="s">
         <v>687</v>
       </c>
@@ -7231,7 +7231,7 @@
       <c r="A262" t="s">
         <v>235</v>
       </c>
-      <c r="C262" s="20" t="s">
+      <c r="C262" s="25" t="s">
         <v>569</v>
       </c>
       <c r="D262" t="s">
@@ -7249,17 +7249,17 @@
       <c r="H262" t="s">
         <v>636</v>
       </c>
-      <c r="I262" s="23" t="s">
+      <c r="I262" s="19" t="s">
         <v>704</v>
       </c>
-      <c r="J262" s="23"/>
-      <c r="K262" s="23"/>
+      <c r="J262" s="19"/>
+      <c r="K262" s="19"/>
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" t="s">
         <v>236</v>
       </c>
-      <c r="C263" s="20"/>
+      <c r="C263" s="25"/>
       <c r="D263" t="s">
         <v>694</v>
       </c>
@@ -7272,15 +7272,15 @@
       <c r="H263" t="s">
         <v>636</v>
       </c>
-      <c r="I263" s="23"/>
-      <c r="J263" s="23"/>
-      <c r="K263" s="23"/>
+      <c r="I263" s="19"/>
+      <c r="J263" s="19"/>
+      <c r="K263" s="19"/>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" t="s">
         <v>237</v>
       </c>
-      <c r="C264" s="20"/>
+      <c r="C264" s="25"/>
       <c r="D264" t="s">
         <v>698</v>
       </c>
@@ -7293,15 +7293,15 @@
       <c r="H264" t="s">
         <v>636</v>
       </c>
-      <c r="I264" s="23"/>
-      <c r="J264" s="23"/>
-      <c r="K264" s="23"/>
+      <c r="I264" s="19"/>
+      <c r="J264" s="19"/>
+      <c r="K264" s="19"/>
     </row>
     <row r="265" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" t="s">
         <v>238</v>
       </c>
-      <c r="C265" s="20"/>
+      <c r="C265" s="25"/>
       <c r="D265" t="s">
         <v>697</v>
       </c>
@@ -7311,15 +7311,15 @@
       <c r="F265" t="s">
         <v>674</v>
       </c>
-      <c r="I265" s="23"/>
-      <c r="J265" s="23"/>
-      <c r="K265" s="23"/>
+      <c r="I265" s="19"/>
+      <c r="J265" s="19"/>
+      <c r="K265" s="19"/>
     </row>
     <row r="266" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" t="s">
         <v>239</v>
       </c>
-      <c r="C266" s="20"/>
+      <c r="C266" s="25"/>
       <c r="E266" t="s">
         <v>357</v>
       </c>
@@ -7337,7 +7337,7 @@
       <c r="A267" t="s">
         <v>240</v>
       </c>
-      <c r="C267" s="20"/>
+      <c r="C267" s="25"/>
       <c r="E267" t="s">
         <v>357</v>
       </c>
@@ -7349,7 +7349,7 @@
       <c r="A268" t="s">
         <v>241</v>
       </c>
-      <c r="C268" s="20"/>
+      <c r="C268" s="25"/>
       <c r="E268" t="s">
         <v>357</v>
       </c>
@@ -7361,7 +7361,7 @@
       <c r="A269" t="s">
         <v>242</v>
       </c>
-      <c r="C269" s="20"/>
+      <c r="C269" s="25"/>
       <c r="E269" t="s">
         <v>364</v>
       </c>
@@ -7373,7 +7373,7 @@
       <c r="A270" t="s">
         <v>243</v>
       </c>
-      <c r="C270" s="20"/>
+      <c r="C270" s="25"/>
       <c r="D270" t="s">
         <v>699</v>
       </c>
@@ -7391,7 +7391,7 @@
       <c r="A271" t="s">
         <v>244</v>
       </c>
-      <c r="C271" s="20"/>
+      <c r="C271" s="25"/>
       <c r="D271" t="s">
         <v>701</v>
       </c>
@@ -7409,7 +7409,7 @@
       <c r="A272" t="s">
         <v>245</v>
       </c>
-      <c r="C272" s="20"/>
+      <c r="C272" s="25"/>
       <c r="D272" t="s">
         <v>695</v>
       </c>
@@ -7427,7 +7427,7 @@
       <c r="A273" t="s">
         <v>246</v>
       </c>
-      <c r="C273" s="20"/>
+      <c r="C273" s="25"/>
       <c r="D273" t="s">
         <v>708</v>
       </c>
@@ -7448,7 +7448,7 @@
       <c r="A274" t="s">
         <v>247</v>
       </c>
-      <c r="C274" s="20"/>
+      <c r="C274" s="25"/>
       <c r="E274" t="s">
         <v>357</v>
       </c>
@@ -7460,7 +7460,7 @@
       <c r="A275" t="s">
         <v>248</v>
       </c>
-      <c r="C275" s="20"/>
+      <c r="C275" s="25"/>
       <c r="D275" t="s">
         <v>696</v>
       </c>
@@ -7481,7 +7481,7 @@
       <c r="A276" t="s">
         <v>249</v>
       </c>
-      <c r="C276" s="20"/>
+      <c r="C276" s="25"/>
       <c r="E276" t="s">
         <v>357</v>
       </c>
@@ -7493,7 +7493,7 @@
       <c r="A277" t="s">
         <v>250</v>
       </c>
-      <c r="C277" s="20"/>
+      <c r="C277" s="25"/>
       <c r="E277" t="s">
         <v>357</v>
       </c>
@@ -7505,7 +7505,7 @@
       <c r="A278" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="C278" s="21"/>
+      <c r="C278" s="26"/>
       <c r="E278" s="6" t="s">
         <v>364</v>
       </c>
@@ -7537,7 +7537,7 @@
       <c r="A280" t="s">
         <v>253</v>
       </c>
-      <c r="C280" s="19" t="s">
+      <c r="C280" s="24" t="s">
         <v>571</v>
       </c>
       <c r="D280" t="s">
@@ -7557,7 +7557,7 @@
       <c r="A281" t="s">
         <v>254</v>
       </c>
-      <c r="C281" s="20"/>
+      <c r="C281" s="25"/>
       <c r="D281" t="s">
         <v>715</v>
       </c>
@@ -7575,7 +7575,7 @@
       <c r="A282" t="s">
         <v>255</v>
       </c>
-      <c r="C282" s="20"/>
+      <c r="C282" s="25"/>
       <c r="E282" t="s">
         <v>357</v>
       </c>
@@ -7587,7 +7587,7 @@
       <c r="A283" t="s">
         <v>256</v>
       </c>
-      <c r="C283" s="20"/>
+      <c r="C283" s="25"/>
       <c r="D283" t="s">
         <v>716</v>
       </c>
@@ -7608,7 +7608,7 @@
       <c r="A284" t="s">
         <v>257</v>
       </c>
-      <c r="C284" s="20"/>
+      <c r="C284" s="25"/>
       <c r="E284" t="s">
         <v>357</v>
       </c>
@@ -7620,7 +7620,7 @@
       <c r="A285" t="s">
         <v>258</v>
       </c>
-      <c r="C285" s="20"/>
+      <c r="C285" s="25"/>
       <c r="E285" t="s">
         <v>357</v>
       </c>
@@ -7632,7 +7632,7 @@
       <c r="A286" t="s">
         <v>259</v>
       </c>
-      <c r="C286" s="20"/>
+      <c r="C286" s="25"/>
       <c r="E286" t="s">
         <v>364</v>
       </c>
@@ -7644,7 +7644,7 @@
       <c r="A287" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C287" s="21"/>
+      <c r="C287" s="26"/>
       <c r="D287" s="6" t="s">
         <v>717</v>
       </c>
@@ -7662,7 +7662,7 @@
       <c r="A288" t="s">
         <v>261</v>
       </c>
-      <c r="C288" s="19" t="s">
+      <c r="C288" s="24" t="s">
         <v>572</v>
       </c>
       <c r="D288" t="s">
@@ -7685,7 +7685,7 @@
       <c r="A289" t="s">
         <v>262</v>
       </c>
-      <c r="C289" s="20"/>
+      <c r="C289" s="25"/>
       <c r="D289" t="s">
         <v>721</v>
       </c>
@@ -7703,7 +7703,7 @@
       <c r="A290" t="s">
         <v>263</v>
       </c>
-      <c r="C290" s="20"/>
+      <c r="C290" s="25"/>
       <c r="D290" t="s">
         <v>722</v>
       </c>
@@ -7721,7 +7721,7 @@
       <c r="A291" t="s">
         <v>264</v>
       </c>
-      <c r="C291" s="20"/>
+      <c r="C291" s="25"/>
       <c r="D291" t="s">
         <v>723</v>
       </c>
@@ -7736,7 +7736,7 @@
       <c r="A292" t="s">
         <v>265</v>
       </c>
-      <c r="C292" s="20"/>
+      <c r="C292" s="25"/>
       <c r="E292" t="s">
         <v>357</v>
       </c>
@@ -7754,7 +7754,7 @@
       <c r="A293" t="s">
         <v>266</v>
       </c>
-      <c r="C293" s="20"/>
+      <c r="C293" s="25"/>
       <c r="E293" t="s">
         <v>357</v>
       </c>
@@ -7766,7 +7766,7 @@
       <c r="A294" t="s">
         <v>267</v>
       </c>
-      <c r="C294" s="20"/>
+      <c r="C294" s="25"/>
       <c r="E294" t="s">
         <v>357</v>
       </c>
@@ -7778,7 +7778,7 @@
       <c r="A295" t="s">
         <v>268</v>
       </c>
-      <c r="C295" s="20"/>
+      <c r="C295" s="25"/>
       <c r="E295" t="s">
         <v>364</v>
       </c>
@@ -7790,7 +7790,7 @@
       <c r="A296" t="s">
         <v>269</v>
       </c>
-      <c r="C296" s="20"/>
+      <c r="C296" s="25"/>
       <c r="D296" t="s">
         <v>724</v>
       </c>
@@ -7808,7 +7808,7 @@
       <c r="A297" t="s">
         <v>270</v>
       </c>
-      <c r="C297" s="20"/>
+      <c r="C297" s="25"/>
       <c r="D297" t="s">
         <v>727</v>
       </c>
@@ -7826,7 +7826,7 @@
       <c r="A298" t="s">
         <v>271</v>
       </c>
-      <c r="C298" s="20"/>
+      <c r="C298" s="25"/>
       <c r="D298" t="s">
         <v>728</v>
       </c>
@@ -7844,7 +7844,7 @@
       <c r="A299" t="s">
         <v>272</v>
       </c>
-      <c r="C299" s="20"/>
+      <c r="C299" s="25"/>
       <c r="E299" t="s">
         <v>357</v>
       </c>
@@ -7856,7 +7856,7 @@
       <c r="A300" t="s">
         <v>273</v>
       </c>
-      <c r="C300" s="20"/>
+      <c r="C300" s="25"/>
       <c r="D300" t="s">
         <v>729</v>
       </c>
@@ -7877,7 +7877,7 @@
       <c r="A301" t="s">
         <v>274</v>
       </c>
-      <c r="C301" s="20"/>
+      <c r="C301" s="25"/>
       <c r="E301" t="s">
         <v>357</v>
       </c>
@@ -7889,7 +7889,7 @@
       <c r="A302" t="s">
         <v>275</v>
       </c>
-      <c r="C302" s="20"/>
+      <c r="C302" s="25"/>
       <c r="E302" t="s">
         <v>357</v>
       </c>
@@ -7901,7 +7901,7 @@
       <c r="A303" t="s">
         <v>276</v>
       </c>
-      <c r="C303" s="20"/>
+      <c r="C303" s="25"/>
       <c r="E303" t="s">
         <v>364</v>
       </c>
@@ -7913,7 +7913,7 @@
       <c r="A304" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C304" s="21"/>
+      <c r="C304" s="26"/>
       <c r="D304" s="6" t="s">
         <v>730</v>
       </c>
@@ -7934,7 +7934,7 @@
       <c r="A305" t="s">
         <v>278</v>
       </c>
-      <c r="C305" s="19" t="s">
+      <c r="C305" s="24" t="s">
         <v>573</v>
       </c>
       <c r="E305" t="s">
@@ -7948,7 +7948,7 @@
       <c r="A306" t="s">
         <v>279</v>
       </c>
-      <c r="C306" s="20"/>
+      <c r="C306" s="25"/>
       <c r="E306" t="s">
         <v>357</v>
       </c>
@@ -7960,7 +7960,7 @@
       <c r="A307" t="s">
         <v>280</v>
       </c>
-      <c r="C307" s="20"/>
+      <c r="C307" s="25"/>
       <c r="E307" t="s">
         <v>357</v>
       </c>
@@ -7972,7 +7972,7 @@
       <c r="A308" t="s">
         <v>281</v>
       </c>
-      <c r="C308" s="20"/>
+      <c r="C308" s="25"/>
       <c r="E308" t="s">
         <v>357</v>
       </c>
@@ -7984,7 +7984,7 @@
       <c r="A309" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="C309" s="22"/>
+      <c r="C309" s="28"/>
       <c r="E309" s="12" t="s">
         <v>364</v>
       </c>
@@ -7996,7 +7996,7 @@
       <c r="A310" t="s">
         <v>283</v>
       </c>
-      <c r="C310" s="20" t="s">
+      <c r="C310" s="25" t="s">
         <v>574</v>
       </c>
       <c r="D310" t="s">
@@ -8016,7 +8016,7 @@
       <c r="A311" t="s">
         <v>284</v>
       </c>
-      <c r="C311" s="20"/>
+      <c r="C311" s="25"/>
       <c r="D311" t="s">
         <v>732</v>
       </c>
@@ -8034,7 +8034,7 @@
       <c r="A312" t="s">
         <v>285</v>
       </c>
-      <c r="C312" s="20"/>
+      <c r="C312" s="25"/>
       <c r="D312" t="s">
         <v>735</v>
       </c>
@@ -8052,7 +8052,7 @@
       <c r="A313" t="s">
         <v>286</v>
       </c>
-      <c r="C313" s="20"/>
+      <c r="C313" s="25"/>
       <c r="D313" t="s">
         <v>736</v>
       </c>
@@ -8070,7 +8070,7 @@
       <c r="A314" t="s">
         <v>287</v>
       </c>
-      <c r="C314" s="20"/>
+      <c r="C314" s="25"/>
       <c r="D314" t="s">
         <v>737</v>
       </c>
@@ -8088,7 +8088,7 @@
       <c r="A315" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C315" s="20"/>
+      <c r="C315" s="25"/>
       <c r="D315" s="6" t="s">
         <v>738</v>
       </c>
@@ -8137,7 +8137,7 @@
       <c r="A318" t="s">
         <v>291</v>
       </c>
-      <c r="C318" s="19" t="s">
+      <c r="C318" s="24" t="s">
         <v>577</v>
       </c>
       <c r="D318" t="s">
@@ -8152,22 +8152,22 @@
       <c r="H318" t="s">
         <v>634</v>
       </c>
-      <c r="I318" s="24" t="s">
+      <c r="I318" s="18" t="s">
         <v>783</v>
       </c>
-      <c r="J318" s="24"/>
-      <c r="K318" s="24"/>
-      <c r="L318" s="24"/>
-      <c r="M318" s="26" t="s">
+      <c r="J318" s="18"/>
+      <c r="K318" s="18"/>
+      <c r="L318" s="18"/>
+      <c r="M318" s="21" t="s">
         <v>785</v>
       </c>
-      <c r="N318" s="26"/>
+      <c r="N318" s="21"/>
     </row>
     <row r="319" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" t="s">
         <v>292</v>
       </c>
-      <c r="C319" s="20"/>
+      <c r="C319" s="25"/>
       <c r="D319" t="s">
         <v>744</v>
       </c>
@@ -8180,18 +8180,18 @@
       <c r="H319" t="s">
         <v>634</v>
       </c>
-      <c r="I319" s="23"/>
-      <c r="J319" s="23"/>
-      <c r="K319" s="23"/>
-      <c r="L319" s="23"/>
-      <c r="M319" s="27"/>
-      <c r="N319" s="27"/>
+      <c r="I319" s="19"/>
+      <c r="J319" s="19"/>
+      <c r="K319" s="19"/>
+      <c r="L319" s="19"/>
+      <c r="M319" s="22"/>
+      <c r="N319" s="22"/>
     </row>
     <row r="320" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" t="s">
         <v>293</v>
       </c>
-      <c r="C320" s="20"/>
+      <c r="C320" s="25"/>
       <c r="D320" t="s">
         <v>751</v>
       </c>
@@ -8207,84 +8207,84 @@
       <c r="H320" t="s">
         <v>634</v>
       </c>
-      <c r="I320" s="23"/>
-      <c r="J320" s="23"/>
-      <c r="K320" s="23"/>
-      <c r="L320" s="23"/>
-      <c r="M320" s="27"/>
-      <c r="N320" s="27"/>
+      <c r="I320" s="19"/>
+      <c r="J320" s="19"/>
+      <c r="K320" s="19"/>
+      <c r="L320" s="19"/>
+      <c r="M320" s="22"/>
+      <c r="N320" s="22"/>
     </row>
     <row r="321" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" t="s">
         <v>294</v>
       </c>
-      <c r="C321" s="20"/>
+      <c r="C321" s="25"/>
       <c r="E321" t="s">
         <v>357</v>
       </c>
       <c r="F321" t="s">
         <v>749</v>
       </c>
-      <c r="I321" s="23"/>
-      <c r="J321" s="23"/>
-      <c r="K321" s="23"/>
-      <c r="L321" s="23"/>
-      <c r="M321" s="27"/>
-      <c r="N321" s="27"/>
+      <c r="I321" s="19"/>
+      <c r="J321" s="19"/>
+      <c r="K321" s="19"/>
+      <c r="L321" s="19"/>
+      <c r="M321" s="22"/>
+      <c r="N321" s="22"/>
     </row>
     <row r="322" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" t="s">
         <v>295</v>
       </c>
-      <c r="C322" s="20"/>
+      <c r="C322" s="25"/>
       <c r="E322" t="s">
         <v>357</v>
       </c>
       <c r="F322" t="s">
         <v>750</v>
       </c>
-      <c r="I322" s="23"/>
-      <c r="J322" s="23"/>
-      <c r="K322" s="23"/>
-      <c r="L322" s="23"/>
-      <c r="M322" s="27"/>
-      <c r="N322" s="27"/>
+      <c r="I322" s="19"/>
+      <c r="J322" s="19"/>
+      <c r="K322" s="19"/>
+      <c r="L322" s="19"/>
+      <c r="M322" s="22"/>
+      <c r="N322" s="22"/>
     </row>
     <row r="323" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" t="s">
         <v>296</v>
       </c>
-      <c r="C323" s="20"/>
+      <c r="C323" s="25"/>
       <c r="E323" t="s">
         <v>357</v>
       </c>
       <c r="F323" t="s">
         <v>663</v>
       </c>
-      <c r="I323" s="23"/>
-      <c r="J323" s="23"/>
-      <c r="K323" s="23"/>
-      <c r="L323" s="23"/>
-      <c r="M323" s="27"/>
-      <c r="N323" s="27"/>
+      <c r="I323" s="19"/>
+      <c r="J323" s="19"/>
+      <c r="K323" s="19"/>
+      <c r="L323" s="19"/>
+      <c r="M323" s="22"/>
+      <c r="N323" s="22"/>
     </row>
     <row r="324" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="C324" s="21"/>
+      <c r="C324" s="26"/>
       <c r="E324" s="6" t="s">
         <v>364</v>
       </c>
       <c r="F324" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="I324" s="25"/>
-      <c r="J324" s="25"/>
-      <c r="K324" s="25"/>
-      <c r="L324" s="25"/>
-      <c r="M324" s="28"/>
-      <c r="N324" s="28"/>
+      <c r="I324" s="20"/>
+      <c r="J324" s="20"/>
+      <c r="K324" s="20"/>
+      <c r="L324" s="20"/>
+      <c r="M324" s="23"/>
+      <c r="N324" s="23"/>
     </row>
     <row r="325" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" s="17" t="s">
@@ -8310,7 +8310,7 @@
       <c r="A326" t="s">
         <v>582</v>
       </c>
-      <c r="C326" s="19" t="s">
+      <c r="C326" s="24" t="s">
         <v>759</v>
       </c>
       <c r="D326" t="s">
@@ -8325,16 +8325,16 @@
       <c r="H326" t="s">
         <v>634</v>
       </c>
-      <c r="M326" s="26" t="s">
+      <c r="M326" s="21" t="s">
         <v>785</v>
       </c>
-      <c r="N326" s="26"/>
+      <c r="N326" s="21"/>
     </row>
     <row r="327" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" t="s">
         <v>583</v>
       </c>
-      <c r="C327" s="20"/>
+      <c r="C327" s="25"/>
       <c r="D327" t="s">
         <v>763</v>
       </c>
@@ -8347,14 +8347,14 @@
       <c r="H327" t="s">
         <v>634</v>
       </c>
-      <c r="M327" s="27"/>
-      <c r="N327" s="27"/>
+      <c r="M327" s="22"/>
+      <c r="N327" s="22"/>
     </row>
     <row r="328" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" t="s">
         <v>301</v>
       </c>
-      <c r="C328" s="20"/>
+      <c r="C328" s="25"/>
       <c r="D328" t="s">
         <v>764</v>
       </c>
@@ -8367,14 +8367,14 @@
       <c r="H328" t="s">
         <v>634</v>
       </c>
-      <c r="M328" s="27"/>
-      <c r="N328" s="27"/>
+      <c r="M328" s="22"/>
+      <c r="N328" s="22"/>
     </row>
     <row r="329" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" t="s">
         <v>302</v>
       </c>
-      <c r="C329" s="20"/>
+      <c r="C329" s="25"/>
       <c r="D329" t="s">
         <v>765</v>
       </c>
@@ -8387,14 +8387,14 @@
       <c r="H329" t="s">
         <v>634</v>
       </c>
-      <c r="M329" s="27"/>
-      <c r="N329" s="27"/>
+      <c r="M329" s="22"/>
+      <c r="N329" s="22"/>
     </row>
     <row r="330" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" t="s">
         <v>303</v>
       </c>
-      <c r="C330" s="20"/>
+      <c r="C330" s="25"/>
       <c r="D330" t="s">
         <v>766</v>
       </c>
@@ -8407,14 +8407,14 @@
       <c r="H330" t="s">
         <v>634</v>
       </c>
-      <c r="M330" s="27"/>
-      <c r="N330" s="27"/>
+      <c r="M330" s="22"/>
+      <c r="N330" s="22"/>
     </row>
     <row r="331" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" t="s">
         <v>304</v>
       </c>
-      <c r="C331" s="20"/>
+      <c r="C331" s="25"/>
       <c r="D331" t="s">
         <v>767</v>
       </c>
@@ -8427,18 +8427,18 @@
       <c r="H331" t="s">
         <v>634</v>
       </c>
-      <c r="I331" s="18" t="s">
+      <c r="I331" s="27" t="s">
         <v>779</v>
       </c>
-      <c r="J331" s="18"/>
-      <c r="M331" s="27"/>
-      <c r="N331" s="27"/>
+      <c r="J331" s="27"/>
+      <c r="M331" s="22"/>
+      <c r="N331" s="22"/>
     </row>
     <row r="332" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" t="s">
         <v>584</v>
       </c>
-      <c r="C332" s="20"/>
+      <c r="C332" s="25"/>
       <c r="D332" t="s">
         <v>768</v>
       </c>
@@ -8451,16 +8451,16 @@
       <c r="H332" t="s">
         <v>634</v>
       </c>
-      <c r="I332" s="18"/>
-      <c r="J332" s="18"/>
-      <c r="M332" s="28"/>
-      <c r="N332" s="28"/>
+      <c r="I332" s="27"/>
+      <c r="J332" s="27"/>
+      <c r="M332" s="23"/>
+      <c r="N332" s="23"/>
     </row>
     <row r="333" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" s="6" t="s">
         <v>585</v>
       </c>
-      <c r="C333" s="21"/>
+      <c r="C333" s="26"/>
       <c r="D333" s="6" t="s">
         <v>769</v>
       </c>
@@ -8473,14 +8473,14 @@
       <c r="H333" s="6" t="s">
         <v>634</v>
       </c>
-      <c r="I333" s="18"/>
-      <c r="J333" s="18"/>
+      <c r="I333" s="27"/>
+      <c r="J333" s="27"/>
     </row>
     <row r="334" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" t="s">
         <v>752</v>
       </c>
-      <c r="C334" s="19" t="s">
+      <c r="C334" s="24" t="s">
         <v>758</v>
       </c>
       <c r="E334" t="s">
@@ -8489,64 +8489,64 @@
       <c r="F334" t="s">
         <v>674</v>
       </c>
-      <c r="I334" s="18"/>
-      <c r="J334" s="18"/>
+      <c r="I334" s="27"/>
+      <c r="J334" s="27"/>
     </row>
     <row r="335" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" t="s">
         <v>753</v>
       </c>
-      <c r="C335" s="20"/>
+      <c r="C335" s="25"/>
       <c r="E335" t="s">
         <v>357</v>
       </c>
       <c r="F335" t="s">
         <v>675</v>
       </c>
-      <c r="I335" s="18"/>
-      <c r="J335" s="18"/>
+      <c r="I335" s="27"/>
+      <c r="J335" s="27"/>
     </row>
     <row r="336" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" t="s">
         <v>754</v>
       </c>
-      <c r="C336" s="20"/>
+      <c r="C336" s="25"/>
       <c r="E336" t="s">
         <v>357</v>
       </c>
       <c r="F336" t="s">
         <v>778</v>
       </c>
-      <c r="I336" s="18"/>
-      <c r="J336" s="18"/>
+      <c r="I336" s="27"/>
+      <c r="J336" s="27"/>
     </row>
     <row r="337" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" t="s">
         <v>755</v>
       </c>
-      <c r="C337" s="20"/>
+      <c r="C337" s="25"/>
       <c r="E337" t="s">
         <v>357</v>
       </c>
       <c r="F337" t="s">
         <v>663</v>
       </c>
-      <c r="I337" s="18"/>
-      <c r="J337" s="18"/>
+      <c r="I337" s="27"/>
+      <c r="J337" s="27"/>
     </row>
     <row r="338" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" s="6" t="s">
         <v>756</v>
       </c>
-      <c r="C338" s="21"/>
+      <c r="C338" s="26"/>
       <c r="E338" s="6" t="s">
         <v>364</v>
       </c>
       <c r="F338" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="I338" s="18"/>
-      <c r="J338" s="18"/>
+      <c r="I338" s="27"/>
+      <c r="J338" s="27"/>
     </row>
     <row r="339" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" t="s">
@@ -8555,7 +8555,7 @@
       <c r="B339" t="s">
         <v>582</v>
       </c>
-      <c r="C339" s="19" t="s">
+      <c r="C339" s="24" t="s">
         <v>757</v>
       </c>
       <c r="D339" t="s">
@@ -8570,12 +8570,12 @@
       <c r="H339" t="s">
         <v>634</v>
       </c>
-      <c r="I339" s="18"/>
-      <c r="J339" s="18"/>
-      <c r="M339" s="26" t="s">
+      <c r="I339" s="27"/>
+      <c r="J339" s="27"/>
+      <c r="M339" s="21" t="s">
         <v>785</v>
       </c>
-      <c r="N339" s="26"/>
+      <c r="N339" s="21"/>
     </row>
     <row r="340" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" t="s">
@@ -8584,7 +8584,7 @@
       <c r="B340" t="s">
         <v>583</v>
       </c>
-      <c r="C340" s="20"/>
+      <c r="C340" s="25"/>
       <c r="D340" t="s">
         <v>763</v>
       </c>
@@ -8597,16 +8597,16 @@
       <c r="H340" t="s">
         <v>634</v>
       </c>
-      <c r="I340" s="18"/>
-      <c r="J340" s="18"/>
-      <c r="M340" s="27"/>
-      <c r="N340" s="27"/>
+      <c r="I340" s="27"/>
+      <c r="J340" s="27"/>
+      <c r="M340" s="22"/>
+      <c r="N340" s="22"/>
     </row>
     <row r="341" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" t="s">
         <v>301</v>
       </c>
-      <c r="C341" s="20"/>
+      <c r="C341" s="25"/>
       <c r="D341" t="s">
         <v>764</v>
       </c>
@@ -8619,16 +8619,16 @@
       <c r="H341" t="s">
         <v>634</v>
       </c>
-      <c r="I341" s="18"/>
-      <c r="J341" s="18"/>
-      <c r="M341" s="27"/>
-      <c r="N341" s="27"/>
+      <c r="I341" s="27"/>
+      <c r="J341" s="27"/>
+      <c r="M341" s="22"/>
+      <c r="N341" s="22"/>
     </row>
     <row r="342" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" t="s">
         <v>302</v>
       </c>
-      <c r="C342" s="20"/>
+      <c r="C342" s="25"/>
       <c r="D342" t="s">
         <v>765</v>
       </c>
@@ -8641,14 +8641,14 @@
       <c r="H342" t="s">
         <v>634</v>
       </c>
-      <c r="M342" s="27"/>
-      <c r="N342" s="27"/>
+      <c r="M342" s="22"/>
+      <c r="N342" s="22"/>
     </row>
     <row r="343" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" t="s">
         <v>303</v>
       </c>
-      <c r="C343" s="20"/>
+      <c r="C343" s="25"/>
       <c r="D343" t="s">
         <v>766</v>
       </c>
@@ -8661,14 +8661,14 @@
       <c r="H343" t="s">
         <v>634</v>
       </c>
-      <c r="M343" s="27"/>
-      <c r="N343" s="27"/>
+      <c r="M343" s="22"/>
+      <c r="N343" s="22"/>
     </row>
     <row r="344" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" t="s">
         <v>304</v>
       </c>
-      <c r="C344" s="20"/>
+      <c r="C344" s="25"/>
       <c r="D344" t="s">
         <v>767</v>
       </c>
@@ -8681,8 +8681,8 @@
       <c r="H344" t="s">
         <v>634</v>
       </c>
-      <c r="M344" s="27"/>
-      <c r="N344" s="27"/>
+      <c r="M344" s="22"/>
+      <c r="N344" s="22"/>
     </row>
     <row r="345" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" t="s">
@@ -8691,7 +8691,7 @@
       <c r="B345" t="s">
         <v>584</v>
       </c>
-      <c r="C345" s="20"/>
+      <c r="C345" s="25"/>
       <c r="D345" t="s">
         <v>768</v>
       </c>
@@ -8704,8 +8704,8 @@
       <c r="H345" t="s">
         <v>634</v>
       </c>
-      <c r="M345" s="28"/>
-      <c r="N345" s="28"/>
+      <c r="M345" s="23"/>
+      <c r="N345" s="23"/>
     </row>
     <row r="346" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" s="6" t="s">
@@ -8714,7 +8714,7 @@
       <c r="B346" s="6" t="s">
         <v>585</v>
       </c>
-      <c r="C346" s="21"/>
+      <c r="C346" s="26"/>
       <c r="D346" s="6" t="s">
         <v>769</v>
       </c>
@@ -8732,7 +8732,7 @@
       <c r="A347" t="s">
         <v>307</v>
       </c>
-      <c r="C347" s="19" t="s">
+      <c r="C347" s="24" t="s">
         <v>578</v>
       </c>
       <c r="E347" t="s">
@@ -8746,7 +8746,7 @@
       <c r="A348" t="s">
         <v>308</v>
       </c>
-      <c r="C348" s="20"/>
+      <c r="C348" s="25"/>
       <c r="E348" t="s">
         <v>357</v>
       </c>
@@ -8758,7 +8758,7 @@
       <c r="A349" t="s">
         <v>309</v>
       </c>
-      <c r="C349" s="20"/>
+      <c r="C349" s="25"/>
       <c r="E349" t="s">
         <v>357</v>
       </c>
@@ -8770,7 +8770,7 @@
       <c r="A350" t="s">
         <v>310</v>
       </c>
-      <c r="C350" s="20"/>
+      <c r="C350" s="25"/>
       <c r="E350" t="s">
         <v>357</v>
       </c>
@@ -8782,7 +8782,7 @@
       <c r="A351" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="C351" s="21"/>
+      <c r="C351" s="26"/>
       <c r="E351" s="6" t="s">
         <v>364</v>
       </c>
@@ -8794,7 +8794,7 @@
       <c r="A352" t="s">
         <v>312</v>
       </c>
-      <c r="C352" s="20" t="s">
+      <c r="C352" s="25" t="s">
         <v>579</v>
       </c>
       <c r="D352" t="s">
@@ -8809,22 +8809,22 @@
       <c r="H352" t="s">
         <v>636</v>
       </c>
-      <c r="I352" s="24" t="s">
+      <c r="I352" s="18" t="s">
         <v>783</v>
       </c>
-      <c r="J352" s="24"/>
-      <c r="K352" s="24"/>
-      <c r="L352" s="24"/>
-      <c r="M352" s="26" t="s">
+      <c r="J352" s="18"/>
+      <c r="K352" s="18"/>
+      <c r="L352" s="18"/>
+      <c r="M352" s="21" t="s">
         <v>785</v>
       </c>
-      <c r="N352" s="26"/>
+      <c r="N352" s="21"/>
     </row>
     <row r="353" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" t="s">
         <v>313</v>
       </c>
-      <c r="C353" s="20"/>
+      <c r="C353" s="25"/>
       <c r="D353" t="s">
         <v>781</v>
       </c>
@@ -8837,18 +8837,18 @@
       <c r="H353" t="s">
         <v>636</v>
       </c>
-      <c r="I353" s="23"/>
-      <c r="J353" s="23"/>
-      <c r="K353" s="23"/>
-      <c r="L353" s="23"/>
-      <c r="M353" s="27"/>
-      <c r="N353" s="27"/>
+      <c r="I353" s="19"/>
+      <c r="J353" s="19"/>
+      <c r="K353" s="19"/>
+      <c r="L353" s="19"/>
+      <c r="M353" s="22"/>
+      <c r="N353" s="22"/>
     </row>
     <row r="354" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" t="s">
         <v>314</v>
       </c>
-      <c r="C354" s="20"/>
+      <c r="C354" s="25"/>
       <c r="D354" t="s">
         <v>782</v>
       </c>
@@ -8864,18 +8864,18 @@
       <c r="H354" t="s">
         <v>636</v>
       </c>
-      <c r="I354" s="23"/>
-      <c r="J354" s="23"/>
-      <c r="K354" s="23"/>
-      <c r="L354" s="23"/>
-      <c r="M354" s="27"/>
-      <c r="N354" s="27"/>
+      <c r="I354" s="19"/>
+      <c r="J354" s="19"/>
+      <c r="K354" s="19"/>
+      <c r="L354" s="19"/>
+      <c r="M354" s="22"/>
+      <c r="N354" s="22"/>
     </row>
     <row r="355" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" t="s">
         <v>315</v>
       </c>
-      <c r="C355" s="20"/>
+      <c r="C355" s="25"/>
       <c r="E355" t="s">
         <v>357</v>
       </c>
@@ -8885,18 +8885,18 @@
       <c r="H355" t="s">
         <v>636</v>
       </c>
-      <c r="I355" s="23"/>
-      <c r="J355" s="23"/>
-      <c r="K355" s="23"/>
-      <c r="L355" s="23"/>
-      <c r="M355" s="27"/>
-      <c r="N355" s="27"/>
+      <c r="I355" s="19"/>
+      <c r="J355" s="19"/>
+      <c r="K355" s="19"/>
+      <c r="L355" s="19"/>
+      <c r="M355" s="22"/>
+      <c r="N355" s="22"/>
     </row>
     <row r="356" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" t="s">
         <v>316</v>
       </c>
-      <c r="C356" s="20"/>
+      <c r="C356" s="25"/>
       <c r="E356" t="s">
         <v>357</v>
       </c>
@@ -8906,18 +8906,18 @@
       <c r="H356" t="s">
         <v>636</v>
       </c>
-      <c r="I356" s="23"/>
-      <c r="J356" s="23"/>
-      <c r="K356" s="23"/>
-      <c r="L356" s="23"/>
-      <c r="M356" s="27"/>
-      <c r="N356" s="27"/>
+      <c r="I356" s="19"/>
+      <c r="J356" s="19"/>
+      <c r="K356" s="19"/>
+      <c r="L356" s="19"/>
+      <c r="M356" s="22"/>
+      <c r="N356" s="22"/>
     </row>
     <row r="357" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" t="s">
         <v>317</v>
       </c>
-      <c r="C357" s="20"/>
+      <c r="C357" s="25"/>
       <c r="E357" t="s">
         <v>357</v>
       </c>
@@ -8927,18 +8927,18 @@
       <c r="H357" t="s">
         <v>636</v>
       </c>
-      <c r="I357" s="23"/>
-      <c r="J357" s="23"/>
-      <c r="K357" s="23"/>
-      <c r="L357" s="23"/>
-      <c r="M357" s="27"/>
-      <c r="N357" s="27"/>
+      <c r="I357" s="19"/>
+      <c r="J357" s="19"/>
+      <c r="K357" s="19"/>
+      <c r="L357" s="19"/>
+      <c r="M357" s="22"/>
+      <c r="N357" s="22"/>
     </row>
     <row r="358" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A358" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="C358" s="21"/>
+      <c r="C358" s="26"/>
       <c r="E358" s="6" t="s">
         <v>364</v>
       </c>
@@ -8948,18 +8948,18 @@
       <c r="H358" s="6" t="s">
         <v>636</v>
       </c>
-      <c r="I358" s="25"/>
-      <c r="J358" s="25"/>
-      <c r="K358" s="25"/>
-      <c r="L358" s="25"/>
-      <c r="M358" s="28"/>
-      <c r="N358" s="28"/>
+      <c r="I358" s="20"/>
+      <c r="J358" s="20"/>
+      <c r="K358" s="20"/>
+      <c r="L358" s="20"/>
+      <c r="M358" s="23"/>
+      <c r="N358" s="23"/>
     </row>
     <row r="359" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" t="s">
         <v>319</v>
       </c>
-      <c r="C359" s="20" t="s">
+      <c r="C359" s="25" t="s">
         <v>580</v>
       </c>
       <c r="D359" t="s">
@@ -8979,7 +8979,7 @@
       <c r="A360" t="s">
         <v>320</v>
       </c>
-      <c r="C360" s="20"/>
+      <c r="C360" s="25"/>
       <c r="D360" t="s">
         <v>788</v>
       </c>
@@ -8997,7 +8997,7 @@
       <c r="A361" t="s">
         <v>321</v>
       </c>
-      <c r="C361" s="20"/>
+      <c r="C361" s="25"/>
       <c r="D361" t="s">
         <v>789</v>
       </c>
@@ -9015,7 +9015,7 @@
       <c r="A362" t="s">
         <v>322</v>
       </c>
-      <c r="C362" s="20"/>
+      <c r="C362" s="25"/>
       <c r="D362" t="s">
         <v>790</v>
       </c>
@@ -9033,7 +9033,7 @@
       <c r="A363" t="s">
         <v>323</v>
       </c>
-      <c r="C363" s="20"/>
+      <c r="C363" s="25"/>
       <c r="D363" t="s">
         <v>791</v>
       </c>
@@ -9051,7 +9051,7 @@
       <c r="A364" t="s">
         <v>324</v>
       </c>
-      <c r="C364" s="20"/>
+      <c r="C364" s="25"/>
       <c r="D364" t="s">
         <v>792</v>
       </c>
@@ -9069,7 +9069,7 @@
       <c r="A365" t="s">
         <v>325</v>
       </c>
-      <c r="C365" s="20"/>
+      <c r="C365" s="25"/>
       <c r="D365" t="s">
         <v>793</v>
       </c>
@@ -9087,7 +9087,7 @@
       <c r="A366" t="s">
         <v>326</v>
       </c>
-      <c r="C366" s="20"/>
+      <c r="C366" s="25"/>
       <c r="D366" t="s">
         <v>794</v>
       </c>
@@ -9105,7 +9105,7 @@
       <c r="A367" t="s">
         <v>327</v>
       </c>
-      <c r="C367" s="20"/>
+      <c r="C367" s="25"/>
       <c r="E367" t="s">
         <v>357</v>
       </c>
@@ -9117,7 +9117,7 @@
       <c r="A368" t="s">
         <v>328</v>
       </c>
-      <c r="C368" s="20"/>
+      <c r="C368" s="25"/>
       <c r="E368" t="s">
         <v>357</v>
       </c>
@@ -9129,7 +9129,7 @@
       <c r="A369" t="s">
         <v>329</v>
       </c>
-      <c r="C369" s="20"/>
+      <c r="C369" s="25"/>
       <c r="E369" t="s">
         <v>357</v>
       </c>
@@ -9141,7 +9141,7 @@
       <c r="A370" t="s">
         <v>330</v>
       </c>
-      <c r="C370" s="20"/>
+      <c r="C370" s="25"/>
       <c r="E370" t="s">
         <v>357</v>
       </c>
@@ -9153,7 +9153,7 @@
       <c r="A371" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C371" s="22"/>
+      <c r="C371" s="28"/>
       <c r="E371" s="12" t="s">
         <v>364</v>
       </c>
@@ -9164,12 +9164,40 @@
     <row r="372" spans="1:6" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="I352:L358"/>
-    <mergeCell ref="I318:L324"/>
-    <mergeCell ref="M318:N324"/>
-    <mergeCell ref="M326:N332"/>
-    <mergeCell ref="M339:N345"/>
-    <mergeCell ref="M352:N358"/>
+    <mergeCell ref="I165:M168"/>
+    <mergeCell ref="C318:C324"/>
+    <mergeCell ref="C347:C351"/>
+    <mergeCell ref="C352:C358"/>
+    <mergeCell ref="C359:C371"/>
+    <mergeCell ref="C339:C346"/>
+    <mergeCell ref="C262:C278"/>
+    <mergeCell ref="C280:C287"/>
+    <mergeCell ref="C288:C304"/>
+    <mergeCell ref="C305:C309"/>
+    <mergeCell ref="C310:C315"/>
+    <mergeCell ref="C227:C240"/>
+    <mergeCell ref="C241:C245"/>
+    <mergeCell ref="C246:C247"/>
+    <mergeCell ref="C248:C252"/>
+    <mergeCell ref="C253:C261"/>
+    <mergeCell ref="C190:C194"/>
+    <mergeCell ref="C195:C199"/>
+    <mergeCell ref="C200:C204"/>
+    <mergeCell ref="C205:C209"/>
+    <mergeCell ref="C210:C226"/>
+    <mergeCell ref="C158:C162"/>
+    <mergeCell ref="C163:C168"/>
+    <mergeCell ref="C169:C182"/>
+    <mergeCell ref="C183:C187"/>
+    <mergeCell ref="C188:C189"/>
+    <mergeCell ref="C112:C130"/>
+    <mergeCell ref="C131:C135"/>
+    <mergeCell ref="C136:C151"/>
+    <mergeCell ref="C153:C157"/>
+    <mergeCell ref="C71:C78"/>
+    <mergeCell ref="C79:C86"/>
+    <mergeCell ref="C87:C91"/>
+    <mergeCell ref="C92:C110"/>
     <mergeCell ref="I262:K265"/>
     <mergeCell ref="C326:C333"/>
     <mergeCell ref="C334:C338"/>
@@ -9186,40 +9214,12 @@
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C36:C40"/>
     <mergeCell ref="C28:C35"/>
-    <mergeCell ref="C112:C130"/>
-    <mergeCell ref="C131:C135"/>
-    <mergeCell ref="C136:C151"/>
-    <mergeCell ref="C153:C157"/>
-    <mergeCell ref="C71:C78"/>
-    <mergeCell ref="C79:C86"/>
-    <mergeCell ref="C87:C91"/>
-    <mergeCell ref="C92:C110"/>
-    <mergeCell ref="C158:C162"/>
-    <mergeCell ref="C163:C168"/>
-    <mergeCell ref="C169:C182"/>
-    <mergeCell ref="C183:C187"/>
-    <mergeCell ref="C188:C189"/>
-    <mergeCell ref="C190:C194"/>
-    <mergeCell ref="C195:C199"/>
-    <mergeCell ref="C200:C204"/>
-    <mergeCell ref="C205:C209"/>
-    <mergeCell ref="C210:C226"/>
-    <mergeCell ref="I165:M168"/>
-    <mergeCell ref="C318:C324"/>
-    <mergeCell ref="C347:C351"/>
-    <mergeCell ref="C352:C358"/>
-    <mergeCell ref="C359:C371"/>
-    <mergeCell ref="C339:C346"/>
-    <mergeCell ref="C262:C278"/>
-    <mergeCell ref="C280:C287"/>
-    <mergeCell ref="C288:C304"/>
-    <mergeCell ref="C305:C309"/>
-    <mergeCell ref="C310:C315"/>
-    <mergeCell ref="C227:C240"/>
-    <mergeCell ref="C241:C245"/>
-    <mergeCell ref="C246:C247"/>
-    <mergeCell ref="C248:C252"/>
-    <mergeCell ref="C253:C261"/>
+    <mergeCell ref="I352:L358"/>
+    <mergeCell ref="I318:L324"/>
+    <mergeCell ref="M318:N324"/>
+    <mergeCell ref="M326:N332"/>
+    <mergeCell ref="M339:N345"/>
+    <mergeCell ref="M352:N358"/>
   </mergeCells>
   <conditionalFormatting sqref="I262 H1:H264 H266:H290 H292:H304 H306:H1048576">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">

</xml_diff>

<commit_message>
Working on separating Switch Task data
</commit_message>
<xml_diff>
--- a/PsychoPyData_ColumnKey.xlsx
+++ b/PsychoPyData_ColumnKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofc-my.sharepoint.com/personal/chelsie_hart_ucalgary_ca/Documents/1_PhD_Project/Scripting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1738" documentId="8_{447AABAE-0265-45CA-9969-8E24E37FF3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECCC3420-6B50-4F27-A63C-EB751776FFE5}"/>
+  <xr:revisionPtr revIDLastSave="1766" documentId="8_{447AABAE-0265-45CA-9969-8E24E37FF3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EB63841-7C44-429F-93B4-47CB82352266}"/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="2592" windowWidth="10800" windowHeight="10608" xr2:uid="{5015AFB7-EBCA-4E4E-B1B8-96F1F0B54514}"/>
+    <workbookView xWindow="7998" yWindow="1932" windowWidth="12294" windowHeight="12090" xr2:uid="{5015AFB7-EBCA-4E4E-B1B8-96F1F0B54514}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="802">
   <si>
     <t>SARTkey_resp_practice.keys</t>
   </si>
@@ -2436,6 +2436,12 @@
   </si>
   <si>
     <t>Note: currently data is loaded into matlab as a table where all variables are of class 'cell'. Note that output usually starts with the practice data from the first task, then the participant ID, then the rest of the data from that task, then the task randomizer loop information.     March 4, 2023 added to tasks to record symm span response times.     March 8, 2023 adding in response times and storage for all responses in routines to check for breaks. adding in syncing to screen refresh for all responses.</t>
+  </si>
+  <si>
+    <t>Switch mixed actual dummy</t>
+  </si>
+  <si>
+    <t>Switch mixed practice dummy</t>
   </si>
 </sst>
 </file>
@@ -2527,7 +2533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2556,10 +2562,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2574,19 +2595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2954,10 +2963,10 @@
   <dimension ref="A1:N372"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2997,12 +3006,12 @@
       <c r="H1" t="s">
         <v>335</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="23" t="s">
         <v>799</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
@@ -3020,10 +3029,10 @@
       <c r="H2" t="s">
         <v>632</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
@@ -3041,10 +3050,10 @@
       <c r="H3" t="s">
         <v>633</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -3062,10 +3071,10 @@
       <c r="H4" t="s">
         <v>632</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
@@ -3083,10 +3092,10 @@
       <c r="H5" t="s">
         <v>632</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
@@ -3104,10 +3113,10 @@
       <c r="H6" t="s">
         <v>632</v>
       </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -3125,10 +3134,10 @@
       <c r="H7" t="s">
         <v>632</v>
       </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
     </row>
     <row r="8" spans="1:12" s="12" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="12" t="s">
@@ -3147,16 +3156,16 @@
       <c r="H8" s="12" t="s">
         <v>632</v>
       </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
     </row>
     <row r="9" spans="1:12" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="19" t="s">
         <v>532</v>
       </c>
       <c r="E9" t="s">
@@ -3165,16 +3174,16 @@
       <c r="F9" t="s">
         <v>398</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="20"/>
       <c r="E10" t="s">
         <v>357</v>
       </c>
@@ -3184,16 +3193,16 @@
       <c r="H10" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="20"/>
       <c r="E11" t="s">
         <v>357</v>
       </c>
@@ -3203,16 +3212,16 @@
       <c r="H11" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="25"/>
+      <c r="C12" s="20"/>
       <c r="E12" t="s">
         <v>357</v>
       </c>
@@ -3222,16 +3231,16 @@
       <c r="H12" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="20"/>
       <c r="E13" t="s">
         <v>364</v>
       </c>
@@ -3243,7 +3252,7 @@
       <c r="A14" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="25"/>
+      <c r="C14" s="20"/>
       <c r="E14" t="s">
         <v>364</v>
       </c>
@@ -3258,7 +3267,7 @@
       <c r="A15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="25"/>
+      <c r="C15" s="20"/>
       <c r="E15" t="s">
         <v>364</v>
       </c>
@@ -3273,7 +3282,7 @@
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="25"/>
+      <c r="C16" s="20"/>
       <c r="E16" t="s">
         <v>364</v>
       </c>
@@ -3288,7 +3297,7 @@
       <c r="A17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="28"/>
+      <c r="C17" s="22"/>
       <c r="E17" s="12" t="s">
         <v>364</v>
       </c>
@@ -3303,7 +3312,7 @@
       <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="20" t="s">
         <v>533</v>
       </c>
       <c r="D18" t="s">
@@ -3323,7 +3332,7 @@
       <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="25"/>
+      <c r="C19" s="20"/>
       <c r="D19" t="s">
         <v>353</v>
       </c>
@@ -3341,7 +3350,7 @@
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="25"/>
+      <c r="C20" s="20"/>
       <c r="D20" t="s">
         <v>354</v>
       </c>
@@ -3362,7 +3371,7 @@
       <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="25"/>
+      <c r="C21" s="20"/>
       <c r="E21" t="s">
         <v>357</v>
       </c>
@@ -3374,7 +3383,7 @@
       <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="25"/>
+      <c r="C22" s="20"/>
       <c r="E22" t="s">
         <v>357</v>
       </c>
@@ -3389,7 +3398,7 @@
       <c r="A23" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="25"/>
+      <c r="C23" s="20"/>
       <c r="D23" t="s">
         <v>384</v>
       </c>
@@ -3410,7 +3419,7 @@
       <c r="A24" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="25"/>
+      <c r="C24" s="20"/>
       <c r="E24" t="s">
         <v>357</v>
       </c>
@@ -3422,7 +3431,7 @@
       <c r="A25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="26"/>
+      <c r="C25" s="21"/>
       <c r="E25" s="6" t="s">
         <v>364</v>
       </c>
@@ -3434,7 +3443,7 @@
       <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="19" t="s">
         <v>534</v>
       </c>
       <c r="D26" t="s">
@@ -3457,7 +3466,7 @@
       <c r="A27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="26"/>
+      <c r="C27" s="21"/>
       <c r="D27" s="6" t="s">
         <v>409</v>
       </c>
@@ -3478,7 +3487,7 @@
       <c r="A28" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="20" t="s">
         <v>535</v>
       </c>
       <c r="D28" t="s">
@@ -3501,7 +3510,7 @@
       <c r="A29" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="25"/>
+      <c r="C29" s="20"/>
       <c r="D29" t="s">
         <v>348</v>
       </c>
@@ -3519,7 +3528,7 @@
       <c r="A30" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="25"/>
+      <c r="C30" s="20"/>
       <c r="D30" t="s">
         <v>378</v>
       </c>
@@ -3537,7 +3546,7 @@
       <c r="A31" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="25"/>
+      <c r="C31" s="20"/>
       <c r="E31" t="s">
         <v>357</v>
       </c>
@@ -3549,7 +3558,7 @@
       <c r="A32" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="25"/>
+      <c r="C32" s="20"/>
       <c r="E32" t="s">
         <v>357</v>
       </c>
@@ -3561,7 +3570,7 @@
       <c r="A33" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="25"/>
+      <c r="C33" s="20"/>
       <c r="D33" t="s">
         <v>385</v>
       </c>
@@ -3582,7 +3591,7 @@
       <c r="A34" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="25"/>
+      <c r="C34" s="20"/>
       <c r="E34" t="s">
         <v>357</v>
       </c>
@@ -3594,7 +3603,7 @@
       <c r="A35" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="26"/>
+      <c r="C35" s="21"/>
       <c r="E35" s="6" t="s">
         <v>364</v>
       </c>
@@ -3606,7 +3615,7 @@
       <c r="A36" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="19" t="s">
         <v>536</v>
       </c>
       <c r="E36" t="s">
@@ -3620,7 +3629,7 @@
       <c r="A37" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="25"/>
+      <c r="C37" s="20"/>
       <c r="E37" t="s">
         <v>357</v>
       </c>
@@ -3632,7 +3641,7 @@
       <c r="A38" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="25"/>
+      <c r="C38" s="20"/>
       <c r="E38" t="s">
         <v>357</v>
       </c>
@@ -3644,7 +3653,7 @@
       <c r="A39" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="25"/>
+      <c r="C39" s="20"/>
       <c r="E39" t="s">
         <v>357</v>
       </c>
@@ -3656,7 +3665,7 @@
       <c r="A40" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="28"/>
+      <c r="C40" s="22"/>
       <c r="E40" s="12" t="s">
         <v>364</v>
       </c>
@@ -3668,7 +3677,7 @@
       <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="20" t="s">
         <v>537</v>
       </c>
       <c r="D41" t="s">
@@ -3691,7 +3700,7 @@
       <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="25"/>
+      <c r="C42" s="20"/>
       <c r="D42" t="s">
         <v>411</v>
       </c>
@@ -3712,7 +3721,7 @@
       <c r="A43" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="25"/>
+      <c r="C43" s="20"/>
       <c r="D43" t="s">
         <v>412</v>
       </c>
@@ -3733,7 +3742,7 @@
       <c r="A44" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="25"/>
+      <c r="C44" s="20"/>
       <c r="E44" t="s">
         <v>357</v>
       </c>
@@ -3745,7 +3754,7 @@
       <c r="A45" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="25"/>
+      <c r="C45" s="20"/>
       <c r="E45" t="s">
         <v>357</v>
       </c>
@@ -3757,7 +3766,7 @@
       <c r="A46" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="25"/>
+      <c r="C46" s="20"/>
       <c r="D46" t="s">
         <v>413</v>
       </c>
@@ -3778,7 +3787,7 @@
       <c r="A47" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="25"/>
+      <c r="C47" s="20"/>
       <c r="E47" t="s">
         <v>357</v>
       </c>
@@ -3790,7 +3799,7 @@
       <c r="A48" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="26"/>
+      <c r="C48" s="21"/>
       <c r="E48" s="6" t="s">
         <v>364</v>
       </c>
@@ -3802,7 +3811,7 @@
       <c r="A49" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="19" t="s">
         <v>538</v>
       </c>
       <c r="D49" t="s">
@@ -3825,7 +3834,7 @@
       <c r="A50" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="26"/>
+      <c r="C50" s="21"/>
       <c r="D50" s="6" t="s">
         <v>422</v>
       </c>
@@ -3846,7 +3855,7 @@
       <c r="A51" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="19" t="s">
         <v>539</v>
       </c>
       <c r="D51" t="s">
@@ -3869,7 +3878,7 @@
       <c r="A52" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="25"/>
+      <c r="C52" s="20"/>
       <c r="D52" t="s">
         <v>415</v>
       </c>
@@ -3890,7 +3899,7 @@
       <c r="A53" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="25"/>
+      <c r="C53" s="20"/>
       <c r="D53" t="s">
         <v>416</v>
       </c>
@@ -3911,7 +3920,7 @@
       <c r="A54" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="25"/>
+      <c r="C54" s="20"/>
       <c r="E54" t="s">
         <v>357</v>
       </c>
@@ -3923,7 +3932,7 @@
       <c r="A55" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="25"/>
+      <c r="C55" s="20"/>
       <c r="E55" t="s">
         <v>357</v>
       </c>
@@ -3935,7 +3944,7 @@
       <c r="A56" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="25"/>
+      <c r="C56" s="20"/>
       <c r="D56" t="s">
         <v>417</v>
       </c>
@@ -3956,7 +3965,7 @@
       <c r="A57" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="25"/>
+      <c r="C57" s="20"/>
       <c r="E57" t="s">
         <v>357</v>
       </c>
@@ -3968,7 +3977,7 @@
       <c r="A58" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="26"/>
+      <c r="C58" s="21"/>
       <c r="E58" s="6" t="s">
         <v>364</v>
       </c>
@@ -3980,7 +3989,7 @@
       <c r="A59" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C59" s="19" t="s">
         <v>540</v>
       </c>
       <c r="E59" t="s">
@@ -3994,7 +4003,7 @@
       <c r="A60" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="25"/>
+      <c r="C60" s="20"/>
       <c r="E60" t="s">
         <v>357</v>
       </c>
@@ -4006,7 +4015,7 @@
       <c r="A61" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="25"/>
+      <c r="C61" s="20"/>
       <c r="E61" t="s">
         <v>357</v>
       </c>
@@ -4018,7 +4027,7 @@
       <c r="A62" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="25"/>
+      <c r="C62" s="20"/>
       <c r="E62" t="s">
         <v>357</v>
       </c>
@@ -4030,7 +4039,7 @@
       <c r="A63" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C63" s="26"/>
+      <c r="C63" s="21"/>
       <c r="E63" s="6" t="s">
         <v>364</v>
       </c>
@@ -4042,7 +4051,7 @@
       <c r="A64" t="s">
         <v>61</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C64" s="19" t="s">
         <v>541</v>
       </c>
       <c r="E64" t="s">
@@ -4056,7 +4065,7 @@
       <c r="A65" t="s">
         <v>62</v>
       </c>
-      <c r="C65" s="25"/>
+      <c r="C65" s="20"/>
       <c r="E65" t="s">
         <v>357</v>
       </c>
@@ -4068,7 +4077,7 @@
       <c r="A66" t="s">
         <v>63</v>
       </c>
-      <c r="C66" s="25"/>
+      <c r="C66" s="20"/>
       <c r="E66" t="s">
         <v>357</v>
       </c>
@@ -4083,7 +4092,7 @@
       <c r="A67" t="s">
         <v>64</v>
       </c>
-      <c r="C67" s="25"/>
+      <c r="C67" s="20"/>
       <c r="E67" t="s">
         <v>357</v>
       </c>
@@ -4098,7 +4107,7 @@
       <c r="A68" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C68" s="26"/>
+      <c r="C68" s="21"/>
       <c r="E68" s="6" t="s">
         <v>364</v>
       </c>
@@ -4111,7 +4120,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="24" t="s">
+      <c r="C69" s="19" t="s">
         <v>542</v>
       </c>
       <c r="E69" t="s">
@@ -4129,7 +4138,7 @@
         <v>67</v>
       </c>
       <c r="B70" s="10"/>
-      <c r="C70" s="26"/>
+      <c r="C70" s="21"/>
       <c r="E70" s="6" t="s">
         <v>364</v>
       </c>
@@ -4144,7 +4153,7 @@
       <c r="A71" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="24" t="s">
+      <c r="C71" s="19" t="s">
         <v>543</v>
       </c>
       <c r="D71" t="s">
@@ -4167,7 +4176,7 @@
       <c r="A72" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="25"/>
+      <c r="C72" s="20"/>
       <c r="D72" t="s">
         <v>428</v>
       </c>
@@ -4188,7 +4197,7 @@
       <c r="A73" t="s">
         <v>70</v>
       </c>
-      <c r="C73" s="25"/>
+      <c r="C73" s="20"/>
       <c r="D73" t="s">
         <v>429</v>
       </c>
@@ -4209,7 +4218,7 @@
       <c r="A74" t="s">
         <v>71</v>
       </c>
-      <c r="C74" s="25"/>
+      <c r="C74" s="20"/>
       <c r="E74" t="s">
         <v>357</v>
       </c>
@@ -4221,7 +4230,7 @@
       <c r="A75" t="s">
         <v>72</v>
       </c>
-      <c r="C75" s="25"/>
+      <c r="C75" s="20"/>
       <c r="E75" t="s">
         <v>357</v>
       </c>
@@ -4233,7 +4242,7 @@
       <c r="A76" t="s">
         <v>73</v>
       </c>
-      <c r="C76" s="25"/>
+      <c r="C76" s="20"/>
       <c r="D76" t="s">
         <v>433</v>
       </c>
@@ -4254,7 +4263,7 @@
       <c r="A77" t="s">
         <v>74</v>
       </c>
-      <c r="C77" s="25"/>
+      <c r="C77" s="20"/>
       <c r="E77" t="s">
         <v>357</v>
       </c>
@@ -4266,7 +4275,7 @@
       <c r="A78" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C78" s="26"/>
+      <c r="C78" s="21"/>
       <c r="E78" s="6" t="s">
         <v>364</v>
       </c>
@@ -4278,7 +4287,7 @@
       <c r="A79" t="s">
         <v>76</v>
       </c>
-      <c r="C79" s="24" t="s">
+      <c r="C79" s="19" t="s">
         <v>544</v>
       </c>
       <c r="D79" t="s">
@@ -4301,7 +4310,7 @@
       <c r="A80" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="25"/>
+      <c r="C80" s="20"/>
       <c r="D80" t="s">
         <v>436</v>
       </c>
@@ -4322,7 +4331,7 @@
       <c r="A81" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="25"/>
+      <c r="C81" s="20"/>
       <c r="D81" t="s">
         <v>437</v>
       </c>
@@ -4343,7 +4352,7 @@
       <c r="A82" t="s">
         <v>79</v>
       </c>
-      <c r="C82" s="25"/>
+      <c r="C82" s="20"/>
       <c r="E82" t="s">
         <v>357</v>
       </c>
@@ -4355,7 +4364,7 @@
       <c r="A83" t="s">
         <v>80</v>
       </c>
-      <c r="C83" s="25"/>
+      <c r="C83" s="20"/>
       <c r="E83" t="s">
         <v>357</v>
       </c>
@@ -4367,7 +4376,7 @@
       <c r="A84" t="s">
         <v>81</v>
       </c>
-      <c r="C84" s="25"/>
+      <c r="C84" s="20"/>
       <c r="D84" t="s">
         <v>435</v>
       </c>
@@ -4388,7 +4397,7 @@
       <c r="A85" t="s">
         <v>82</v>
       </c>
-      <c r="C85" s="25"/>
+      <c r="C85" s="20"/>
       <c r="E85" t="s">
         <v>357</v>
       </c>
@@ -4400,7 +4409,7 @@
       <c r="A86" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C86" s="26"/>
+      <c r="C86" s="21"/>
       <c r="E86" s="6" t="s">
         <v>364</v>
       </c>
@@ -4412,7 +4421,7 @@
       <c r="A87" t="s">
         <v>84</v>
       </c>
-      <c r="C87" s="24" t="s">
+      <c r="C87" s="19" t="s">
         <v>545</v>
       </c>
       <c r="E87" t="s">
@@ -4426,7 +4435,7 @@
       <c r="A88" t="s">
         <v>85</v>
       </c>
-      <c r="C88" s="25"/>
+      <c r="C88" s="20"/>
       <c r="E88" t="s">
         <v>357</v>
       </c>
@@ -4438,7 +4447,7 @@
       <c r="A89" t="s">
         <v>86</v>
       </c>
-      <c r="C89" s="25"/>
+      <c r="C89" s="20"/>
       <c r="E89" t="s">
         <v>357</v>
       </c>
@@ -4450,7 +4459,7 @@
       <c r="A90" t="s">
         <v>87</v>
       </c>
-      <c r="C90" s="25"/>
+      <c r="C90" s="20"/>
       <c r="E90" t="s">
         <v>357</v>
       </c>
@@ -4462,7 +4471,7 @@
       <c r="A91" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="26"/>
+      <c r="C91" s="21"/>
       <c r="E91" s="6" t="s">
         <v>364</v>
       </c>
@@ -4474,8 +4483,8 @@
       <c r="A92" t="s">
         <v>89</v>
       </c>
-      <c r="C92" s="24" t="s">
-        <v>546</v>
+      <c r="C92" s="19" t="s">
+        <v>801</v>
       </c>
       <c r="D92" t="s">
         <v>445</v>
@@ -4497,7 +4506,7 @@
       <c r="A93" t="s">
         <v>90</v>
       </c>
-      <c r="C93" s="25"/>
+      <c r="C93" s="20"/>
       <c r="D93" t="s">
         <v>448</v>
       </c>
@@ -4518,7 +4527,7 @@
       <c r="A94" t="s">
         <v>91</v>
       </c>
-      <c r="C94" s="25"/>
+      <c r="C94" s="20"/>
       <c r="D94" t="s">
         <v>450</v>
       </c>
@@ -4539,7 +4548,7 @@
       <c r="A95" t="s">
         <v>92</v>
       </c>
-      <c r="C95" s="25"/>
+      <c r="C95" s="20"/>
       <c r="D95" t="s">
         <v>453</v>
       </c>
@@ -4560,7 +4569,7 @@
       <c r="A96" t="s">
         <v>93</v>
       </c>
-      <c r="C96" s="25"/>
+      <c r="C96" s="20"/>
       <c r="D96" t="s">
         <v>454</v>
       </c>
@@ -4581,7 +4590,7 @@
       <c r="A97" t="s">
         <v>94</v>
       </c>
-      <c r="C97" s="25"/>
+      <c r="C97" s="20"/>
       <c r="D97" t="s">
         <v>455</v>
       </c>
@@ -4598,24 +4607,24 @@
         <v>634</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" t="s">
+    <row r="98" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C98" s="25"/>
-      <c r="D98" t="s">
+      <c r="C98" s="21"/>
+      <c r="D98" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F98" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G98" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="H98" t="s">
+      <c r="H98" s="6" t="s">
         <v>634</v>
       </c>
     </row>
@@ -4623,7 +4632,9 @@
       <c r="A99" t="s">
         <v>96</v>
       </c>
-      <c r="C99" s="25"/>
+      <c r="C99" s="19" t="s">
+        <v>546</v>
+      </c>
       <c r="D99" t="s">
         <v>459</v>
       </c>
@@ -4644,7 +4655,7 @@
       <c r="A100" t="s">
         <v>97</v>
       </c>
-      <c r="C100" s="25"/>
+      <c r="C100" s="29"/>
       <c r="D100" t="s">
         <v>460</v>
       </c>
@@ -4665,7 +4676,7 @@
       <c r="A101" t="s">
         <v>98</v>
       </c>
-      <c r="C101" s="25"/>
+      <c r="C101" s="29"/>
       <c r="D101" t="s">
         <v>461</v>
       </c>
@@ -4686,7 +4697,7 @@
       <c r="A102" t="s">
         <v>99</v>
       </c>
-      <c r="C102" s="25"/>
+      <c r="C102" s="29"/>
       <c r="D102" t="s">
         <v>465</v>
       </c>
@@ -4707,7 +4718,7 @@
       <c r="A103" t="s">
         <v>100</v>
       </c>
-      <c r="C103" s="25"/>
+      <c r="C103" s="29"/>
       <c r="D103" t="s">
         <v>466</v>
       </c>
@@ -4728,7 +4739,7 @@
       <c r="A104" t="s">
         <v>101</v>
       </c>
-      <c r="C104" s="25"/>
+      <c r="C104" s="29"/>
       <c r="D104" t="s">
         <v>467</v>
       </c>
@@ -4749,7 +4760,7 @@
       <c r="A105" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="25"/>
+      <c r="C105" s="29"/>
       <c r="D105" t="s">
         <v>468</v>
       </c>
@@ -4770,7 +4781,7 @@
       <c r="A106" t="s">
         <v>103</v>
       </c>
-      <c r="C106" s="25"/>
+      <c r="C106" s="29"/>
       <c r="E106" t="s">
         <v>357</v>
       </c>
@@ -4782,7 +4793,7 @@
       <c r="A107" t="s">
         <v>104</v>
       </c>
-      <c r="C107" s="25"/>
+      <c r="C107" s="29"/>
       <c r="E107" t="s">
         <v>357</v>
       </c>
@@ -4794,7 +4805,7 @@
       <c r="A108" t="s">
         <v>105</v>
       </c>
-      <c r="C108" s="25"/>
+      <c r="C108" s="29"/>
       <c r="D108" t="s">
         <v>472</v>
       </c>
@@ -4815,7 +4826,7 @@
       <c r="A109" t="s">
         <v>106</v>
       </c>
-      <c r="C109" s="25"/>
+      <c r="C109" s="29"/>
       <c r="E109" t="s">
         <v>357</v>
       </c>
@@ -4827,7 +4838,7 @@
       <c r="A110" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C110" s="26"/>
+      <c r="C110" s="21"/>
       <c r="E110" s="6" t="s">
         <v>364</v>
       </c>
@@ -4853,8 +4864,8 @@
       <c r="A112" t="s">
         <v>109</v>
       </c>
-      <c r="C112" s="24" t="s">
-        <v>548</v>
+      <c r="C112" s="19" t="s">
+        <v>800</v>
       </c>
       <c r="D112" t="s">
         <v>476</v>
@@ -4873,7 +4884,7 @@
       <c r="A113" t="s">
         <v>110</v>
       </c>
-      <c r="C113" s="25"/>
+      <c r="C113" s="20"/>
       <c r="D113" t="s">
         <v>477</v>
       </c>
@@ -4891,7 +4902,7 @@
       <c r="A114" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="25"/>
+      <c r="C114" s="20"/>
       <c r="D114" t="s">
         <v>478</v>
       </c>
@@ -4909,7 +4920,7 @@
       <c r="A115" t="s">
         <v>112</v>
       </c>
-      <c r="C115" s="25"/>
+      <c r="C115" s="20"/>
       <c r="D115" t="s">
         <v>479</v>
       </c>
@@ -4927,7 +4938,7 @@
       <c r="A116" t="s">
         <v>113</v>
       </c>
-      <c r="C116" s="25"/>
+      <c r="C116" s="20"/>
       <c r="D116" t="s">
         <v>480</v>
       </c>
@@ -4948,7 +4959,7 @@
       <c r="A117" t="s">
         <v>114</v>
       </c>
-      <c r="C117" s="25"/>
+      <c r="C117" s="20"/>
       <c r="D117" t="s">
         <v>481</v>
       </c>
@@ -4965,24 +4976,24 @@
         <v>636</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" t="s">
+    <row r="118" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C118" s="25"/>
-      <c r="D118" t="s">
+      <c r="C118" s="21"/>
+      <c r="D118" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E118" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="F118" t="s">
+      <c r="F118" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="G118" t="s">
+      <c r="G118" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="H118" t="s">
+      <c r="H118" s="6" t="s">
         <v>636</v>
       </c>
     </row>
@@ -4990,7 +5001,9 @@
       <c r="A119" t="s">
         <v>116</v>
       </c>
-      <c r="C119" s="25"/>
+      <c r="C119" s="19" t="s">
+        <v>548</v>
+      </c>
       <c r="D119" t="s">
         <v>442</v>
       </c>
@@ -5011,7 +5024,7 @@
       <c r="A120" t="s">
         <v>117</v>
       </c>
-      <c r="C120" s="25"/>
+      <c r="C120" s="29"/>
       <c r="D120" t="s">
         <v>483</v>
       </c>
@@ -5032,7 +5045,7 @@
       <c r="A121" t="s">
         <v>118</v>
       </c>
-      <c r="C121" s="25"/>
+      <c r="C121" s="29"/>
       <c r="D121" t="s">
         <v>487</v>
       </c>
@@ -5053,7 +5066,7 @@
       <c r="A122" t="s">
         <v>119</v>
       </c>
-      <c r="C122" s="25"/>
+      <c r="C122" s="29"/>
       <c r="D122" t="s">
         <v>484</v>
       </c>
@@ -5074,7 +5087,7 @@
       <c r="A123" t="s">
         <v>120</v>
       </c>
-      <c r="C123" s="25"/>
+      <c r="C123" s="29"/>
       <c r="D123" t="s">
         <v>485</v>
       </c>
@@ -5095,7 +5108,7 @@
       <c r="A124" t="s">
         <v>121</v>
       </c>
-      <c r="C124" s="25"/>
+      <c r="C124" s="29"/>
       <c r="D124" t="s">
         <v>486</v>
       </c>
@@ -5116,7 +5129,7 @@
       <c r="A125" t="s">
         <v>122</v>
       </c>
-      <c r="C125" s="25"/>
+      <c r="C125" s="29"/>
       <c r="D125" t="s">
         <v>482</v>
       </c>
@@ -5137,7 +5150,7 @@
       <c r="A126" t="s">
         <v>123</v>
       </c>
-      <c r="C126" s="25"/>
+      <c r="C126" s="29"/>
       <c r="E126" t="s">
         <v>357</v>
       </c>
@@ -5149,7 +5162,7 @@
       <c r="A127" t="s">
         <v>124</v>
       </c>
-      <c r="C127" s="25"/>
+      <c r="C127" s="29"/>
       <c r="E127" t="s">
         <v>357</v>
       </c>
@@ -5161,7 +5174,7 @@
       <c r="A128" t="s">
         <v>125</v>
       </c>
-      <c r="C128" s="25"/>
+      <c r="C128" s="29"/>
       <c r="D128" t="s">
         <v>491</v>
       </c>
@@ -5182,7 +5195,7 @@
       <c r="A129" t="s">
         <v>126</v>
       </c>
-      <c r="C129" s="25"/>
+      <c r="C129" s="29"/>
       <c r="E129" t="s">
         <v>357</v>
       </c>
@@ -5194,7 +5207,7 @@
       <c r="A130" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C130" s="26"/>
+      <c r="C130" s="21"/>
       <c r="E130" s="6" t="s">
         <v>364</v>
       </c>
@@ -5206,7 +5219,7 @@
       <c r="A131" t="s">
         <v>128</v>
       </c>
-      <c r="C131" s="24" t="s">
+      <c r="C131" s="19" t="s">
         <v>549</v>
       </c>
       <c r="E131" t="s">
@@ -5220,7 +5233,7 @@
       <c r="A132" t="s">
         <v>129</v>
       </c>
-      <c r="C132" s="25"/>
+      <c r="C132" s="20"/>
       <c r="E132" t="s">
         <v>357</v>
       </c>
@@ -5232,7 +5245,7 @@
       <c r="A133" t="s">
         <v>130</v>
       </c>
-      <c r="C133" s="25"/>
+      <c r="C133" s="20"/>
       <c r="E133" t="s">
         <v>357</v>
       </c>
@@ -5244,7 +5257,7 @@
       <c r="A134" t="s">
         <v>131</v>
       </c>
-      <c r="C134" s="25"/>
+      <c r="C134" s="20"/>
       <c r="E134" t="s">
         <v>357</v>
       </c>
@@ -5256,7 +5269,7 @@
       <c r="A135" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C135" s="28"/>
+      <c r="C135" s="22"/>
       <c r="E135" s="12" t="s">
         <v>364</v>
       </c>
@@ -5268,7 +5281,7 @@
       <c r="A136" t="s">
         <v>133</v>
       </c>
-      <c r="C136" s="25" t="s">
+      <c r="C136" s="20" t="s">
         <v>550</v>
       </c>
       <c r="D136" t="s">
@@ -5291,7 +5304,7 @@
       <c r="A137" t="s">
         <v>134</v>
       </c>
-      <c r="C137" s="25"/>
+      <c r="C137" s="20"/>
       <c r="D137" t="s">
         <v>501</v>
       </c>
@@ -5312,7 +5325,7 @@
       <c r="A138" t="s">
         <v>135</v>
       </c>
-      <c r="C138" s="25"/>
+      <c r="C138" s="20"/>
       <c r="E138" t="s">
         <v>497</v>
       </c>
@@ -5327,7 +5340,7 @@
       <c r="A139" t="s">
         <v>136</v>
       </c>
-      <c r="C139" s="25"/>
+      <c r="C139" s="20"/>
       <c r="D139" t="s">
         <v>502</v>
       </c>
@@ -5348,7 +5361,7 @@
       <c r="A140" t="s">
         <v>637</v>
       </c>
-      <c r="C140" s="25"/>
+      <c r="C140" s="20"/>
       <c r="E140" t="s">
         <v>623</v>
       </c>
@@ -5366,7 +5379,7 @@
       <c r="A141" t="s">
         <v>638</v>
       </c>
-      <c r="C141" s="25"/>
+      <c r="C141" s="20"/>
       <c r="E141" t="s">
         <v>623</v>
       </c>
@@ -5384,7 +5397,7 @@
       <c r="A142" t="s">
         <v>639</v>
       </c>
-      <c r="C142" s="25"/>
+      <c r="C142" s="20"/>
       <c r="E142" t="s">
         <v>629</v>
       </c>
@@ -5402,7 +5415,7 @@
       <c r="A143" t="s">
         <v>640</v>
       </c>
-      <c r="C143" s="25"/>
+      <c r="C143" s="20"/>
       <c r="E143" t="s">
         <v>629</v>
       </c>
@@ -5420,7 +5433,7 @@
       <c r="A144" t="s">
         <v>641</v>
       </c>
-      <c r="C144" s="25"/>
+      <c r="C144" s="20"/>
       <c r="E144" t="s">
         <v>629</v>
       </c>
@@ -5438,7 +5451,7 @@
       <c r="A145" t="s">
         <v>642</v>
       </c>
-      <c r="C145" s="25"/>
+      <c r="C145" s="20"/>
       <c r="D145" t="s">
         <v>656</v>
       </c>
@@ -5462,7 +5475,7 @@
       <c r="A146" t="s">
         <v>137</v>
       </c>
-      <c r="C146" s="25"/>
+      <c r="C146" s="20"/>
       <c r="D146" t="s">
         <v>503</v>
       </c>
@@ -5483,7 +5496,7 @@
       <c r="A147" t="s">
         <v>138</v>
       </c>
-      <c r="C147" s="25"/>
+      <c r="C147" s="20"/>
       <c r="E147" t="s">
         <v>357</v>
       </c>
@@ -5495,7 +5508,7 @@
       <c r="A148" t="s">
         <v>139</v>
       </c>
-      <c r="C148" s="25"/>
+      <c r="C148" s="20"/>
       <c r="E148" t="s">
         <v>357</v>
       </c>
@@ -5507,7 +5520,7 @@
       <c r="A149" t="s">
         <v>140</v>
       </c>
-      <c r="C149" s="25"/>
+      <c r="C149" s="20"/>
       <c r="D149" t="s">
         <v>504</v>
       </c>
@@ -5528,7 +5541,7 @@
       <c r="A150" t="s">
         <v>141</v>
       </c>
-      <c r="C150" s="25"/>
+      <c r="C150" s="20"/>
       <c r="E150" t="s">
         <v>357</v>
       </c>
@@ -5540,7 +5553,7 @@
       <c r="A151" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C151" s="26"/>
+      <c r="C151" s="21"/>
       <c r="E151" s="6" t="s">
         <v>364</v>
       </c>
@@ -5566,7 +5579,7 @@
       <c r="A153" t="s">
         <v>144</v>
       </c>
-      <c r="C153" s="24" t="s">
+      <c r="C153" s="19" t="s">
         <v>551</v>
       </c>
       <c r="E153" t="s">
@@ -5580,7 +5593,7 @@
       <c r="A154" t="s">
         <v>145</v>
       </c>
-      <c r="C154" s="25"/>
+      <c r="C154" s="20"/>
       <c r="E154" t="s">
         <v>357</v>
       </c>
@@ -5592,7 +5605,7 @@
       <c r="A155" t="s">
         <v>146</v>
       </c>
-      <c r="C155" s="25"/>
+      <c r="C155" s="20"/>
       <c r="E155" t="s">
         <v>357</v>
       </c>
@@ -5604,7 +5617,7 @@
       <c r="A156" t="s">
         <v>147</v>
       </c>
-      <c r="C156" s="25"/>
+      <c r="C156" s="20"/>
       <c r="E156" t="s">
         <v>357</v>
       </c>
@@ -5616,7 +5629,7 @@
       <c r="A157" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C157" s="26"/>
+      <c r="C157" s="21"/>
       <c r="E157" s="6" t="s">
         <v>364</v>
       </c>
@@ -5628,7 +5641,7 @@
       <c r="A158" t="s">
         <v>149</v>
       </c>
-      <c r="C158" s="24" t="s">
+      <c r="C158" s="19" t="s">
         <v>552</v>
       </c>
       <c r="E158" t="s">
@@ -5642,7 +5655,7 @@
       <c r="A159" t="s">
         <v>150</v>
       </c>
-      <c r="C159" s="25"/>
+      <c r="C159" s="20"/>
       <c r="E159" t="s">
         <v>357</v>
       </c>
@@ -5654,7 +5667,7 @@
       <c r="A160" t="s">
         <v>151</v>
       </c>
-      <c r="C160" s="25"/>
+      <c r="C160" s="20"/>
       <c r="E160" t="s">
         <v>357</v>
       </c>
@@ -5669,7 +5682,7 @@
       <c r="A161" t="s">
         <v>152</v>
       </c>
-      <c r="C161" s="25"/>
+      <c r="C161" s="20"/>
       <c r="E161" t="s">
         <v>357</v>
       </c>
@@ -5684,7 +5697,7 @@
       <c r="A162" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C162" s="26"/>
+      <c r="C162" s="21"/>
       <c r="E162" s="6" t="s">
         <v>364</v>
       </c>
@@ -5696,7 +5709,7 @@
       <c r="A163" t="s">
         <v>154</v>
       </c>
-      <c r="C163" s="24" t="s">
+      <c r="C163" s="19" t="s">
         <v>553</v>
       </c>
       <c r="D163" t="s">
@@ -5719,7 +5732,7 @@
       <c r="A164" t="s">
         <v>155</v>
       </c>
-      <c r="C164" s="25"/>
+      <c r="C164" s="20"/>
       <c r="E164" t="s">
         <v>357</v>
       </c>
@@ -5731,26 +5744,26 @@
       <c r="A165" t="s">
         <v>156</v>
       </c>
-      <c r="C165" s="25"/>
+      <c r="C165" s="20"/>
       <c r="E165" t="s">
         <v>357</v>
       </c>
       <c r="F165" t="s">
         <v>522</v>
       </c>
-      <c r="I165" s="27" t="s">
+      <c r="I165" s="18" t="s">
         <v>601</v>
       </c>
-      <c r="J165" s="27"/>
-      <c r="K165" s="27"/>
-      <c r="L165" s="27"/>
-      <c r="M165" s="27"/>
+      <c r="J165" s="18"/>
+      <c r="K165" s="18"/>
+      <c r="L165" s="18"/>
+      <c r="M165" s="18"/>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
         <v>157</v>
       </c>
-      <c r="C166" s="25"/>
+      <c r="C166" s="20"/>
       <c r="D166" t="s">
         <v>511</v>
       </c>
@@ -5766,51 +5779,51 @@
       <c r="H166" t="s">
         <v>634</v>
       </c>
-      <c r="I166" s="27"/>
-      <c r="J166" s="27"/>
-      <c r="K166" s="27"/>
-      <c r="L166" s="27"/>
-      <c r="M166" s="27"/>
+      <c r="I166" s="18"/>
+      <c r="J166" s="18"/>
+      <c r="K166" s="18"/>
+      <c r="L166" s="18"/>
+      <c r="M166" s="18"/>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="s">
         <v>158</v>
       </c>
-      <c r="C167" s="25"/>
+      <c r="C167" s="20"/>
       <c r="E167" t="s">
         <v>357</v>
       </c>
       <c r="F167" t="s">
         <v>492</v>
       </c>
-      <c r="I167" s="27"/>
-      <c r="J167" s="27"/>
-      <c r="K167" s="27"/>
-      <c r="L167" s="27"/>
-      <c r="M167" s="27"/>
+      <c r="I167" s="18"/>
+      <c r="J167" s="18"/>
+      <c r="K167" s="18"/>
+      <c r="L167" s="18"/>
+      <c r="M167" s="18"/>
     </row>
     <row r="168" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C168" s="26"/>
+      <c r="C168" s="21"/>
       <c r="E168" s="6" t="s">
         <v>364</v>
       </c>
       <c r="F168" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="I168" s="27"/>
-      <c r="J168" s="27"/>
-      <c r="K168" s="27"/>
-      <c r="L168" s="27"/>
-      <c r="M168" s="27"/>
+      <c r="I168" s="18"/>
+      <c r="J168" s="18"/>
+      <c r="K168" s="18"/>
+      <c r="L168" s="18"/>
+      <c r="M168" s="18"/>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
         <v>160</v>
       </c>
-      <c r="C169" s="24" t="s">
+      <c r="C169" s="19" t="s">
         <v>555</v>
       </c>
       <c r="E169" t="s">
@@ -5827,7 +5840,7 @@
       <c r="A170" t="s">
         <v>161</v>
       </c>
-      <c r="C170" s="25"/>
+      <c r="C170" s="20"/>
       <c r="D170" t="s">
         <v>520</v>
       </c>
@@ -5848,7 +5861,7 @@
       <c r="A171" t="s">
         <v>620</v>
       </c>
-      <c r="C171" s="25"/>
+      <c r="C171" s="20"/>
       <c r="E171" t="s">
         <v>623</v>
       </c>
@@ -5866,7 +5879,7 @@
       <c r="A172" t="s">
         <v>621</v>
       </c>
-      <c r="C172" s="25"/>
+      <c r="C172" s="20"/>
       <c r="E172" t="s">
         <v>623</v>
       </c>
@@ -5884,7 +5897,7 @@
       <c r="A173" t="s">
         <v>625</v>
       </c>
-      <c r="C173" s="25"/>
+      <c r="C173" s="20"/>
       <c r="E173" t="s">
         <v>629</v>
       </c>
@@ -5902,7 +5915,7 @@
       <c r="A174" t="s">
         <v>626</v>
       </c>
-      <c r="C174" s="25"/>
+      <c r="C174" s="20"/>
       <c r="E174" t="s">
         <v>629</v>
       </c>
@@ -5920,7 +5933,7 @@
       <c r="A175" t="s">
         <v>627</v>
       </c>
-      <c r="C175" s="25"/>
+      <c r="C175" s="20"/>
       <c r="E175" t="s">
         <v>629</v>
       </c>
@@ -5938,7 +5951,7 @@
       <c r="A176" t="s">
         <v>628</v>
       </c>
-      <c r="C176" s="25"/>
+      <c r="C176" s="20"/>
       <c r="D176" t="s">
         <v>657</v>
       </c>
@@ -5962,7 +5975,7 @@
       <c r="A177" t="s">
         <v>162</v>
       </c>
-      <c r="C177" s="25"/>
+      <c r="C177" s="20"/>
       <c r="D177" t="s">
         <v>521</v>
       </c>
@@ -5983,7 +5996,7 @@
       <c r="A178" t="s">
         <v>163</v>
       </c>
-      <c r="C178" s="25"/>
+      <c r="C178" s="20"/>
       <c r="E178" t="s">
         <v>357</v>
       </c>
@@ -5995,7 +6008,7 @@
       <c r="A179" t="s">
         <v>164</v>
       </c>
-      <c r="C179" s="25"/>
+      <c r="C179" s="20"/>
       <c r="E179" t="s">
         <v>357</v>
       </c>
@@ -6007,7 +6020,7 @@
       <c r="A180" t="s">
         <v>165</v>
       </c>
-      <c r="C180" s="25"/>
+      <c r="C180" s="20"/>
       <c r="E180" t="s">
         <v>357</v>
       </c>
@@ -6019,7 +6032,7 @@
       <c r="A181" t="s">
         <v>166</v>
       </c>
-      <c r="C181" s="25"/>
+      <c r="C181" s="20"/>
       <c r="E181" t="s">
         <v>357</v>
       </c>
@@ -6031,7 +6044,7 @@
       <c r="A182" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C182" s="26"/>
+      <c r="C182" s="21"/>
       <c r="E182" s="6" t="s">
         <v>364</v>
       </c>
@@ -6043,7 +6056,7 @@
       <c r="A183" t="s">
         <v>168</v>
       </c>
-      <c r="C183" s="24" t="s">
+      <c r="C183" s="19" t="s">
         <v>556</v>
       </c>
       <c r="E183" t="s">
@@ -6057,7 +6070,7 @@
       <c r="A184" t="s">
         <v>169</v>
       </c>
-      <c r="C184" s="25"/>
+      <c r="C184" s="20"/>
       <c r="E184" t="s">
         <v>357</v>
       </c>
@@ -6069,7 +6082,7 @@
       <c r="A185" t="s">
         <v>170</v>
       </c>
-      <c r="C185" s="25"/>
+      <c r="C185" s="20"/>
       <c r="D185" t="s">
         <v>524</v>
       </c>
@@ -6090,7 +6103,7 @@
       <c r="A186" t="s">
         <v>171</v>
       </c>
-      <c r="C186" s="25"/>
+      <c r="C186" s="20"/>
       <c r="E186" t="s">
         <v>357</v>
       </c>
@@ -6102,7 +6115,7 @@
       <c r="A187" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C187" s="26"/>
+      <c r="C187" s="21"/>
       <c r="E187" s="6" t="s">
         <v>364</v>
       </c>
@@ -6114,7 +6127,7 @@
       <c r="A188" t="s">
         <v>173</v>
       </c>
-      <c r="C188" s="24" t="s">
+      <c r="C188" s="19" t="s">
         <v>557</v>
       </c>
       <c r="E188" t="s">
@@ -6128,7 +6141,7 @@
       <c r="A189" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C189" s="26"/>
+      <c r="C189" s="21"/>
       <c r="D189" s="6" t="s">
         <v>530</v>
       </c>
@@ -6149,7 +6162,7 @@
       <c r="A190" t="s">
         <v>175</v>
       </c>
-      <c r="C190" s="24" t="s">
+      <c r="C190" s="19" t="s">
         <v>558</v>
       </c>
       <c r="E190" t="s">
@@ -6163,7 +6176,7 @@
       <c r="A191" t="s">
         <v>176</v>
       </c>
-      <c r="C191" s="25"/>
+      <c r="C191" s="20"/>
       <c r="E191" t="s">
         <v>357</v>
       </c>
@@ -6175,7 +6188,7 @@
       <c r="A192" t="s">
         <v>177</v>
       </c>
-      <c r="C192" s="25"/>
+      <c r="C192" s="20"/>
       <c r="E192" t="s">
         <v>357</v>
       </c>
@@ -6187,7 +6200,7 @@
       <c r="A193" t="s">
         <v>178</v>
       </c>
-      <c r="C193" s="25"/>
+      <c r="C193" s="20"/>
       <c r="E193" t="s">
         <v>357</v>
       </c>
@@ -6199,7 +6212,7 @@
       <c r="A194" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C194" s="26"/>
+      <c r="C194" s="21"/>
       <c r="E194" s="6" t="s">
         <v>364</v>
       </c>
@@ -6211,7 +6224,7 @@
       <c r="A195" t="s">
         <v>180</v>
       </c>
-      <c r="C195" s="24" t="s">
+      <c r="C195" s="19" t="s">
         <v>559</v>
       </c>
       <c r="E195" t="s">
@@ -6225,7 +6238,7 @@
       <c r="A196" t="s">
         <v>181</v>
       </c>
-      <c r="C196" s="25"/>
+      <c r="C196" s="20"/>
       <c r="E196" t="s">
         <v>357</v>
       </c>
@@ -6237,7 +6250,7 @@
       <c r="A197" t="s">
         <v>182</v>
       </c>
-      <c r="C197" s="25"/>
+      <c r="C197" s="20"/>
       <c r="D197" t="s">
         <v>596</v>
       </c>
@@ -6258,7 +6271,7 @@
       <c r="A198" t="s">
         <v>183</v>
       </c>
-      <c r="C198" s="25"/>
+      <c r="C198" s="20"/>
       <c r="E198" t="s">
         <v>357</v>
       </c>
@@ -6270,7 +6283,7 @@
       <c r="A199" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C199" s="26"/>
+      <c r="C199" s="21"/>
       <c r="E199" s="6" t="s">
         <v>364</v>
       </c>
@@ -6282,7 +6295,7 @@
       <c r="A200" t="s">
         <v>185</v>
       </c>
-      <c r="C200" s="24" t="s">
+      <c r="C200" s="19" t="s">
         <v>560</v>
       </c>
       <c r="E200" t="s">
@@ -6296,7 +6309,7 @@
       <c r="A201" t="s">
         <v>186</v>
       </c>
-      <c r="C201" s="25"/>
+      <c r="C201" s="20"/>
       <c r="E201" t="s">
         <v>357</v>
       </c>
@@ -6308,7 +6321,7 @@
       <c r="A202" t="s">
         <v>187</v>
       </c>
-      <c r="C202" s="25"/>
+      <c r="C202" s="20"/>
       <c r="D202" t="s">
         <v>595</v>
       </c>
@@ -6329,7 +6342,7 @@
       <c r="A203" t="s">
         <v>188</v>
       </c>
-      <c r="C203" s="25"/>
+      <c r="C203" s="20"/>
       <c r="E203" t="s">
         <v>357</v>
       </c>
@@ -6341,7 +6354,7 @@
       <c r="A204" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C204" s="26"/>
+      <c r="C204" s="21"/>
       <c r="E204" s="6" t="s">
         <v>364</v>
       </c>
@@ -6353,7 +6366,7 @@
       <c r="A205" t="s">
         <v>190</v>
       </c>
-      <c r="C205" s="24" t="s">
+      <c r="C205" s="19" t="s">
         <v>563</v>
       </c>
       <c r="E205" t="s">
@@ -6367,7 +6380,7 @@
       <c r="A206" t="s">
         <v>191</v>
       </c>
-      <c r="C206" s="25"/>
+      <c r="C206" s="20"/>
       <c r="E206" t="s">
         <v>357</v>
       </c>
@@ -6379,7 +6392,7 @@
       <c r="A207" t="s">
         <v>192</v>
       </c>
-      <c r="C207" s="25"/>
+      <c r="C207" s="20"/>
       <c r="D207" t="s">
         <v>600</v>
       </c>
@@ -6400,7 +6413,7 @@
       <c r="A208" t="s">
         <v>193</v>
       </c>
-      <c r="C208" s="25"/>
+      <c r="C208" s="20"/>
       <c r="E208" t="s">
         <v>357</v>
       </c>
@@ -6412,7 +6425,7 @@
       <c r="A209" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C209" s="26"/>
+      <c r="C209" s="21"/>
       <c r="E209" s="6" t="s">
         <v>364</v>
       </c>
@@ -6424,7 +6437,7 @@
       <c r="A210" t="s">
         <v>195</v>
       </c>
-      <c r="C210" s="24" t="s">
+      <c r="C210" s="19" t="s">
         <v>561</v>
       </c>
       <c r="D210" t="s">
@@ -6450,7 +6463,7 @@
       <c r="A211" t="s">
         <v>196</v>
       </c>
-      <c r="C211" s="25"/>
+      <c r="C211" s="20"/>
       <c r="D211" t="s">
         <v>609</v>
       </c>
@@ -6471,7 +6484,7 @@
       <c r="A212" t="s">
         <v>197</v>
       </c>
-      <c r="C212" s="25"/>
+      <c r="C212" s="20"/>
       <c r="D212" t="s">
         <v>610</v>
       </c>
@@ -6489,7 +6502,7 @@
       <c r="A213" t="s">
         <v>198</v>
       </c>
-      <c r="C213" s="25"/>
+      <c r="C213" s="20"/>
       <c r="D213" t="s">
         <v>611</v>
       </c>
@@ -6510,7 +6523,7 @@
       <c r="A214" t="s">
         <v>643</v>
       </c>
-      <c r="C214" s="25"/>
+      <c r="C214" s="20"/>
       <c r="E214" t="s">
         <v>623</v>
       </c>
@@ -6525,7 +6538,7 @@
       <c r="A215" t="s">
         <v>644</v>
       </c>
-      <c r="C215" s="25"/>
+      <c r="C215" s="20"/>
       <c r="E215" t="s">
         <v>623</v>
       </c>
@@ -6540,7 +6553,7 @@
       <c r="A216" t="s">
         <v>645</v>
       </c>
-      <c r="C216" s="25"/>
+      <c r="C216" s="20"/>
       <c r="E216" t="s">
         <v>629</v>
       </c>
@@ -6555,7 +6568,7 @@
       <c r="A217" t="s">
         <v>646</v>
       </c>
-      <c r="C217" s="25"/>
+      <c r="C217" s="20"/>
       <c r="E217" t="s">
         <v>629</v>
       </c>
@@ -6570,7 +6583,7 @@
       <c r="A218" t="s">
         <v>647</v>
       </c>
-      <c r="C218" s="25"/>
+      <c r="C218" s="20"/>
       <c r="E218" t="s">
         <v>629</v>
       </c>
@@ -6585,7 +6598,7 @@
       <c r="A219" t="s">
         <v>648</v>
       </c>
-      <c r="C219" s="25"/>
+      <c r="C219" s="20"/>
       <c r="D219" t="s">
         <v>658</v>
       </c>
@@ -6606,7 +6619,7 @@
       <c r="A220" t="s">
         <v>199</v>
       </c>
-      <c r="C220" s="25"/>
+      <c r="C220" s="20"/>
       <c r="E220" t="s">
         <v>612</v>
       </c>
@@ -6618,7 +6631,7 @@
       <c r="A221" t="s">
         <v>200</v>
       </c>
-      <c r="C221" s="25"/>
+      <c r="C221" s="20"/>
       <c r="D221" t="s">
         <v>614</v>
       </c>
@@ -6636,7 +6649,7 @@
       <c r="A222" t="s">
         <v>201</v>
       </c>
-      <c r="C222" s="25"/>
+      <c r="C222" s="20"/>
       <c r="E222" t="s">
         <v>357</v>
       </c>
@@ -6648,7 +6661,7 @@
       <c r="A223" t="s">
         <v>202</v>
       </c>
-      <c r="C223" s="25"/>
+      <c r="C223" s="20"/>
       <c r="D223" t="s">
         <v>665</v>
       </c>
@@ -6672,7 +6685,7 @@
       <c r="A224" t="s">
         <v>203</v>
       </c>
-      <c r="C224" s="25"/>
+      <c r="C224" s="20"/>
       <c r="E224" t="s">
         <v>357</v>
       </c>
@@ -6684,7 +6697,7 @@
       <c r="A225" t="s">
         <v>204</v>
       </c>
-      <c r="C225" s="25"/>
+      <c r="C225" s="20"/>
       <c r="E225" t="s">
         <v>357</v>
       </c>
@@ -6696,7 +6709,7 @@
       <c r="A226" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C226" s="26"/>
+      <c r="C226" s="21"/>
       <c r="E226" s="6" t="s">
         <v>364</v>
       </c>
@@ -6708,7 +6721,7 @@
       <c r="A227" t="s">
         <v>206</v>
       </c>
-      <c r="C227" s="24" t="s">
+      <c r="C227" s="19" t="s">
         <v>562</v>
       </c>
       <c r="E227" t="s">
@@ -6722,7 +6735,7 @@
       <c r="A228" t="s">
         <v>207</v>
       </c>
-      <c r="C228" s="25"/>
+      <c r="C228" s="20"/>
       <c r="D228" t="s">
         <v>617</v>
       </c>
@@ -6740,7 +6753,7 @@
       <c r="A229" t="s">
         <v>650</v>
       </c>
-      <c r="C229" s="25"/>
+      <c r="C229" s="20"/>
       <c r="E229" t="s">
         <v>623</v>
       </c>
@@ -6755,7 +6768,7 @@
       <c r="A230" t="s">
         <v>651</v>
       </c>
-      <c r="C230" s="25"/>
+      <c r="C230" s="20"/>
       <c r="E230" t="s">
         <v>623</v>
       </c>
@@ -6770,7 +6783,7 @@
       <c r="A231" t="s">
         <v>652</v>
       </c>
-      <c r="C231" s="25"/>
+      <c r="C231" s="20"/>
       <c r="E231" t="s">
         <v>629</v>
       </c>
@@ -6785,7 +6798,7 @@
       <c r="A232" t="s">
         <v>653</v>
       </c>
-      <c r="C232" s="25"/>
+      <c r="C232" s="20"/>
       <c r="E232" t="s">
         <v>629</v>
       </c>
@@ -6800,7 +6813,7 @@
       <c r="A233" t="s">
         <v>654</v>
       </c>
-      <c r="C233" s="25"/>
+      <c r="C233" s="20"/>
       <c r="E233" t="s">
         <v>629</v>
       </c>
@@ -6815,7 +6828,7 @@
       <c r="A234" t="s">
         <v>655</v>
       </c>
-      <c r="C234" s="25"/>
+      <c r="C234" s="20"/>
       <c r="D234" t="s">
         <v>659</v>
       </c>
@@ -6836,7 +6849,7 @@
       <c r="A235" t="s">
         <v>208</v>
       </c>
-      <c r="C235" s="25"/>
+      <c r="C235" s="20"/>
       <c r="D235" t="s">
         <v>616</v>
       </c>
@@ -6854,7 +6867,7 @@
       <c r="A236" t="s">
         <v>209</v>
       </c>
-      <c r="C236" s="25"/>
+      <c r="C236" s="20"/>
       <c r="E236" t="s">
         <v>357</v>
       </c>
@@ -6866,7 +6879,7 @@
       <c r="A237" t="s">
         <v>210</v>
       </c>
-      <c r="C237" s="25"/>
+      <c r="C237" s="20"/>
       <c r="E237" t="s">
         <v>357</v>
       </c>
@@ -6878,7 +6891,7 @@
       <c r="A238" t="s">
         <v>211</v>
       </c>
-      <c r="C238" s="25"/>
+      <c r="C238" s="20"/>
       <c r="D238" t="s">
         <v>664</v>
       </c>
@@ -6899,7 +6912,7 @@
       <c r="A239" t="s">
         <v>212</v>
       </c>
-      <c r="C239" s="25"/>
+      <c r="C239" s="20"/>
       <c r="E239" t="s">
         <v>357</v>
       </c>
@@ -6911,7 +6924,7 @@
       <c r="A240" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="C240" s="26"/>
+      <c r="C240" s="21"/>
       <c r="E240" s="6" t="s">
         <v>364</v>
       </c>
@@ -6923,7 +6936,7 @@
       <c r="A241" t="s">
         <v>214</v>
       </c>
-      <c r="C241" s="24" t="s">
+      <c r="C241" s="19" t="s">
         <v>564</v>
       </c>
       <c r="E241" t="s">
@@ -6937,7 +6950,7 @@
       <c r="A242" t="s">
         <v>215</v>
       </c>
-      <c r="C242" s="25"/>
+      <c r="C242" s="20"/>
       <c r="E242" t="s">
         <v>357</v>
       </c>
@@ -6949,7 +6962,7 @@
       <c r="A243" t="s">
         <v>216</v>
       </c>
-      <c r="C243" s="25"/>
+      <c r="C243" s="20"/>
       <c r="D243" t="s">
         <v>669</v>
       </c>
@@ -6970,7 +6983,7 @@
       <c r="A244" t="s">
         <v>217</v>
       </c>
-      <c r="C244" s="25"/>
+      <c r="C244" s="20"/>
       <c r="E244" t="s">
         <v>357</v>
       </c>
@@ -6982,7 +6995,7 @@
       <c r="A245" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C245" s="26"/>
+      <c r="C245" s="21"/>
       <c r="E245" s="6" t="s">
         <v>364</v>
       </c>
@@ -6994,7 +7007,7 @@
       <c r="A246" t="s">
         <v>219</v>
       </c>
-      <c r="C246" s="24" t="s">
+      <c r="C246" s="19" t="s">
         <v>565</v>
       </c>
       <c r="E246" t="s">
@@ -7008,7 +7021,7 @@
       <c r="A247" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C247" s="26"/>
+      <c r="C247" s="21"/>
       <c r="E247" s="6" t="s">
         <v>379</v>
       </c>
@@ -7023,7 +7036,7 @@
       <c r="A248" t="s">
         <v>221</v>
       </c>
-      <c r="C248" s="24" t="s">
+      <c r="C248" s="19" t="s">
         <v>566</v>
       </c>
       <c r="E248" t="s">
@@ -7037,7 +7050,7 @@
       <c r="A249" t="s">
         <v>222</v>
       </c>
-      <c r="C249" s="25"/>
+      <c r="C249" s="20"/>
       <c r="E249" t="s">
         <v>357</v>
       </c>
@@ -7049,7 +7062,7 @@
       <c r="A250" t="s">
         <v>223</v>
       </c>
-      <c r="C250" s="25"/>
+      <c r="C250" s="20"/>
       <c r="E250" t="s">
         <v>357</v>
       </c>
@@ -7061,7 +7074,7 @@
       <c r="A251" t="s">
         <v>224</v>
       </c>
-      <c r="C251" s="25"/>
+      <c r="C251" s="20"/>
       <c r="E251" t="s">
         <v>357</v>
       </c>
@@ -7073,7 +7086,7 @@
       <c r="A252" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="C252" s="28"/>
+      <c r="C252" s="22"/>
       <c r="E252" s="12" t="s">
         <v>364</v>
       </c>
@@ -7085,7 +7098,7 @@
       <c r="A253" t="s">
         <v>226</v>
       </c>
-      <c r="C253" s="25" t="s">
+      <c r="C253" s="20" t="s">
         <v>567</v>
       </c>
       <c r="D253" t="s">
@@ -7105,7 +7118,7 @@
       <c r="A254" t="s">
         <v>227</v>
       </c>
-      <c r="C254" s="25"/>
+      <c r="C254" s="20"/>
       <c r="D254" t="s">
         <v>683</v>
       </c>
@@ -7123,7 +7136,7 @@
       <c r="A255" t="s">
         <v>228</v>
       </c>
-      <c r="C255" s="25"/>
+      <c r="C255" s="20"/>
       <c r="E255" t="s">
         <v>357</v>
       </c>
@@ -7135,7 +7148,7 @@
       <c r="A256" t="s">
         <v>229</v>
       </c>
-      <c r="C256" s="25"/>
+      <c r="C256" s="20"/>
       <c r="D256" t="s">
         <v>682</v>
       </c>
@@ -7156,7 +7169,7 @@
       <c r="A257" t="s">
         <v>230</v>
       </c>
-      <c r="C257" s="25"/>
+      <c r="C257" s="20"/>
       <c r="E257" t="s">
         <v>357</v>
       </c>
@@ -7168,7 +7181,7 @@
       <c r="A258" t="s">
         <v>231</v>
       </c>
-      <c r="C258" s="25"/>
+      <c r="C258" s="20"/>
       <c r="E258" t="s">
         <v>357</v>
       </c>
@@ -7180,7 +7193,7 @@
       <c r="A259" t="s">
         <v>232</v>
       </c>
-      <c r="C259" s="25"/>
+      <c r="C259" s="20"/>
       <c r="E259" t="s">
         <v>364</v>
       </c>
@@ -7192,7 +7205,7 @@
       <c r="A260" t="s">
         <v>233</v>
       </c>
-      <c r="C260" s="25"/>
+      <c r="C260" s="20"/>
       <c r="D260" t="s">
         <v>684</v>
       </c>
@@ -7213,7 +7226,7 @@
       <c r="A261" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C261" s="25"/>
+      <c r="C261" s="20"/>
       <c r="D261" s="6" t="s">
         <v>687</v>
       </c>
@@ -7231,7 +7244,7 @@
       <c r="A262" t="s">
         <v>235</v>
       </c>
-      <c r="C262" s="25" t="s">
+      <c r="C262" s="20" t="s">
         <v>569</v>
       </c>
       <c r="D262" t="s">
@@ -7249,17 +7262,17 @@
       <c r="H262" t="s">
         <v>636</v>
       </c>
-      <c r="I262" s="19" t="s">
+      <c r="I262" s="23" t="s">
         <v>704</v>
       </c>
-      <c r="J262" s="19"/>
-      <c r="K262" s="19"/>
+      <c r="J262" s="23"/>
+      <c r="K262" s="23"/>
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" t="s">
         <v>236</v>
       </c>
-      <c r="C263" s="25"/>
+      <c r="C263" s="20"/>
       <c r="D263" t="s">
         <v>694</v>
       </c>
@@ -7272,15 +7285,15 @@
       <c r="H263" t="s">
         <v>636</v>
       </c>
-      <c r="I263" s="19"/>
-      <c r="J263" s="19"/>
-      <c r="K263" s="19"/>
+      <c r="I263" s="23"/>
+      <c r="J263" s="23"/>
+      <c r="K263" s="23"/>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" t="s">
         <v>237</v>
       </c>
-      <c r="C264" s="25"/>
+      <c r="C264" s="20"/>
       <c r="D264" t="s">
         <v>698</v>
       </c>
@@ -7293,15 +7306,15 @@
       <c r="H264" t="s">
         <v>636</v>
       </c>
-      <c r="I264" s="19"/>
-      <c r="J264" s="19"/>
-      <c r="K264" s="19"/>
+      <c r="I264" s="23"/>
+      <c r="J264" s="23"/>
+      <c r="K264" s="23"/>
     </row>
     <row r="265" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" t="s">
         <v>238</v>
       </c>
-      <c r="C265" s="25"/>
+      <c r="C265" s="20"/>
       <c r="D265" t="s">
         <v>697</v>
       </c>
@@ -7311,15 +7324,15 @@
       <c r="F265" t="s">
         <v>674</v>
       </c>
-      <c r="I265" s="19"/>
-      <c r="J265" s="19"/>
-      <c r="K265" s="19"/>
+      <c r="I265" s="23"/>
+      <c r="J265" s="23"/>
+      <c r="K265" s="23"/>
     </row>
     <row r="266" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" t="s">
         <v>239</v>
       </c>
-      <c r="C266" s="25"/>
+      <c r="C266" s="20"/>
       <c r="E266" t="s">
         <v>357</v>
       </c>
@@ -7337,7 +7350,7 @@
       <c r="A267" t="s">
         <v>240</v>
       </c>
-      <c r="C267" s="25"/>
+      <c r="C267" s="20"/>
       <c r="E267" t="s">
         <v>357</v>
       </c>
@@ -7349,7 +7362,7 @@
       <c r="A268" t="s">
         <v>241</v>
       </c>
-      <c r="C268" s="25"/>
+      <c r="C268" s="20"/>
       <c r="E268" t="s">
         <v>357</v>
       </c>
@@ -7361,7 +7374,7 @@
       <c r="A269" t="s">
         <v>242</v>
       </c>
-      <c r="C269" s="25"/>
+      <c r="C269" s="20"/>
       <c r="E269" t="s">
         <v>364</v>
       </c>
@@ -7373,7 +7386,7 @@
       <c r="A270" t="s">
         <v>243</v>
       </c>
-      <c r="C270" s="25"/>
+      <c r="C270" s="20"/>
       <c r="D270" t="s">
         <v>699</v>
       </c>
@@ -7391,7 +7404,7 @@
       <c r="A271" t="s">
         <v>244</v>
       </c>
-      <c r="C271" s="25"/>
+      <c r="C271" s="20"/>
       <c r="D271" t="s">
         <v>701</v>
       </c>
@@ -7409,7 +7422,7 @@
       <c r="A272" t="s">
         <v>245</v>
       </c>
-      <c r="C272" s="25"/>
+      <c r="C272" s="20"/>
       <c r="D272" t="s">
         <v>695</v>
       </c>
@@ -7427,7 +7440,7 @@
       <c r="A273" t="s">
         <v>246</v>
       </c>
-      <c r="C273" s="25"/>
+      <c r="C273" s="20"/>
       <c r="D273" t="s">
         <v>708</v>
       </c>
@@ -7448,7 +7461,7 @@
       <c r="A274" t="s">
         <v>247</v>
       </c>
-      <c r="C274" s="25"/>
+      <c r="C274" s="20"/>
       <c r="E274" t="s">
         <v>357</v>
       </c>
@@ -7460,7 +7473,7 @@
       <c r="A275" t="s">
         <v>248</v>
       </c>
-      <c r="C275" s="25"/>
+      <c r="C275" s="20"/>
       <c r="D275" t="s">
         <v>696</v>
       </c>
@@ -7481,7 +7494,7 @@
       <c r="A276" t="s">
         <v>249</v>
       </c>
-      <c r="C276" s="25"/>
+      <c r="C276" s="20"/>
       <c r="E276" t="s">
         <v>357</v>
       </c>
@@ -7493,7 +7506,7 @@
       <c r="A277" t="s">
         <v>250</v>
       </c>
-      <c r="C277" s="25"/>
+      <c r="C277" s="20"/>
       <c r="E277" t="s">
         <v>357</v>
       </c>
@@ -7505,7 +7518,7 @@
       <c r="A278" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="C278" s="26"/>
+      <c r="C278" s="21"/>
       <c r="E278" s="6" t="s">
         <v>364</v>
       </c>
@@ -7537,7 +7550,7 @@
       <c r="A280" t="s">
         <v>253</v>
       </c>
-      <c r="C280" s="24" t="s">
+      <c r="C280" s="19" t="s">
         <v>571</v>
       </c>
       <c r="D280" t="s">
@@ -7557,7 +7570,7 @@
       <c r="A281" t="s">
         <v>254</v>
       </c>
-      <c r="C281" s="25"/>
+      <c r="C281" s="20"/>
       <c r="D281" t="s">
         <v>715</v>
       </c>
@@ -7575,7 +7588,7 @@
       <c r="A282" t="s">
         <v>255</v>
       </c>
-      <c r="C282" s="25"/>
+      <c r="C282" s="20"/>
       <c r="E282" t="s">
         <v>357</v>
       </c>
@@ -7587,7 +7600,7 @@
       <c r="A283" t="s">
         <v>256</v>
       </c>
-      <c r="C283" s="25"/>
+      <c r="C283" s="20"/>
       <c r="D283" t="s">
         <v>716</v>
       </c>
@@ -7608,7 +7621,7 @@
       <c r="A284" t="s">
         <v>257</v>
       </c>
-      <c r="C284" s="25"/>
+      <c r="C284" s="20"/>
       <c r="E284" t="s">
         <v>357</v>
       </c>
@@ -7620,7 +7633,7 @@
       <c r="A285" t="s">
         <v>258</v>
       </c>
-      <c r="C285" s="25"/>
+      <c r="C285" s="20"/>
       <c r="E285" t="s">
         <v>357</v>
       </c>
@@ -7632,7 +7645,7 @@
       <c r="A286" t="s">
         <v>259</v>
       </c>
-      <c r="C286" s="25"/>
+      <c r="C286" s="20"/>
       <c r="E286" t="s">
         <v>364</v>
       </c>
@@ -7644,7 +7657,7 @@
       <c r="A287" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C287" s="26"/>
+      <c r="C287" s="21"/>
       <c r="D287" s="6" t="s">
         <v>717</v>
       </c>
@@ -7662,7 +7675,7 @@
       <c r="A288" t="s">
         <v>261</v>
       </c>
-      <c r="C288" s="24" t="s">
+      <c r="C288" s="19" t="s">
         <v>572</v>
       </c>
       <c r="D288" t="s">
@@ -7685,7 +7698,7 @@
       <c r="A289" t="s">
         <v>262</v>
       </c>
-      <c r="C289" s="25"/>
+      <c r="C289" s="20"/>
       <c r="D289" t="s">
         <v>721</v>
       </c>
@@ -7703,7 +7716,7 @@
       <c r="A290" t="s">
         <v>263</v>
       </c>
-      <c r="C290" s="25"/>
+      <c r="C290" s="20"/>
       <c r="D290" t="s">
         <v>722</v>
       </c>
@@ -7721,7 +7734,7 @@
       <c r="A291" t="s">
         <v>264</v>
       </c>
-      <c r="C291" s="25"/>
+      <c r="C291" s="20"/>
       <c r="D291" t="s">
         <v>723</v>
       </c>
@@ -7736,7 +7749,7 @@
       <c r="A292" t="s">
         <v>265</v>
       </c>
-      <c r="C292" s="25"/>
+      <c r="C292" s="20"/>
       <c r="E292" t="s">
         <v>357</v>
       </c>
@@ -7754,7 +7767,7 @@
       <c r="A293" t="s">
         <v>266</v>
       </c>
-      <c r="C293" s="25"/>
+      <c r="C293" s="20"/>
       <c r="E293" t="s">
         <v>357</v>
       </c>
@@ -7766,7 +7779,7 @@
       <c r="A294" t="s">
         <v>267</v>
       </c>
-      <c r="C294" s="25"/>
+      <c r="C294" s="20"/>
       <c r="E294" t="s">
         <v>357</v>
       </c>
@@ -7778,7 +7791,7 @@
       <c r="A295" t="s">
         <v>268</v>
       </c>
-      <c r="C295" s="25"/>
+      <c r="C295" s="20"/>
       <c r="E295" t="s">
         <v>364</v>
       </c>
@@ -7790,7 +7803,7 @@
       <c r="A296" t="s">
         <v>269</v>
       </c>
-      <c r="C296" s="25"/>
+      <c r="C296" s="20"/>
       <c r="D296" t="s">
         <v>724</v>
       </c>
@@ -7808,7 +7821,7 @@
       <c r="A297" t="s">
         <v>270</v>
       </c>
-      <c r="C297" s="25"/>
+      <c r="C297" s="20"/>
       <c r="D297" t="s">
         <v>727</v>
       </c>
@@ -7826,7 +7839,7 @@
       <c r="A298" t="s">
         <v>271</v>
       </c>
-      <c r="C298" s="25"/>
+      <c r="C298" s="20"/>
       <c r="D298" t="s">
         <v>728</v>
       </c>
@@ -7844,7 +7857,7 @@
       <c r="A299" t="s">
         <v>272</v>
       </c>
-      <c r="C299" s="25"/>
+      <c r="C299" s="20"/>
       <c r="E299" t="s">
         <v>357</v>
       </c>
@@ -7856,7 +7869,7 @@
       <c r="A300" t="s">
         <v>273</v>
       </c>
-      <c r="C300" s="25"/>
+      <c r="C300" s="20"/>
       <c r="D300" t="s">
         <v>729</v>
       </c>
@@ -7877,7 +7890,7 @@
       <c r="A301" t="s">
         <v>274</v>
       </c>
-      <c r="C301" s="25"/>
+      <c r="C301" s="20"/>
       <c r="E301" t="s">
         <v>357</v>
       </c>
@@ -7889,7 +7902,7 @@
       <c r="A302" t="s">
         <v>275</v>
       </c>
-      <c r="C302" s="25"/>
+      <c r="C302" s="20"/>
       <c r="E302" t="s">
         <v>357</v>
       </c>
@@ -7901,7 +7914,7 @@
       <c r="A303" t="s">
         <v>276</v>
       </c>
-      <c r="C303" s="25"/>
+      <c r="C303" s="20"/>
       <c r="E303" t="s">
         <v>364</v>
       </c>
@@ -7913,7 +7926,7 @@
       <c r="A304" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C304" s="26"/>
+      <c r="C304" s="21"/>
       <c r="D304" s="6" t="s">
         <v>730</v>
       </c>
@@ -7934,7 +7947,7 @@
       <c r="A305" t="s">
         <v>278</v>
       </c>
-      <c r="C305" s="24" t="s">
+      <c r="C305" s="19" t="s">
         <v>573</v>
       </c>
       <c r="E305" t="s">
@@ -7948,7 +7961,7 @@
       <c r="A306" t="s">
         <v>279</v>
       </c>
-      <c r="C306" s="25"/>
+      <c r="C306" s="20"/>
       <c r="E306" t="s">
         <v>357</v>
       </c>
@@ -7960,7 +7973,7 @@
       <c r="A307" t="s">
         <v>280</v>
       </c>
-      <c r="C307" s="25"/>
+      <c r="C307" s="20"/>
       <c r="E307" t="s">
         <v>357</v>
       </c>
@@ -7972,7 +7985,7 @@
       <c r="A308" t="s">
         <v>281</v>
       </c>
-      <c r="C308" s="25"/>
+      <c r="C308" s="20"/>
       <c r="E308" t="s">
         <v>357</v>
       </c>
@@ -7984,7 +7997,7 @@
       <c r="A309" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="C309" s="28"/>
+      <c r="C309" s="22"/>
       <c r="E309" s="12" t="s">
         <v>364</v>
       </c>
@@ -7996,7 +8009,7 @@
       <c r="A310" t="s">
         <v>283</v>
       </c>
-      <c r="C310" s="25" t="s">
+      <c r="C310" s="20" t="s">
         <v>574</v>
       </c>
       <c r="D310" t="s">
@@ -8016,7 +8029,7 @@
       <c r="A311" t="s">
         <v>284</v>
       </c>
-      <c r="C311" s="25"/>
+      <c r="C311" s="20"/>
       <c r="D311" t="s">
         <v>732</v>
       </c>
@@ -8034,7 +8047,7 @@
       <c r="A312" t="s">
         <v>285</v>
       </c>
-      <c r="C312" s="25"/>
+      <c r="C312" s="20"/>
       <c r="D312" t="s">
         <v>735</v>
       </c>
@@ -8052,7 +8065,7 @@
       <c r="A313" t="s">
         <v>286</v>
       </c>
-      <c r="C313" s="25"/>
+      <c r="C313" s="20"/>
       <c r="D313" t="s">
         <v>736</v>
       </c>
@@ -8070,7 +8083,7 @@
       <c r="A314" t="s">
         <v>287</v>
       </c>
-      <c r="C314" s="25"/>
+      <c r="C314" s="20"/>
       <c r="D314" t="s">
         <v>737</v>
       </c>
@@ -8088,7 +8101,7 @@
       <c r="A315" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C315" s="25"/>
+      <c r="C315" s="20"/>
       <c r="D315" s="6" t="s">
         <v>738</v>
       </c>
@@ -8137,7 +8150,7 @@
       <c r="A318" t="s">
         <v>291</v>
       </c>
-      <c r="C318" s="24" t="s">
+      <c r="C318" s="19" t="s">
         <v>577</v>
       </c>
       <c r="D318" t="s">
@@ -8152,22 +8165,22 @@
       <c r="H318" t="s">
         <v>634</v>
       </c>
-      <c r="I318" s="18" t="s">
+      <c r="I318" s="24" t="s">
         <v>783</v>
       </c>
-      <c r="J318" s="18"/>
-      <c r="K318" s="18"/>
-      <c r="L318" s="18"/>
-      <c r="M318" s="21" t="s">
+      <c r="J318" s="24"/>
+      <c r="K318" s="24"/>
+      <c r="L318" s="24"/>
+      <c r="M318" s="26" t="s">
         <v>785</v>
       </c>
-      <c r="N318" s="21"/>
+      <c r="N318" s="26"/>
     </row>
     <row r="319" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" t="s">
         <v>292</v>
       </c>
-      <c r="C319" s="25"/>
+      <c r="C319" s="20"/>
       <c r="D319" t="s">
         <v>744</v>
       </c>
@@ -8180,18 +8193,18 @@
       <c r="H319" t="s">
         <v>634</v>
       </c>
-      <c r="I319" s="19"/>
-      <c r="J319" s="19"/>
-      <c r="K319" s="19"/>
-      <c r="L319" s="19"/>
-      <c r="M319" s="22"/>
-      <c r="N319" s="22"/>
+      <c r="I319" s="23"/>
+      <c r="J319" s="23"/>
+      <c r="K319" s="23"/>
+      <c r="L319" s="23"/>
+      <c r="M319" s="27"/>
+      <c r="N319" s="27"/>
     </row>
     <row r="320" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" t="s">
         <v>293</v>
       </c>
-      <c r="C320" s="25"/>
+      <c r="C320" s="20"/>
       <c r="D320" t="s">
         <v>751</v>
       </c>
@@ -8207,84 +8220,84 @@
       <c r="H320" t="s">
         <v>634</v>
       </c>
-      <c r="I320" s="19"/>
-      <c r="J320" s="19"/>
-      <c r="K320" s="19"/>
-      <c r="L320" s="19"/>
-      <c r="M320" s="22"/>
-      <c r="N320" s="22"/>
+      <c r="I320" s="23"/>
+      <c r="J320" s="23"/>
+      <c r="K320" s="23"/>
+      <c r="L320" s="23"/>
+      <c r="M320" s="27"/>
+      <c r="N320" s="27"/>
     </row>
     <row r="321" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" t="s">
         <v>294</v>
       </c>
-      <c r="C321" s="25"/>
+      <c r="C321" s="20"/>
       <c r="E321" t="s">
         <v>357</v>
       </c>
       <c r="F321" t="s">
         <v>749</v>
       </c>
-      <c r="I321" s="19"/>
-      <c r="J321" s="19"/>
-      <c r="K321" s="19"/>
-      <c r="L321" s="19"/>
-      <c r="M321" s="22"/>
-      <c r="N321" s="22"/>
+      <c r="I321" s="23"/>
+      <c r="J321" s="23"/>
+      <c r="K321" s="23"/>
+      <c r="L321" s="23"/>
+      <c r="M321" s="27"/>
+      <c r="N321" s="27"/>
     </row>
     <row r="322" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" t="s">
         <v>295</v>
       </c>
-      <c r="C322" s="25"/>
+      <c r="C322" s="20"/>
       <c r="E322" t="s">
         <v>357</v>
       </c>
       <c r="F322" t="s">
         <v>750</v>
       </c>
-      <c r="I322" s="19"/>
-      <c r="J322" s="19"/>
-      <c r="K322" s="19"/>
-      <c r="L322" s="19"/>
-      <c r="M322" s="22"/>
-      <c r="N322" s="22"/>
+      <c r="I322" s="23"/>
+      <c r="J322" s="23"/>
+      <c r="K322" s="23"/>
+      <c r="L322" s="23"/>
+      <c r="M322" s="27"/>
+      <c r="N322" s="27"/>
     </row>
     <row r="323" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" t="s">
         <v>296</v>
       </c>
-      <c r="C323" s="25"/>
+      <c r="C323" s="20"/>
       <c r="E323" t="s">
         <v>357</v>
       </c>
       <c r="F323" t="s">
         <v>663</v>
       </c>
-      <c r="I323" s="19"/>
-      <c r="J323" s="19"/>
-      <c r="K323" s="19"/>
-      <c r="L323" s="19"/>
-      <c r="M323" s="22"/>
-      <c r="N323" s="22"/>
+      <c r="I323" s="23"/>
+      <c r="J323" s="23"/>
+      <c r="K323" s="23"/>
+      <c r="L323" s="23"/>
+      <c r="M323" s="27"/>
+      <c r="N323" s="27"/>
     </row>
     <row r="324" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="C324" s="26"/>
+      <c r="C324" s="21"/>
       <c r="E324" s="6" t="s">
         <v>364</v>
       </c>
       <c r="F324" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="I324" s="20"/>
-      <c r="J324" s="20"/>
-      <c r="K324" s="20"/>
-      <c r="L324" s="20"/>
-      <c r="M324" s="23"/>
-      <c r="N324" s="23"/>
+      <c r="I324" s="25"/>
+      <c r="J324" s="25"/>
+      <c r="K324" s="25"/>
+      <c r="L324" s="25"/>
+      <c r="M324" s="28"/>
+      <c r="N324" s="28"/>
     </row>
     <row r="325" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" s="17" t="s">
@@ -8310,7 +8323,7 @@
       <c r="A326" t="s">
         <v>582</v>
       </c>
-      <c r="C326" s="24" t="s">
+      <c r="C326" s="19" t="s">
         <v>759</v>
       </c>
       <c r="D326" t="s">
@@ -8325,16 +8338,16 @@
       <c r="H326" t="s">
         <v>634</v>
       </c>
-      <c r="M326" s="21" t="s">
+      <c r="M326" s="26" t="s">
         <v>785</v>
       </c>
-      <c r="N326" s="21"/>
+      <c r="N326" s="26"/>
     </row>
     <row r="327" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" t="s">
         <v>583</v>
       </c>
-      <c r="C327" s="25"/>
+      <c r="C327" s="20"/>
       <c r="D327" t="s">
         <v>763</v>
       </c>
@@ -8347,14 +8360,14 @@
       <c r="H327" t="s">
         <v>634</v>
       </c>
-      <c r="M327" s="22"/>
-      <c r="N327" s="22"/>
+      <c r="M327" s="27"/>
+      <c r="N327" s="27"/>
     </row>
     <row r="328" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" t="s">
         <v>301</v>
       </c>
-      <c r="C328" s="25"/>
+      <c r="C328" s="20"/>
       <c r="D328" t="s">
         <v>764</v>
       </c>
@@ -8367,14 +8380,14 @@
       <c r="H328" t="s">
         <v>634</v>
       </c>
-      <c r="M328" s="22"/>
-      <c r="N328" s="22"/>
+      <c r="M328" s="27"/>
+      <c r="N328" s="27"/>
     </row>
     <row r="329" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" t="s">
         <v>302</v>
       </c>
-      <c r="C329" s="25"/>
+      <c r="C329" s="20"/>
       <c r="D329" t="s">
         <v>765</v>
       </c>
@@ -8387,14 +8400,14 @@
       <c r="H329" t="s">
         <v>634</v>
       </c>
-      <c r="M329" s="22"/>
-      <c r="N329" s="22"/>
+      <c r="M329" s="27"/>
+      <c r="N329" s="27"/>
     </row>
     <row r="330" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" t="s">
         <v>303</v>
       </c>
-      <c r="C330" s="25"/>
+      <c r="C330" s="20"/>
       <c r="D330" t="s">
         <v>766</v>
       </c>
@@ -8407,14 +8420,14 @@
       <c r="H330" t="s">
         <v>634</v>
       </c>
-      <c r="M330" s="22"/>
-      <c r="N330" s="22"/>
+      <c r="M330" s="27"/>
+      <c r="N330" s="27"/>
     </row>
     <row r="331" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" t="s">
         <v>304</v>
       </c>
-      <c r="C331" s="25"/>
+      <c r="C331" s="20"/>
       <c r="D331" t="s">
         <v>767</v>
       </c>
@@ -8427,18 +8440,18 @@
       <c r="H331" t="s">
         <v>634</v>
       </c>
-      <c r="I331" s="27" t="s">
+      <c r="I331" s="18" t="s">
         <v>779</v>
       </c>
-      <c r="J331" s="27"/>
-      <c r="M331" s="22"/>
-      <c r="N331" s="22"/>
+      <c r="J331" s="18"/>
+      <c r="M331" s="27"/>
+      <c r="N331" s="27"/>
     </row>
     <row r="332" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" t="s">
         <v>584</v>
       </c>
-      <c r="C332" s="25"/>
+      <c r="C332" s="20"/>
       <c r="D332" t="s">
         <v>768</v>
       </c>
@@ -8451,16 +8464,16 @@
       <c r="H332" t="s">
         <v>634</v>
       </c>
-      <c r="I332" s="27"/>
-      <c r="J332" s="27"/>
-      <c r="M332" s="23"/>
-      <c r="N332" s="23"/>
+      <c r="I332" s="18"/>
+      <c r="J332" s="18"/>
+      <c r="M332" s="28"/>
+      <c r="N332" s="28"/>
     </row>
     <row r="333" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" s="6" t="s">
         <v>585</v>
       </c>
-      <c r="C333" s="26"/>
+      <c r="C333" s="21"/>
       <c r="D333" s="6" t="s">
         <v>769</v>
       </c>
@@ -8473,14 +8486,14 @@
       <c r="H333" s="6" t="s">
         <v>634</v>
       </c>
-      <c r="I333" s="27"/>
-      <c r="J333" s="27"/>
+      <c r="I333" s="18"/>
+      <c r="J333" s="18"/>
     </row>
     <row r="334" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" t="s">
         <v>752</v>
       </c>
-      <c r="C334" s="24" t="s">
+      <c r="C334" s="19" t="s">
         <v>758</v>
       </c>
       <c r="E334" t="s">
@@ -8489,64 +8502,64 @@
       <c r="F334" t="s">
         <v>674</v>
       </c>
-      <c r="I334" s="27"/>
-      <c r="J334" s="27"/>
+      <c r="I334" s="18"/>
+      <c r="J334" s="18"/>
     </row>
     <row r="335" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" t="s">
         <v>753</v>
       </c>
-      <c r="C335" s="25"/>
+      <c r="C335" s="20"/>
       <c r="E335" t="s">
         <v>357</v>
       </c>
       <c r="F335" t="s">
         <v>675</v>
       </c>
-      <c r="I335" s="27"/>
-      <c r="J335" s="27"/>
+      <c r="I335" s="18"/>
+      <c r="J335" s="18"/>
     </row>
     <row r="336" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" t="s">
         <v>754</v>
       </c>
-      <c r="C336" s="25"/>
+      <c r="C336" s="20"/>
       <c r="E336" t="s">
         <v>357</v>
       </c>
       <c r="F336" t="s">
         <v>778</v>
       </c>
-      <c r="I336" s="27"/>
-      <c r="J336" s="27"/>
+      <c r="I336" s="18"/>
+      <c r="J336" s="18"/>
     </row>
     <row r="337" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" t="s">
         <v>755</v>
       </c>
-      <c r="C337" s="25"/>
+      <c r="C337" s="20"/>
       <c r="E337" t="s">
         <v>357</v>
       </c>
       <c r="F337" t="s">
         <v>663</v>
       </c>
-      <c r="I337" s="27"/>
-      <c r="J337" s="27"/>
+      <c r="I337" s="18"/>
+      <c r="J337" s="18"/>
     </row>
     <row r="338" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" s="6" t="s">
         <v>756</v>
       </c>
-      <c r="C338" s="26"/>
+      <c r="C338" s="21"/>
       <c r="E338" s="6" t="s">
         <v>364</v>
       </c>
       <c r="F338" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="I338" s="27"/>
-      <c r="J338" s="27"/>
+      <c r="I338" s="18"/>
+      <c r="J338" s="18"/>
     </row>
     <row r="339" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" t="s">
@@ -8555,7 +8568,7 @@
       <c r="B339" t="s">
         <v>582</v>
       </c>
-      <c r="C339" s="24" t="s">
+      <c r="C339" s="19" t="s">
         <v>757</v>
       </c>
       <c r="D339" t="s">
@@ -8570,12 +8583,12 @@
       <c r="H339" t="s">
         <v>634</v>
       </c>
-      <c r="I339" s="27"/>
-      <c r="J339" s="27"/>
-      <c r="M339" s="21" t="s">
+      <c r="I339" s="18"/>
+      <c r="J339" s="18"/>
+      <c r="M339" s="26" t="s">
         <v>785</v>
       </c>
-      <c r="N339" s="21"/>
+      <c r="N339" s="26"/>
     </row>
     <row r="340" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" t="s">
@@ -8584,7 +8597,7 @@
       <c r="B340" t="s">
         <v>583</v>
       </c>
-      <c r="C340" s="25"/>
+      <c r="C340" s="20"/>
       <c r="D340" t="s">
         <v>763</v>
       </c>
@@ -8597,16 +8610,16 @@
       <c r="H340" t="s">
         <v>634</v>
       </c>
-      <c r="I340" s="27"/>
-      <c r="J340" s="27"/>
-      <c r="M340" s="22"/>
-      <c r="N340" s="22"/>
+      <c r="I340" s="18"/>
+      <c r="J340" s="18"/>
+      <c r="M340" s="27"/>
+      <c r="N340" s="27"/>
     </row>
     <row r="341" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" t="s">
         <v>301</v>
       </c>
-      <c r="C341" s="25"/>
+      <c r="C341" s="20"/>
       <c r="D341" t="s">
         <v>764</v>
       </c>
@@ -8619,16 +8632,16 @@
       <c r="H341" t="s">
         <v>634</v>
       </c>
-      <c r="I341" s="27"/>
-      <c r="J341" s="27"/>
-      <c r="M341" s="22"/>
-      <c r="N341" s="22"/>
+      <c r="I341" s="18"/>
+      <c r="J341" s="18"/>
+      <c r="M341" s="27"/>
+      <c r="N341" s="27"/>
     </row>
     <row r="342" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" t="s">
         <v>302</v>
       </c>
-      <c r="C342" s="25"/>
+      <c r="C342" s="20"/>
       <c r="D342" t="s">
         <v>765</v>
       </c>
@@ -8641,14 +8654,14 @@
       <c r="H342" t="s">
         <v>634</v>
       </c>
-      <c r="M342" s="22"/>
-      <c r="N342" s="22"/>
+      <c r="M342" s="27"/>
+      <c r="N342" s="27"/>
     </row>
     <row r="343" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" t="s">
         <v>303</v>
       </c>
-      <c r="C343" s="25"/>
+      <c r="C343" s="20"/>
       <c r="D343" t="s">
         <v>766</v>
       </c>
@@ -8661,14 +8674,14 @@
       <c r="H343" t="s">
         <v>634</v>
       </c>
-      <c r="M343" s="22"/>
-      <c r="N343" s="22"/>
+      <c r="M343" s="27"/>
+      <c r="N343" s="27"/>
     </row>
     <row r="344" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" t="s">
         <v>304</v>
       </c>
-      <c r="C344" s="25"/>
+      <c r="C344" s="20"/>
       <c r="D344" t="s">
         <v>767</v>
       </c>
@@ -8681,8 +8694,8 @@
       <c r="H344" t="s">
         <v>634</v>
       </c>
-      <c r="M344" s="22"/>
-      <c r="N344" s="22"/>
+      <c r="M344" s="27"/>
+      <c r="N344" s="27"/>
     </row>
     <row r="345" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" t="s">
@@ -8691,7 +8704,7 @@
       <c r="B345" t="s">
         <v>584</v>
       </c>
-      <c r="C345" s="25"/>
+      <c r="C345" s="20"/>
       <c r="D345" t="s">
         <v>768</v>
       </c>
@@ -8704,8 +8717,8 @@
       <c r="H345" t="s">
         <v>634</v>
       </c>
-      <c r="M345" s="23"/>
-      <c r="N345" s="23"/>
+      <c r="M345" s="28"/>
+      <c r="N345" s="28"/>
     </row>
     <row r="346" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" s="6" t="s">
@@ -8714,7 +8727,7 @@
       <c r="B346" s="6" t="s">
         <v>585</v>
       </c>
-      <c r="C346" s="26"/>
+      <c r="C346" s="21"/>
       <c r="D346" s="6" t="s">
         <v>769</v>
       </c>
@@ -8732,7 +8745,7 @@
       <c r="A347" t="s">
         <v>307</v>
       </c>
-      <c r="C347" s="24" t="s">
+      <c r="C347" s="19" t="s">
         <v>578</v>
       </c>
       <c r="E347" t="s">
@@ -8746,7 +8759,7 @@
       <c r="A348" t="s">
         <v>308</v>
       </c>
-      <c r="C348" s="25"/>
+      <c r="C348" s="20"/>
       <c r="E348" t="s">
         <v>357</v>
       </c>
@@ -8758,7 +8771,7 @@
       <c r="A349" t="s">
         <v>309</v>
       </c>
-      <c r="C349" s="25"/>
+      <c r="C349" s="20"/>
       <c r="E349" t="s">
         <v>357</v>
       </c>
@@ -8770,7 +8783,7 @@
       <c r="A350" t="s">
         <v>310</v>
       </c>
-      <c r="C350" s="25"/>
+      <c r="C350" s="20"/>
       <c r="E350" t="s">
         <v>357</v>
       </c>
@@ -8782,7 +8795,7 @@
       <c r="A351" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="C351" s="26"/>
+      <c r="C351" s="21"/>
       <c r="E351" s="6" t="s">
         <v>364</v>
       </c>
@@ -8794,7 +8807,7 @@
       <c r="A352" t="s">
         <v>312</v>
       </c>
-      <c r="C352" s="25" t="s">
+      <c r="C352" s="20" t="s">
         <v>579</v>
       </c>
       <c r="D352" t="s">
@@ -8809,22 +8822,22 @@
       <c r="H352" t="s">
         <v>636</v>
       </c>
-      <c r="I352" s="18" t="s">
+      <c r="I352" s="24" t="s">
         <v>783</v>
       </c>
-      <c r="J352" s="18"/>
-      <c r="K352" s="18"/>
-      <c r="L352" s="18"/>
-      <c r="M352" s="21" t="s">
+      <c r="J352" s="24"/>
+      <c r="K352" s="24"/>
+      <c r="L352" s="24"/>
+      <c r="M352" s="26" t="s">
         <v>785</v>
       </c>
-      <c r="N352" s="21"/>
+      <c r="N352" s="26"/>
     </row>
     <row r="353" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" t="s">
         <v>313</v>
       </c>
-      <c r="C353" s="25"/>
+      <c r="C353" s="20"/>
       <c r="D353" t="s">
         <v>781</v>
       </c>
@@ -8837,18 +8850,18 @@
       <c r="H353" t="s">
         <v>636</v>
       </c>
-      <c r="I353" s="19"/>
-      <c r="J353" s="19"/>
-      <c r="K353" s="19"/>
-      <c r="L353" s="19"/>
-      <c r="M353" s="22"/>
-      <c r="N353" s="22"/>
+      <c r="I353" s="23"/>
+      <c r="J353" s="23"/>
+      <c r="K353" s="23"/>
+      <c r="L353" s="23"/>
+      <c r="M353" s="27"/>
+      <c r="N353" s="27"/>
     </row>
     <row r="354" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" t="s">
         <v>314</v>
       </c>
-      <c r="C354" s="25"/>
+      <c r="C354" s="20"/>
       <c r="D354" t="s">
         <v>782</v>
       </c>
@@ -8864,18 +8877,18 @@
       <c r="H354" t="s">
         <v>636</v>
       </c>
-      <c r="I354" s="19"/>
-      <c r="J354" s="19"/>
-      <c r="K354" s="19"/>
-      <c r="L354" s="19"/>
-      <c r="M354" s="22"/>
-      <c r="N354" s="22"/>
+      <c r="I354" s="23"/>
+      <c r="J354" s="23"/>
+      <c r="K354" s="23"/>
+      <c r="L354" s="23"/>
+      <c r="M354" s="27"/>
+      <c r="N354" s="27"/>
     </row>
     <row r="355" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" t="s">
         <v>315</v>
       </c>
-      <c r="C355" s="25"/>
+      <c r="C355" s="20"/>
       <c r="E355" t="s">
         <v>357</v>
       </c>
@@ -8885,18 +8898,18 @@
       <c r="H355" t="s">
         <v>636</v>
       </c>
-      <c r="I355" s="19"/>
-      <c r="J355" s="19"/>
-      <c r="K355" s="19"/>
-      <c r="L355" s="19"/>
-      <c r="M355" s="22"/>
-      <c r="N355" s="22"/>
+      <c r="I355" s="23"/>
+      <c r="J355" s="23"/>
+      <c r="K355" s="23"/>
+      <c r="L355" s="23"/>
+      <c r="M355" s="27"/>
+      <c r="N355" s="27"/>
     </row>
     <row r="356" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" t="s">
         <v>316</v>
       </c>
-      <c r="C356" s="25"/>
+      <c r="C356" s="20"/>
       <c r="E356" t="s">
         <v>357</v>
       </c>
@@ -8906,18 +8919,18 @@
       <c r="H356" t="s">
         <v>636</v>
       </c>
-      <c r="I356" s="19"/>
-      <c r="J356" s="19"/>
-      <c r="K356" s="19"/>
-      <c r="L356" s="19"/>
-      <c r="M356" s="22"/>
-      <c r="N356" s="22"/>
+      <c r="I356" s="23"/>
+      <c r="J356" s="23"/>
+      <c r="K356" s="23"/>
+      <c r="L356" s="23"/>
+      <c r="M356" s="27"/>
+      <c r="N356" s="27"/>
     </row>
     <row r="357" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" t="s">
         <v>317</v>
       </c>
-      <c r="C357" s="25"/>
+      <c r="C357" s="20"/>
       <c r="E357" t="s">
         <v>357</v>
       </c>
@@ -8927,18 +8940,18 @@
       <c r="H357" t="s">
         <v>636</v>
       </c>
-      <c r="I357" s="19"/>
-      <c r="J357" s="19"/>
-      <c r="K357" s="19"/>
-      <c r="L357" s="19"/>
-      <c r="M357" s="22"/>
-      <c r="N357" s="22"/>
+      <c r="I357" s="23"/>
+      <c r="J357" s="23"/>
+      <c r="K357" s="23"/>
+      <c r="L357" s="23"/>
+      <c r="M357" s="27"/>
+      <c r="N357" s="27"/>
     </row>
     <row r="358" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A358" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="C358" s="26"/>
+      <c r="C358" s="21"/>
       <c r="E358" s="6" t="s">
         <v>364</v>
       </c>
@@ -8948,18 +8961,18 @@
       <c r="H358" s="6" t="s">
         <v>636</v>
       </c>
-      <c r="I358" s="20"/>
-      <c r="J358" s="20"/>
-      <c r="K358" s="20"/>
-      <c r="L358" s="20"/>
-      <c r="M358" s="23"/>
-      <c r="N358" s="23"/>
+      <c r="I358" s="25"/>
+      <c r="J358" s="25"/>
+      <c r="K358" s="25"/>
+      <c r="L358" s="25"/>
+      <c r="M358" s="28"/>
+      <c r="N358" s="28"/>
     </row>
     <row r="359" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" t="s">
         <v>319</v>
       </c>
-      <c r="C359" s="25" t="s">
+      <c r="C359" s="20" t="s">
         <v>580</v>
       </c>
       <c r="D359" t="s">
@@ -8979,7 +8992,7 @@
       <c r="A360" t="s">
         <v>320</v>
       </c>
-      <c r="C360" s="25"/>
+      <c r="C360" s="20"/>
       <c r="D360" t="s">
         <v>788</v>
       </c>
@@ -8997,7 +9010,7 @@
       <c r="A361" t="s">
         <v>321</v>
       </c>
-      <c r="C361" s="25"/>
+      <c r="C361" s="20"/>
       <c r="D361" t="s">
         <v>789</v>
       </c>
@@ -9015,7 +9028,7 @@
       <c r="A362" t="s">
         <v>322</v>
       </c>
-      <c r="C362" s="25"/>
+      <c r="C362" s="20"/>
       <c r="D362" t="s">
         <v>790</v>
       </c>
@@ -9033,7 +9046,7 @@
       <c r="A363" t="s">
         <v>323</v>
       </c>
-      <c r="C363" s="25"/>
+      <c r="C363" s="20"/>
       <c r="D363" t="s">
         <v>791</v>
       </c>
@@ -9051,7 +9064,7 @@
       <c r="A364" t="s">
         <v>324</v>
       </c>
-      <c r="C364" s="25"/>
+      <c r="C364" s="20"/>
       <c r="D364" t="s">
         <v>792</v>
       </c>
@@ -9069,7 +9082,7 @@
       <c r="A365" t="s">
         <v>325</v>
       </c>
-      <c r="C365" s="25"/>
+      <c r="C365" s="20"/>
       <c r="D365" t="s">
         <v>793</v>
       </c>
@@ -9087,7 +9100,7 @@
       <c r="A366" t="s">
         <v>326</v>
       </c>
-      <c r="C366" s="25"/>
+      <c r="C366" s="20"/>
       <c r="D366" t="s">
         <v>794</v>
       </c>
@@ -9105,7 +9118,7 @@
       <c r="A367" t="s">
         <v>327</v>
       </c>
-      <c r="C367" s="25"/>
+      <c r="C367" s="20"/>
       <c r="E367" t="s">
         <v>357</v>
       </c>
@@ -9117,7 +9130,7 @@
       <c r="A368" t="s">
         <v>328</v>
       </c>
-      <c r="C368" s="25"/>
+      <c r="C368" s="20"/>
       <c r="E368" t="s">
         <v>357</v>
       </c>
@@ -9129,7 +9142,7 @@
       <c r="A369" t="s">
         <v>329</v>
       </c>
-      <c r="C369" s="25"/>
+      <c r="C369" s="20"/>
       <c r="E369" t="s">
         <v>357</v>
       </c>
@@ -9141,7 +9154,7 @@
       <c r="A370" t="s">
         <v>330</v>
       </c>
-      <c r="C370" s="25"/>
+      <c r="C370" s="20"/>
       <c r="E370" t="s">
         <v>357</v>
       </c>
@@ -9153,7 +9166,7 @@
       <c r="A371" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C371" s="28"/>
+      <c r="C371" s="22"/>
       <c r="E371" s="12" t="s">
         <v>364</v>
       </c>
@@ -9163,7 +9176,49 @@
     </row>
     <row r="372" spans="1:6" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="58">
+    <mergeCell ref="I352:L358"/>
+    <mergeCell ref="I318:L324"/>
+    <mergeCell ref="M318:N324"/>
+    <mergeCell ref="M326:N332"/>
+    <mergeCell ref="M339:N345"/>
+    <mergeCell ref="M352:N358"/>
+    <mergeCell ref="I262:K265"/>
+    <mergeCell ref="C326:C333"/>
+    <mergeCell ref="C334:C338"/>
+    <mergeCell ref="I331:J341"/>
+    <mergeCell ref="I1:L12"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C41:C48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C51:C58"/>
+    <mergeCell ref="C59:C63"/>
+    <mergeCell ref="C64:C68"/>
+    <mergeCell ref="C9:C17"/>
+    <mergeCell ref="C18:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="C28:C35"/>
+    <mergeCell ref="C131:C135"/>
+    <mergeCell ref="C136:C151"/>
+    <mergeCell ref="C153:C157"/>
+    <mergeCell ref="C71:C78"/>
+    <mergeCell ref="C79:C86"/>
+    <mergeCell ref="C87:C91"/>
+    <mergeCell ref="C119:C130"/>
+    <mergeCell ref="C112:C118"/>
+    <mergeCell ref="C99:C110"/>
+    <mergeCell ref="C92:C98"/>
+    <mergeCell ref="C158:C162"/>
+    <mergeCell ref="C163:C168"/>
+    <mergeCell ref="C169:C182"/>
+    <mergeCell ref="C183:C187"/>
+    <mergeCell ref="C188:C189"/>
+    <mergeCell ref="C190:C194"/>
+    <mergeCell ref="C195:C199"/>
+    <mergeCell ref="C200:C204"/>
+    <mergeCell ref="C205:C209"/>
+    <mergeCell ref="C210:C226"/>
     <mergeCell ref="I165:M168"/>
     <mergeCell ref="C318:C324"/>
     <mergeCell ref="C347:C351"/>
@@ -9180,46 +9235,6 @@
     <mergeCell ref="C246:C247"/>
     <mergeCell ref="C248:C252"/>
     <mergeCell ref="C253:C261"/>
-    <mergeCell ref="C190:C194"/>
-    <mergeCell ref="C195:C199"/>
-    <mergeCell ref="C200:C204"/>
-    <mergeCell ref="C205:C209"/>
-    <mergeCell ref="C210:C226"/>
-    <mergeCell ref="C158:C162"/>
-    <mergeCell ref="C163:C168"/>
-    <mergeCell ref="C169:C182"/>
-    <mergeCell ref="C183:C187"/>
-    <mergeCell ref="C188:C189"/>
-    <mergeCell ref="C112:C130"/>
-    <mergeCell ref="C131:C135"/>
-    <mergeCell ref="C136:C151"/>
-    <mergeCell ref="C153:C157"/>
-    <mergeCell ref="C71:C78"/>
-    <mergeCell ref="C79:C86"/>
-    <mergeCell ref="C87:C91"/>
-    <mergeCell ref="C92:C110"/>
-    <mergeCell ref="I262:K265"/>
-    <mergeCell ref="C326:C333"/>
-    <mergeCell ref="C334:C338"/>
-    <mergeCell ref="I331:J341"/>
-    <mergeCell ref="I1:L12"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C41:C48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C51:C58"/>
-    <mergeCell ref="C59:C63"/>
-    <mergeCell ref="C64:C68"/>
-    <mergeCell ref="C9:C17"/>
-    <mergeCell ref="C18:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="C28:C35"/>
-    <mergeCell ref="I352:L358"/>
-    <mergeCell ref="I318:L324"/>
-    <mergeCell ref="M318:N324"/>
-    <mergeCell ref="M326:N332"/>
-    <mergeCell ref="M339:N345"/>
-    <mergeCell ref="M352:N358"/>
   </mergeCells>
   <conditionalFormatting sqref="I262 H1:H264 H266:H290 H292:H304 H306:H1048576">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">

</xml_diff>

<commit_message>
Finished n-back data organization, started on separating MCT practice and task data
</commit_message>
<xml_diff>
--- a/PsychoPyData_ColumnKey.xlsx
+++ b/PsychoPyData_ColumnKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofc-my.sharepoint.com/personal/chelsie_hart_ucalgary_ca/Documents/1_PhD_Project/Scripting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1832" documentId="8_{447AABAE-0265-45CA-9969-8E24E37FF3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F950BBC8-5819-4C6C-8AE9-DE80A63FCBCE}"/>
+  <xr:revisionPtr revIDLastSave="1842" documentId="8_{447AABAE-0265-45CA-9969-8E24E37FF3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF713541-C118-4576-984B-76A66E139BFB}"/>
   <bookViews>
-    <workbookView xWindow="-19330" yWindow="790" windowWidth="19360" windowHeight="19610" xr2:uid="{5015AFB7-EBCA-4E4E-B1B8-96F1F0B54514}"/>
+    <workbookView xWindow="-32940" yWindow="5230" windowWidth="19360" windowHeight="15340" xr2:uid="{5015AFB7-EBCA-4E4E-B1B8-96F1F0B54514}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="804">
   <si>
     <t>SARTkey_resp_practice.keys</t>
   </si>
@@ -2010,9 +2010,6 @@
   </si>
   <si>
     <t>NBack1PAcc</t>
-  </si>
-  <si>
-    <t>NBack1PStim (and) NBack2PStim</t>
   </si>
   <si>
     <t>(a letter)</t>
@@ -2582,6 +2579,15 @@
   </si>
   <si>
     <t>SymSpanMixPresTrialsPerSeries</t>
+  </si>
+  <si>
+    <t>NBackPStim</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>May be marked as '0' despite correctly withholding response</t>
   </si>
 </sst>
 </file>
@@ -2681,7 +2687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2741,6 +2747,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3107,11 +3117,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071F2C75-EFE1-4D36-A5E8-DE0C4083E759}">
   <dimension ref="A1:N372"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C209" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B321" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F230" sqref="F230"/>
+      <selection pane="bottomRight" activeCell="A351" sqref="A351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3152,7 +3162,7 @@
         <v>335</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
@@ -3960,7 +3970,7 @@
         <v>519</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E49" t="s">
         <v>407</v>
@@ -3981,7 +3991,7 @@
       </c>
       <c r="C50" s="26"/>
       <c r="D50" s="15" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>402</v>
@@ -4629,7 +4639,7 @@
         <v>89</v>
       </c>
       <c r="C92" s="24" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D92" t="s">
         <v>443</v>
@@ -4674,7 +4684,7 @@
       </c>
       <c r="C94" s="25"/>
       <c r="D94" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E94" t="s">
         <v>407</v>
@@ -4695,7 +4705,7 @@
       </c>
       <c r="C95" s="25"/>
       <c r="D95" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>402</v>
@@ -4823,7 +4833,7 @@
       </c>
       <c r="C101" s="25"/>
       <c r="D101" s="5" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E101" t="s">
         <v>407</v>
@@ -4844,7 +4854,7 @@
       </c>
       <c r="C102" s="25"/>
       <c r="D102" s="5" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>402</v>
@@ -5010,7 +5020,7 @@
         <v>109</v>
       </c>
       <c r="C112" s="24" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D112" t="s">
         <v>470</v>
@@ -5049,7 +5059,7 @@
       </c>
       <c r="C114" s="25"/>
       <c r="D114" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E114" t="s">
         <v>407</v>
@@ -5067,7 +5077,7 @@
       </c>
       <c r="C115" s="25"/>
       <c r="D115" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>402</v>
@@ -5192,7 +5202,7 @@
       </c>
       <c r="C121" s="25"/>
       <c r="D121" s="5" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E121" t="s">
         <v>407</v>
@@ -5213,7 +5223,7 @@
       </c>
       <c r="C122" s="25"/>
       <c r="D122" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>402</v>
@@ -5430,7 +5440,7 @@
         <v>531</v>
       </c>
       <c r="D136" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E136" t="s">
         <v>483</v>
@@ -5451,7 +5461,7 @@
       </c>
       <c r="C137" s="25"/>
       <c r="D137" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E137" t="s">
         <v>487</v>
@@ -5487,7 +5497,7 @@
       </c>
       <c r="C139" s="25"/>
       <c r="D139" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E139" t="s">
         <v>587</v>
@@ -5598,13 +5608,13 @@
       </c>
       <c r="C145" s="25"/>
       <c r="D145" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E145" t="s">
         <v>379</v>
       </c>
       <c r="F145" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G145" t="s">
         <v>489</v>
@@ -5622,7 +5632,7 @@
       </c>
       <c r="C146" s="25"/>
       <c r="D146" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E146" t="s">
         <v>487</v>
@@ -5858,7 +5868,7 @@
         <v>534</v>
       </c>
       <c r="D163" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E163" t="s">
         <v>493</v>
@@ -5910,7 +5920,7 @@
       </c>
       <c r="C166" s="25"/>
       <c r="D166" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E166" t="s">
         <v>357</v>
@@ -5987,7 +5997,7 @@
       </c>
       <c r="C170" s="25"/>
       <c r="D170" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E170" t="s">
         <v>587</v>
@@ -6098,7 +6108,7 @@
       </c>
       <c r="C176" s="25"/>
       <c r="D176" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E176" t="s">
         <v>379</v>
@@ -6122,7 +6132,7 @@
       </c>
       <c r="C177" s="25"/>
       <c r="D177" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E177" t="s">
         <v>493</v>
@@ -6288,7 +6298,7 @@
       </c>
       <c r="C189" s="26"/>
       <c r="D189" s="6" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E189" s="6" t="s">
         <v>509</v>
@@ -6397,7 +6407,7 @@
       </c>
       <c r="C197" s="25"/>
       <c r="D197" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E197" t="s">
         <v>357</v>
@@ -6468,7 +6478,7 @@
       </c>
       <c r="C202" s="25"/>
       <c r="D202" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E202" t="s">
         <v>357</v>
@@ -6778,7 +6788,7 @@
       </c>
       <c r="C221" s="25"/>
       <c r="D221" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E221" t="s">
         <v>493</v>
@@ -6808,7 +6818,7 @@
       </c>
       <c r="C223" s="25"/>
       <c r="D223" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E223" t="s">
         <v>357</v>
@@ -7038,7 +7048,7 @@
       </c>
       <c r="C238" s="25"/>
       <c r="D238" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E238" t="s">
         <v>357</v>
@@ -7352,16 +7362,16 @@
       </c>
       <c r="C260" s="25"/>
       <c r="D260" t="s">
+        <v>801</v>
+      </c>
+      <c r="E260" t="s">
         <v>658</v>
       </c>
-      <c r="E260" t="s">
+      <c r="F260" t="s">
         <v>659</v>
       </c>
-      <c r="F260" t="s">
-        <v>660</v>
-      </c>
       <c r="G260" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H260" t="s">
         <v>612</v>
@@ -7373,19 +7383,19 @@
       </c>
       <c r="C261" s="25"/>
       <c r="D261" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E261" s="6" t="s">
         <v>379</v>
       </c>
       <c r="F261" s="6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="H261" s="6" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="262" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>235</v>
       </c>
@@ -7393,13 +7403,13 @@
         <v>550</v>
       </c>
       <c r="D262" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E262" t="s">
+        <v>663</v>
+      </c>
+      <c r="F262" t="s">
         <v>664</v>
-      </c>
-      <c r="F262" t="s">
-        <v>665</v>
       </c>
       <c r="G262" t="s">
         <v>549</v>
@@ -7408,7 +7418,7 @@
         <v>614</v>
       </c>
       <c r="I262" s="19" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J262" s="19"/>
       <c r="K262" s="19"/>
@@ -7419,13 +7429,13 @@
       </c>
       <c r="C263" s="25"/>
       <c r="D263" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E263" t="s">
         <v>351</v>
       </c>
       <c r="F263" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="H263" t="s">
         <v>614</v>
@@ -7440,13 +7450,16 @@
       </c>
       <c r="C264" s="25"/>
       <c r="D264" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E264" t="s">
         <v>350</v>
       </c>
       <c r="F264" t="s">
         <v>360</v>
+      </c>
+      <c r="G264" s="29" t="s">
+        <v>803</v>
       </c>
       <c r="H264" t="s">
         <v>614</v>
@@ -7461,7 +7474,7 @@
       </c>
       <c r="C265" s="25"/>
       <c r="D265" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E265" t="s">
         <v>357</v>
@@ -7500,7 +7513,7 @@
         <v>357</v>
       </c>
       <c r="F267" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="268" spans="1:11" x14ac:dyDescent="0.35">
@@ -7533,13 +7546,13 @@
       </c>
       <c r="C270" s="25"/>
       <c r="D270" t="s">
+        <v>672</v>
+      </c>
+      <c r="E270" t="s">
+        <v>663</v>
+      </c>
+      <c r="F270" t="s">
         <v>673</v>
-      </c>
-      <c r="E270" t="s">
-        <v>664</v>
-      </c>
-      <c r="F270" t="s">
-        <v>674</v>
       </c>
       <c r="H270" t="s">
         <v>614</v>
@@ -7551,13 +7564,13 @@
       </c>
       <c r="C271" s="25"/>
       <c r="D271" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E271" t="s">
         <v>351</v>
       </c>
       <c r="F271" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H271" t="s">
         <v>614</v>
@@ -7569,13 +7582,13 @@
       </c>
       <c r="C272" s="25"/>
       <c r="D272" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E272" t="s">
         <v>350</v>
       </c>
       <c r="F272" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H272" t="s">
         <v>614</v>
@@ -7587,16 +7600,16 @@
       </c>
       <c r="C273" s="25"/>
       <c r="D273" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E273" t="s">
         <v>379</v>
       </c>
       <c r="F273" t="s">
+        <v>678</v>
+      </c>
+      <c r="G273" t="s">
         <v>679</v>
-      </c>
-      <c r="G273" t="s">
-        <v>680</v>
       </c>
       <c r="H273" t="s">
         <v>614</v>
@@ -7620,7 +7633,7 @@
       </c>
       <c r="C275" s="25"/>
       <c r="D275" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E275" t="s">
         <v>357</v>
@@ -7629,7 +7642,7 @@
         <v>653</v>
       </c>
       <c r="G275" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H275" t="s">
         <v>614</v>
@@ -7644,7 +7657,7 @@
         <v>357</v>
       </c>
       <c r="F276" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.35">
@@ -7678,14 +7691,17 @@
       <c r="C279" s="7" t="s">
         <v>551</v>
       </c>
+      <c r="D279" s="6" t="s">
+        <v>802</v>
+      </c>
       <c r="E279" s="6" t="s">
         <v>364</v>
       </c>
       <c r="F279" s="6" t="s">
+        <v>683</v>
+      </c>
+      <c r="G279" s="6" t="s">
         <v>684</v>
-      </c>
-      <c r="G279" s="6" t="s">
-        <v>685</v>
       </c>
       <c r="H279" s="6" t="s">
         <v>614</v>
@@ -7699,13 +7715,13 @@
         <v>552</v>
       </c>
       <c r="D280" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E280" t="s">
         <v>351</v>
       </c>
       <c r="F280" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="H280" t="s">
         <v>612</v>
@@ -7717,7 +7733,7 @@
       </c>
       <c r="C281" s="25"/>
       <c r="D281" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E281" t="s">
         <v>350</v>
@@ -7747,7 +7763,7 @@
       </c>
       <c r="C283" s="25"/>
       <c r="D283" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E283" t="s">
         <v>357</v>
@@ -7804,13 +7820,13 @@
       </c>
       <c r="C287" s="26"/>
       <c r="D287" s="6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E287" s="6" t="s">
         <v>379</v>
       </c>
       <c r="F287" s="6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="H287" s="6" t="s">
         <v>612</v>
@@ -7824,13 +7840,13 @@
         <v>553</v>
       </c>
       <c r="D288" t="s">
+        <v>691</v>
+      </c>
+      <c r="E288" t="s">
+        <v>663</v>
+      </c>
+      <c r="F288" t="s">
         <v>692</v>
-      </c>
-      <c r="E288" t="s">
-        <v>664</v>
-      </c>
-      <c r="F288" t="s">
-        <v>693</v>
       </c>
       <c r="G288" t="s">
         <v>549</v>
@@ -7845,13 +7861,13 @@
       </c>
       <c r="C289" s="25"/>
       <c r="D289" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E289" t="s">
         <v>351</v>
       </c>
       <c r="F289" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H289" t="s">
         <v>614</v>
@@ -7863,13 +7879,16 @@
       </c>
       <c r="C290" s="25"/>
       <c r="D290" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E290" t="s">
         <v>350</v>
       </c>
       <c r="F290" t="s">
         <v>360</v>
+      </c>
+      <c r="G290" t="s">
+        <v>803</v>
       </c>
       <c r="H290" t="s">
         <v>614</v>
@@ -7881,7 +7900,7 @@
       </c>
       <c r="C291" s="25"/>
       <c r="D291" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E291" t="s">
         <v>357</v>
@@ -7917,7 +7936,7 @@
         <v>357</v>
       </c>
       <c r="F293" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="294" spans="1:8" x14ac:dyDescent="0.35">
@@ -7950,13 +7969,13 @@
       </c>
       <c r="C296" s="25"/>
       <c r="D296" t="s">
+        <v>697</v>
+      </c>
+      <c r="E296" t="s">
+        <v>663</v>
+      </c>
+      <c r="F296" t="s">
         <v>698</v>
-      </c>
-      <c r="E296" t="s">
-        <v>664</v>
-      </c>
-      <c r="F296" t="s">
-        <v>699</v>
       </c>
       <c r="H296" t="s">
         <v>614</v>
@@ -7968,13 +7987,13 @@
       </c>
       <c r="C297" s="25"/>
       <c r="D297" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E297" t="s">
         <v>351</v>
       </c>
       <c r="F297" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="H297" t="s">
         <v>614</v>
@@ -7986,13 +8005,13 @@
       </c>
       <c r="C298" s="25"/>
       <c r="D298" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E298" t="s">
         <v>350</v>
       </c>
       <c r="F298" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H298" t="s">
         <v>614</v>
@@ -8016,7 +8035,7 @@
       </c>
       <c r="C300" s="25"/>
       <c r="D300" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E300" t="s">
         <v>357</v>
@@ -8025,7 +8044,7 @@
         <v>653</v>
       </c>
       <c r="G300" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H300" t="s">
         <v>614</v>
@@ -8040,7 +8059,7 @@
         <v>357</v>
       </c>
       <c r="F301" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="302" spans="1:8" x14ac:dyDescent="0.35">
@@ -8073,16 +8092,16 @@
       </c>
       <c r="C304" s="26"/>
       <c r="D304" s="6" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E304" s="6" t="s">
         <v>379</v>
       </c>
       <c r="F304" s="6" t="s">
+        <v>678</v>
+      </c>
+      <c r="G304" s="6" t="s">
         <v>679</v>
-      </c>
-      <c r="G304" s="6" t="s">
-        <v>680</v>
       </c>
       <c r="H304" s="6" t="s">
         <v>614</v>
@@ -8106,7 +8125,7 @@
       <c r="A306" t="s">
         <v>279</v>
       </c>
-      <c r="C306" s="25"/>
+      <c r="C306" s="30"/>
       <c r="E306" t="s">
         <v>357</v>
       </c>
@@ -8118,7 +8137,7 @@
       <c r="A307" t="s">
         <v>280</v>
       </c>
-      <c r="C307" s="25"/>
+      <c r="C307" s="30"/>
       <c r="E307" t="s">
         <v>357</v>
       </c>
@@ -8130,7 +8149,7 @@
       <c r="A308" t="s">
         <v>281</v>
       </c>
-      <c r="C308" s="25"/>
+      <c r="C308" s="30"/>
       <c r="E308" t="s">
         <v>357</v>
       </c>
@@ -8138,33 +8157,33 @@
         <v>639</v>
       </c>
     </row>
-    <row r="309" spans="1:14" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A309" s="12" t="s">
+    <row r="309" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A309" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="C309" s="28"/>
-      <c r="E309" s="12" t="s">
+      <c r="C309" s="26"/>
+      <c r="E309" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="F309" s="12" t="s">
+      <c r="F309" s="6" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="310" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>283</v>
       </c>
-      <c r="C310" s="25" t="s">
+      <c r="C310" s="30" t="s">
         <v>555</v>
       </c>
       <c r="D310" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E310" t="s">
         <v>402</v>
       </c>
       <c r="F310" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="H310" t="s">
         <v>612</v>
@@ -8174,15 +8193,15 @@
       <c r="A311" t="s">
         <v>284</v>
       </c>
-      <c r="C311" s="25"/>
+      <c r="C311" s="30"/>
       <c r="D311" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E311" t="s">
         <v>379</v>
       </c>
       <c r="F311" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H311" t="s">
         <v>612</v>
@@ -8192,15 +8211,15 @@
       <c r="A312" t="s">
         <v>285</v>
       </c>
-      <c r="C312" s="25"/>
+      <c r="C312" s="30"/>
       <c r="D312" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E312" t="s">
         <v>402</v>
       </c>
       <c r="F312" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="H312" t="s">
         <v>612</v>
@@ -8210,15 +8229,15 @@
       <c r="A313" t="s">
         <v>286</v>
       </c>
-      <c r="C313" s="25"/>
+      <c r="C313" s="30"/>
       <c r="D313" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E313" t="s">
         <v>379</v>
       </c>
       <c r="F313" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H313" t="s">
         <v>612</v>
@@ -8228,39 +8247,39 @@
       <c r="A314" t="s">
         <v>287</v>
       </c>
-      <c r="C314" s="25"/>
+      <c r="C314" s="30"/>
       <c r="D314" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E314" t="s">
         <v>402</v>
       </c>
       <c r="F314" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="H314" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="315" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A315" s="6" t="s">
+    <row r="315" spans="1:14" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A315" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="C315" s="25"/>
-      <c r="D315" s="6" t="s">
-        <v>712</v>
-      </c>
-      <c r="E315" s="6" t="s">
+      <c r="C315" s="28"/>
+      <c r="D315" s="12" t="s">
+        <v>711</v>
+      </c>
+      <c r="E315" s="12" t="s">
         <v>379</v>
       </c>
-      <c r="F315" s="6" t="s">
-        <v>708</v>
-      </c>
-      <c r="H315" s="6" t="s">
+      <c r="F315" s="12" t="s">
+        <v>707</v>
+      </c>
+      <c r="H315" s="12" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="316" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:14" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A316" s="6" t="s">
         <v>289</v>
       </c>
@@ -8268,13 +8287,13 @@
         <v>556</v>
       </c>
       <c r="D316" s="6" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E316" s="6" t="s">
+        <v>712</v>
+      </c>
+      <c r="F316" s="6" t="s">
         <v>713</v>
-      </c>
-      <c r="F316" s="6" t="s">
-        <v>714</v>
       </c>
       <c r="H316" s="6" t="s">
         <v>613</v>
@@ -8288,7 +8307,7 @@
         <v>557</v>
       </c>
       <c r="F317" s="6" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="318" spans="1:14" x14ac:dyDescent="0.35">
@@ -8299,25 +8318,25 @@
         <v>558</v>
       </c>
       <c r="D318" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E318" t="s">
+        <v>718</v>
+      </c>
+      <c r="F318" t="s">
         <v>719</v>
-      </c>
-      <c r="F318" t="s">
-        <v>720</v>
       </c>
       <c r="H318" t="s">
         <v>612</v>
       </c>
       <c r="I318" s="18" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="J318" s="18"/>
       <c r="K318" s="18"/>
       <c r="L318" s="18"/>
       <c r="M318" s="21" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="N318" s="21"/>
     </row>
@@ -8327,13 +8346,13 @@
       </c>
       <c r="C319" s="25"/>
       <c r="D319" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E319" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F319" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="H319" t="s">
         <v>612</v>
@@ -8351,13 +8370,13 @@
       </c>
       <c r="C320" s="25"/>
       <c r="D320" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E320" t="s">
         <v>357</v>
       </c>
       <c r="F320" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="G320" s="2" t="s">
         <v>362</v>
@@ -8381,7 +8400,7 @@
         <v>357</v>
       </c>
       <c r="F321" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="I321" s="19"/>
       <c r="J321" s="19"/>
@@ -8399,7 +8418,7 @@
         <v>357</v>
       </c>
       <c r="F322" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="I322" s="19"/>
       <c r="J322" s="19"/>
@@ -8452,13 +8471,13 @@
         <v>562</v>
       </c>
       <c r="D325" s="17" t="s">
+        <v>733</v>
+      </c>
+      <c r="E325" s="17" t="s">
+        <v>750</v>
+      </c>
+      <c r="F325" s="17" t="s">
         <v>734</v>
-      </c>
-      <c r="E325" s="17" t="s">
-        <v>751</v>
-      </c>
-      <c r="F325" s="17" t="s">
-        <v>735</v>
       </c>
       <c r="H325" s="17" t="s">
         <v>613</v>
@@ -8469,22 +8488,22 @@
         <v>563</v>
       </c>
       <c r="C326" s="24" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D326" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E326" t="s">
+        <v>745</v>
+      </c>
+      <c r="F326" t="s">
         <v>746</v>
-      </c>
-      <c r="F326" t="s">
-        <v>747</v>
       </c>
       <c r="H326" t="s">
         <v>612</v>
       </c>
       <c r="M326" s="21" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="N326" s="21"/>
     </row>
@@ -8494,13 +8513,13 @@
       </c>
       <c r="C327" s="25"/>
       <c r="D327" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E327" t="s">
         <v>379</v>
       </c>
       <c r="F327" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H327" t="s">
         <v>612</v>
@@ -8514,13 +8533,13 @@
       </c>
       <c r="C328" s="25"/>
       <c r="D328" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E328" t="s">
         <v>402</v>
       </c>
       <c r="F328" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="H328" t="s">
         <v>612</v>
@@ -8534,13 +8553,13 @@
       </c>
       <c r="C329" s="25"/>
       <c r="D329" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E329" t="s">
         <v>379</v>
       </c>
       <c r="F329" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H329" t="s">
         <v>612</v>
@@ -8554,13 +8573,13 @@
       </c>
       <c r="C330" s="25"/>
       <c r="D330" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E330" t="s">
         <v>402</v>
       </c>
       <c r="F330" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="H330" t="s">
         <v>612</v>
@@ -8574,19 +8593,19 @@
       </c>
       <c r="C331" s="25"/>
       <c r="D331" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E331" t="s">
         <v>379</v>
       </c>
       <c r="F331" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H331" t="s">
         <v>612</v>
       </c>
       <c r="I331" s="27" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="J331" s="27"/>
       <c r="M331" s="22"/>
@@ -8598,13 +8617,13 @@
       </c>
       <c r="C332" s="25"/>
       <c r="D332" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E332" t="s">
         <v>402</v>
       </c>
       <c r="F332" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="H332" t="s">
         <v>612</v>
@@ -8620,13 +8639,13 @@
       </c>
       <c r="C333" s="26"/>
       <c r="D333" s="6" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E333" s="6" t="s">
         <v>379</v>
       </c>
       <c r="F333" s="6" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H333" s="6" t="s">
         <v>612</v>
@@ -8636,10 +8655,10 @@
     </row>
     <row r="334" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C334" s="24" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E334" t="s">
         <v>357</v>
@@ -8652,7 +8671,7 @@
     </row>
     <row r="335" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C335" s="25"/>
       <c r="E335" t="s">
@@ -8666,21 +8685,21 @@
     </row>
     <row r="336" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C336" s="25"/>
       <c r="E336" t="s">
         <v>357</v>
       </c>
       <c r="F336" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="I336" s="27"/>
       <c r="J336" s="27"/>
     </row>
     <row r="337" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C337" s="25"/>
       <c r="E337" t="s">
@@ -8694,7 +8713,7 @@
     </row>
     <row r="338" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A338" s="6" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C338" s="26"/>
       <c r="E338" s="6" t="s">
@@ -8714,16 +8733,16 @@
         <v>563</v>
       </c>
       <c r="C339" s="24" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D339" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E339" t="s">
+        <v>745</v>
+      </c>
+      <c r="F339" t="s">
         <v>746</v>
-      </c>
-      <c r="F339" t="s">
-        <v>747</v>
       </c>
       <c r="H339" t="s">
         <v>612</v>
@@ -8731,7 +8750,7 @@
       <c r="I339" s="27"/>
       <c r="J339" s="27"/>
       <c r="M339" s="21" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="N339" s="21"/>
     </row>
@@ -8744,13 +8763,13 @@
       </c>
       <c r="C340" s="25"/>
       <c r="D340" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E340" t="s">
         <v>379</v>
       </c>
       <c r="F340" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H340" t="s">
         <v>612</v>
@@ -8766,13 +8785,13 @@
       </c>
       <c r="C341" s="25"/>
       <c r="D341" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E341" t="s">
         <v>402</v>
       </c>
       <c r="F341" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="H341" t="s">
         <v>612</v>
@@ -8788,13 +8807,13 @@
       </c>
       <c r="C342" s="25"/>
       <c r="D342" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E342" t="s">
         <v>379</v>
       </c>
       <c r="F342" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H342" t="s">
         <v>612</v>
@@ -8808,13 +8827,13 @@
       </c>
       <c r="C343" s="25"/>
       <c r="D343" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E343" t="s">
         <v>402</v>
       </c>
       <c r="F343" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="H343" t="s">
         <v>612</v>
@@ -8828,13 +8847,13 @@
       </c>
       <c r="C344" s="25"/>
       <c r="D344" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E344" t="s">
         <v>379</v>
       </c>
       <c r="F344" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H344" t="s">
         <v>612</v>
@@ -8851,13 +8870,13 @@
       </c>
       <c r="C345" s="25"/>
       <c r="D345" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E345" t="s">
         <v>402</v>
       </c>
       <c r="F345" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="H345" t="s">
         <v>612</v>
@@ -8874,13 +8893,13 @@
       </c>
       <c r="C346" s="26"/>
       <c r="D346" s="6" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E346" s="6" t="s">
         <v>379</v>
       </c>
       <c r="F346" s="6" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H346" s="6" t="s">
         <v>612</v>
@@ -8921,7 +8940,7 @@
         <v>357</v>
       </c>
       <c r="F349" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="350" spans="1:14" x14ac:dyDescent="0.35">
@@ -8956,25 +8975,25 @@
         <v>560</v>
       </c>
       <c r="D352" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E352" t="s">
+        <v>718</v>
+      </c>
+      <c r="F352" t="s">
         <v>719</v>
-      </c>
-      <c r="F352" t="s">
-        <v>720</v>
       </c>
       <c r="H352" t="s">
         <v>614</v>
       </c>
       <c r="I352" s="18" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="J352" s="18"/>
       <c r="K352" s="18"/>
       <c r="L352" s="18"/>
       <c r="M352" s="21" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="N352" s="21"/>
     </row>
@@ -8984,13 +9003,13 @@
       </c>
       <c r="C353" s="25"/>
       <c r="D353" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E353" t="s">
         <v>379</v>
       </c>
       <c r="F353" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="H353" t="s">
         <v>614</v>
@@ -9008,16 +9027,16 @@
       </c>
       <c r="C354" s="25"/>
       <c r="D354" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E354" t="s">
         <v>357</v>
       </c>
       <c r="F354" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="G354" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="H354" t="s">
         <v>614</v>
@@ -9038,7 +9057,7 @@
         <v>357</v>
       </c>
       <c r="F355" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H355" t="s">
         <v>614</v>
@@ -9059,7 +9078,7 @@
         <v>357</v>
       </c>
       <c r="F356" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="H356" t="s">
         <v>614</v>
@@ -9121,13 +9140,13 @@
         <v>561</v>
       </c>
       <c r="D359" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E359" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F359" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H359" t="s">
         <v>614</v>
@@ -9139,13 +9158,13 @@
       </c>
       <c r="C360" s="25"/>
       <c r="D360" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E360" t="s">
         <v>379</v>
       </c>
       <c r="F360" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H360" t="s">
         <v>614</v>
@@ -9157,13 +9176,13 @@
       </c>
       <c r="C361" s="25"/>
       <c r="D361" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E361" t="s">
         <v>402</v>
       </c>
       <c r="F361" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="H361" t="s">
         <v>614</v>
@@ -9175,13 +9194,13 @@
       </c>
       <c r="C362" s="25"/>
       <c r="D362" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E362" t="s">
         <v>379</v>
       </c>
       <c r="F362" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H362" t="s">
         <v>614</v>
@@ -9193,13 +9212,13 @@
       </c>
       <c r="C363" s="25"/>
       <c r="D363" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E363" t="s">
         <v>402</v>
       </c>
       <c r="F363" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="H363" t="s">
         <v>614</v>
@@ -9211,13 +9230,13 @@
       </c>
       <c r="C364" s="25"/>
       <c r="D364" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E364" t="s">
         <v>379</v>
       </c>
       <c r="F364" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H364" t="s">
         <v>614</v>
@@ -9229,13 +9248,13 @@
       </c>
       <c r="C365" s="25"/>
       <c r="D365" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E365" t="s">
         <v>402</v>
       </c>
       <c r="F365" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H365" t="s">
         <v>614</v>
@@ -9247,13 +9266,13 @@
       </c>
       <c r="C366" s="25"/>
       <c r="D366" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E366" t="s">
         <v>379</v>
       </c>
       <c r="F366" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H366" t="s">
         <v>614</v>
@@ -9292,7 +9311,7 @@
         <v>357</v>
       </c>
       <c r="F369" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="370" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Encountered an issue where function nrows didn't exist, not sure what toolbox that was in, changed all nrows to height instead. MCT data separated into practice and task, currently working on shifting rows to match probe with trial and remove extra rows.
</commit_message>
<xml_diff>
--- a/PsychoPyData_ColumnKey.xlsx
+++ b/PsychoPyData_ColumnKey.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1842" documentId="8_{447AABAE-0265-45CA-9969-8E24E37FF3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF713541-C118-4576-984B-76A66E139BFB}"/>
   <bookViews>
-    <workbookView xWindow="-32940" yWindow="5230" windowWidth="19360" windowHeight="15340" xr2:uid="{5015AFB7-EBCA-4E4E-B1B8-96F1F0B54514}"/>
+    <workbookView xWindow="264" yWindow="1158" windowWidth="8304" windowHeight="12090" xr2:uid="{5015AFB7-EBCA-4E4E-B1B8-96F1F0B54514}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2687,7 +2687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2747,10 +2747,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3117,26 +3113,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071F2C75-EFE1-4D36-A5E8-DE0C4083E759}">
   <dimension ref="A1:N372"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B321" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C346" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A351" sqref="A351"/>
+      <selection pane="bottomRight" activeCell="D359" sqref="D359:D366"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="31.90625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.36328125" customWidth="1"/>
+    <col min="1" max="1" width="26.62890625" customWidth="1"/>
+    <col min="2" max="2" width="10.5234375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="31.89453125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.3671875" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="36.6328125" customWidth="1"/>
-    <col min="7" max="7" width="25.36328125" customWidth="1"/>
-    <col min="8" max="8" width="37.54296875" customWidth="1"/>
+    <col min="6" max="6" width="36.62890625" customWidth="1"/>
+    <col min="7" max="7" width="25.3671875" customWidth="1"/>
+    <col min="8" max="8" width="37.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>567</v>
       </c>
@@ -3168,7 +3164,7 @@
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>343</v>
       </c>
@@ -3189,7 +3185,7 @@
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3210,7 +3206,7 @@
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -3231,7 +3227,7 @@
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3252,7 +3248,7 @@
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -3273,7 +3269,7 @@
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -3294,7 +3290,7 @@
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="1:12" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" s="12" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="12" t="s">
         <v>15</v>
       </c>
@@ -3316,7 +3312,7 @@
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -3334,7 +3330,7 @@
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -3353,7 +3349,7 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3372,7 +3368,7 @@
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -3391,7 +3387,7 @@
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -3403,7 +3399,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -3418,7 +3414,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -3433,7 +3429,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -3448,7 +3444,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" s="12" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A17" s="12" t="s">
         <v>37</v>
       </c>
@@ -3463,7 +3459,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -3483,7 +3479,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -3501,7 +3497,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -3522,7 +3518,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -3534,7 +3530,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -3549,7 +3545,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -3570,7 +3566,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -3582,7 +3578,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="6" t="s">
         <v>7</v>
       </c>
@@ -3594,7 +3590,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -3617,7 +3613,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="6" t="s">
         <v>9</v>
       </c>
@@ -3638,7 +3634,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -3661,7 +3657,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -3679,7 +3675,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -3697,7 +3693,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -3709,7 +3705,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -3721,7 +3717,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -3742,7 +3738,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -3754,7 +3750,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="6" t="s">
         <v>23</v>
       </c>
@@ -3766,7 +3762,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -3780,7 +3776,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -3792,7 +3788,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -3804,7 +3800,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>27</v>
       </c>
@@ -3816,7 +3812,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:8" s="12" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A40" s="12" t="s">
         <v>28</v>
       </c>
@@ -3828,7 +3824,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -3851,7 +3847,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -3872,7 +3868,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -3893,7 +3889,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -3905,7 +3901,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -3917,7 +3913,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -3938,7 +3934,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -3950,7 +3946,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="6" t="s">
         <v>45</v>
       </c>
@@ -3962,7 +3958,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -3985,7 +3981,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="6" t="s">
         <v>47</v>
       </c>
@@ -4006,7 +4002,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -4029,7 +4025,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -4050,7 +4046,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -4071,7 +4067,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -4083,7 +4079,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -4095,7 +4091,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -4116,7 +4112,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -4128,7 +4124,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="6" t="s">
         <v>55</v>
       </c>
@@ -4140,7 +4136,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -4154,7 +4150,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -4166,7 +4162,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -4178,7 +4174,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -4190,7 +4186,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="6" t="s">
         <v>60</v>
       </c>
@@ -4202,7 +4198,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -4216,7 +4212,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -4228,7 +4224,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -4243,7 +4239,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -4258,7 +4254,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="6" t="s">
         <v>65</v>
       </c>
@@ -4270,7 +4266,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2" t="s">
         <v>66</v>
       </c>
@@ -4288,7 +4284,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="10" t="s">
         <v>67</v>
       </c>
@@ -4304,7 +4300,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -4327,7 +4323,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -4348,7 +4344,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -4369,7 +4365,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -4381,7 +4377,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -4393,7 +4389,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -4414,7 +4410,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -4426,7 +4422,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="6" t="s">
         <v>75</v>
       </c>
@@ -4438,7 +4434,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -4461,7 +4457,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -4482,7 +4478,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -4503,7 +4499,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -4515,7 +4511,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>80</v>
       </c>
@@ -4527,7 +4523,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>81</v>
       </c>
@@ -4548,7 +4544,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>82</v>
       </c>
@@ -4560,7 +4556,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="6" t="s">
         <v>83</v>
       </c>
@@ -4572,7 +4568,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>84</v>
       </c>
@@ -4586,7 +4582,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>85</v>
       </c>
@@ -4598,7 +4594,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>86</v>
       </c>
@@ -4610,7 +4606,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>87</v>
       </c>
@@ -4622,7 +4618,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="91" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="6" t="s">
         <v>88</v>
       </c>
@@ -4634,7 +4630,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>89</v>
       </c>
@@ -4657,7 +4653,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>90</v>
       </c>
@@ -4678,7 +4674,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>91</v>
       </c>
@@ -4699,7 +4695,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>92</v>
       </c>
@@ -4720,7 +4716,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>93</v>
       </c>
@@ -4741,7 +4737,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>94</v>
       </c>
@@ -4762,7 +4758,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="98" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="6" t="s">
         <v>95</v>
       </c>
@@ -4783,7 +4779,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>96</v>
       </c>
@@ -4806,7 +4802,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>97</v>
       </c>
@@ -4827,7 +4823,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>98</v>
       </c>
@@ -4848,7 +4844,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>99</v>
       </c>
@@ -4869,7 +4865,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>100</v>
       </c>
@@ -4890,7 +4886,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
         <v>101</v>
       </c>
@@ -4911,7 +4907,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>102</v>
       </c>
@@ -4932,7 +4928,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>103</v>
       </c>
@@ -4944,7 +4940,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
         <v>104</v>
       </c>
@@ -4956,7 +4952,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
         <v>105</v>
       </c>
@@ -4977,7 +4973,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
         <v>106</v>
       </c>
@@ -4989,7 +4985,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="110" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="6" t="s">
         <v>107</v>
       </c>
@@ -5001,7 +4997,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="111" spans="1:8" s="6" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" s="6" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="6" t="s">
         <v>108</v>
       </c>
@@ -5015,7 +5011,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
         <v>109</v>
       </c>
@@ -5035,7 +5031,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
         <v>110</v>
       </c>
@@ -5053,7 +5049,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
         <v>111</v>
       </c>
@@ -5071,7 +5067,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
         <v>112</v>
       </c>
@@ -5089,7 +5085,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
         <v>113</v>
       </c>
@@ -5110,7 +5106,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
         <v>114</v>
       </c>
@@ -5131,7 +5127,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="118" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="6" t="s">
         <v>115</v>
       </c>
@@ -5152,7 +5148,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>116</v>
       </c>
@@ -5175,7 +5171,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
         <v>117</v>
       </c>
@@ -5196,7 +5192,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
         <v>118</v>
       </c>
@@ -5217,7 +5213,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
         <v>119</v>
       </c>
@@ -5238,7 +5234,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
         <v>120</v>
       </c>
@@ -5259,7 +5255,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
         <v>121</v>
       </c>
@@ -5280,7 +5276,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
         <v>122</v>
       </c>
@@ -5301,7 +5297,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
         <v>123</v>
       </c>
@@ -5313,7 +5309,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
         <v>124</v>
       </c>
@@ -5325,7 +5321,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
         <v>125</v>
       </c>
@@ -5346,7 +5342,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
         <v>126</v>
       </c>
@@ -5358,7 +5354,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="130" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="6" t="s">
         <v>127</v>
       </c>
@@ -5370,7 +5366,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
         <v>128</v>
       </c>
@@ -5384,7 +5380,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
         <v>129</v>
       </c>
@@ -5396,7 +5392,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
         <v>130</v>
       </c>
@@ -5408,7 +5404,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
         <v>131</v>
       </c>
@@ -5420,7 +5416,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="135" spans="1:9" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:9" s="12" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A135" s="12" t="s">
         <v>132</v>
       </c>
@@ -5432,7 +5428,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
         <v>133</v>
       </c>
@@ -5455,7 +5451,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
         <v>134</v>
       </c>
@@ -5476,7 +5472,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" t="s">
         <v>135</v>
       </c>
@@ -5491,7 +5487,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" t="s">
         <v>136</v>
       </c>
@@ -5512,7 +5508,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="s">
         <v>615</v>
       </c>
@@ -5530,7 +5526,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="s">
         <v>616</v>
       </c>
@@ -5548,7 +5544,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" t="s">
         <v>617</v>
       </c>
@@ -5566,7 +5562,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" t="s">
         <v>618</v>
       </c>
@@ -5584,7 +5580,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" t="s">
         <v>619</v>
       </c>
@@ -5602,7 +5598,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" t="s">
         <v>620</v>
       </c>
@@ -5626,7 +5622,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="s">
         <v>137</v>
       </c>
@@ -5647,7 +5643,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
         <v>138</v>
       </c>
@@ -5659,7 +5655,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="s">
         <v>139</v>
       </c>
@@ -5671,7 +5667,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
         <v>140</v>
       </c>
@@ -5692,7 +5688,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
         <v>141</v>
       </c>
@@ -5704,7 +5700,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="151" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="6" t="s">
         <v>142</v>
       </c>
@@ -5716,7 +5712,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="152" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="6" t="s">
         <v>143</v>
       </c>
@@ -5730,7 +5726,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
         <v>144</v>
       </c>
@@ -5744,7 +5740,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
         <v>145</v>
       </c>
@@ -5756,7 +5752,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
         <v>146</v>
       </c>
@@ -5768,7 +5764,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
         <v>147</v>
       </c>
@@ -5780,7 +5776,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="157" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="6" t="s">
         <v>148</v>
       </c>
@@ -5792,7 +5788,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
         <v>149</v>
       </c>
@@ -5806,7 +5802,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" t="s">
         <v>150</v>
       </c>
@@ -5818,7 +5814,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
         <v>151</v>
       </c>
@@ -5833,7 +5829,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" t="s">
         <v>152</v>
       </c>
@@ -5848,7 +5844,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="162" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="6" t="s">
         <v>153</v>
       </c>
@@ -5860,7 +5856,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" t="s">
         <v>154</v>
       </c>
@@ -5883,7 +5879,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="s">
         <v>155</v>
       </c>
@@ -5895,7 +5891,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" t="s">
         <v>156</v>
       </c>
@@ -5914,7 +5910,7 @@
       <c r="L165" s="27"/>
       <c r="M165" s="27"/>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
         <v>157</v>
       </c>
@@ -5940,7 +5936,7 @@
       <c r="L166" s="27"/>
       <c r="M166" s="27"/>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="s">
         <v>158</v>
       </c>
@@ -5957,7 +5953,7 @@
       <c r="L167" s="27"/>
       <c r="M167" s="27"/>
     </row>
-    <row r="168" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="6" t="s">
         <v>159</v>
       </c>
@@ -5974,7 +5970,7 @@
       <c r="L168" s="27"/>
       <c r="M168" s="27"/>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
         <v>160</v>
       </c>
@@ -5991,7 +5987,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" t="s">
         <v>161</v>
       </c>
@@ -6012,7 +6008,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
         <v>598</v>
       </c>
@@ -6030,7 +6026,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="s">
         <v>599</v>
       </c>
@@ -6048,7 +6044,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
         <v>603</v>
       </c>
@@ -6066,7 +6062,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
         <v>604</v>
       </c>
@@ -6084,7 +6080,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
         <v>605</v>
       </c>
@@ -6102,7 +6098,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" t="s">
         <v>606</v>
       </c>
@@ -6126,7 +6122,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
         <v>162</v>
       </c>
@@ -6147,7 +6143,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" t="s">
         <v>163</v>
       </c>
@@ -6159,7 +6155,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" t="s">
         <v>164</v>
       </c>
@@ -6171,7 +6167,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
         <v>165</v>
       </c>
@@ -6183,7 +6179,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="s">
         <v>166</v>
       </c>
@@ -6195,7 +6191,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="182" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="6" t="s">
         <v>167</v>
       </c>
@@ -6207,7 +6203,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" t="s">
         <v>168</v>
       </c>
@@ -6221,7 +6217,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
         <v>169</v>
       </c>
@@ -6233,7 +6229,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
         <v>170</v>
       </c>
@@ -6254,7 +6250,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
         <v>171</v>
       </c>
@@ -6266,7 +6262,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="187" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="6" t="s">
         <v>172</v>
       </c>
@@ -6278,7 +6274,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" t="s">
         <v>173</v>
       </c>
@@ -6292,7 +6288,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="189" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="6" t="s">
         <v>174</v>
       </c>
@@ -6313,7 +6309,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" t="s">
         <v>175</v>
       </c>
@@ -6327,7 +6323,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" t="s">
         <v>176</v>
       </c>
@@ -6339,7 +6335,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" t="s">
         <v>177</v>
       </c>
@@ -6351,7 +6347,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" t="s">
         <v>178</v>
       </c>
@@ -6363,7 +6359,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="194" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="6" t="s">
         <v>179</v>
       </c>
@@ -6375,7 +6371,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" t="s">
         <v>180</v>
       </c>
@@ -6389,7 +6385,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" t="s">
         <v>181</v>
       </c>
@@ -6401,7 +6397,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" t="s">
         <v>182</v>
       </c>
@@ -6422,7 +6418,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" t="s">
         <v>183</v>
       </c>
@@ -6434,7 +6430,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="199" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="6" t="s">
         <v>184</v>
       </c>
@@ -6446,7 +6442,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" t="s">
         <v>185</v>
       </c>
@@ -6460,7 +6456,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" t="s">
         <v>186</v>
       </c>
@@ -6472,7 +6468,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" t="s">
         <v>187</v>
       </c>
@@ -6493,7 +6489,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" t="s">
         <v>188</v>
       </c>
@@ -6505,7 +6501,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="204" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="6" t="s">
         <v>189</v>
       </c>
@@ -6517,7 +6513,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" t="s">
         <v>190</v>
       </c>
@@ -6531,7 +6527,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" t="s">
         <v>191</v>
       </c>
@@ -6543,7 +6539,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" t="s">
         <v>192</v>
       </c>
@@ -6564,7 +6560,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" t="s">
         <v>193</v>
       </c>
@@ -6576,7 +6572,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="209" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="6" t="s">
         <v>194</v>
       </c>
@@ -6588,7 +6584,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" t="s">
         <v>195</v>
       </c>
@@ -6614,7 +6610,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" t="s">
         <v>196</v>
       </c>
@@ -6635,7 +6631,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" t="s">
         <v>197</v>
       </c>
@@ -6653,7 +6649,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" t="s">
         <v>198</v>
       </c>
@@ -6674,7 +6670,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" t="s">
         <v>621</v>
       </c>
@@ -6689,7 +6685,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" t="s">
         <v>622</v>
       </c>
@@ -6704,7 +6700,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" t="s">
         <v>623</v>
       </c>
@@ -6719,7 +6715,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" t="s">
         <v>624</v>
       </c>
@@ -6734,7 +6730,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" t="s">
         <v>625</v>
       </c>
@@ -6749,7 +6745,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" t="s">
         <v>626</v>
       </c>
@@ -6770,7 +6766,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" t="s">
         <v>199</v>
       </c>
@@ -6782,7 +6778,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" t="s">
         <v>200</v>
       </c>
@@ -6800,7 +6796,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" t="s">
         <v>201</v>
       </c>
@@ -6812,7 +6808,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" t="s">
         <v>202</v>
       </c>
@@ -6836,7 +6832,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" t="s">
         <v>203</v>
       </c>
@@ -6848,7 +6844,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" t="s">
         <v>204</v>
       </c>
@@ -6860,7 +6856,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="226" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="6" t="s">
         <v>205</v>
       </c>
@@ -6872,7 +6868,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" t="s">
         <v>206</v>
       </c>
@@ -6886,7 +6882,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" t="s">
         <v>207</v>
       </c>
@@ -6904,7 +6900,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" t="s">
         <v>628</v>
       </c>
@@ -6919,7 +6915,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" t="s">
         <v>629</v>
       </c>
@@ -6934,7 +6930,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" t="s">
         <v>630</v>
       </c>
@@ -6949,7 +6945,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" t="s">
         <v>631</v>
       </c>
@@ -6964,7 +6960,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" t="s">
         <v>632</v>
       </c>
@@ -6979,7 +6975,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" t="s">
         <v>633</v>
       </c>
@@ -7000,7 +6996,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" t="s">
         <v>208</v>
       </c>
@@ -7018,7 +7014,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" t="s">
         <v>209</v>
       </c>
@@ -7030,7 +7026,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" t="s">
         <v>210</v>
       </c>
@@ -7042,7 +7038,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" t="s">
         <v>211</v>
       </c>
@@ -7063,7 +7059,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" t="s">
         <v>212</v>
       </c>
@@ -7075,7 +7071,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="240" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="6" t="s">
         <v>213</v>
       </c>
@@ -7087,7 +7083,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" t="s">
         <v>214</v>
       </c>
@@ -7101,7 +7097,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" t="s">
         <v>215</v>
       </c>
@@ -7113,7 +7109,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" t="s">
         <v>216</v>
       </c>
@@ -7134,7 +7130,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" t="s">
         <v>217</v>
       </c>
@@ -7146,7 +7142,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="245" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="6" t="s">
         <v>218</v>
       </c>
@@ -7158,7 +7154,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" t="s">
         <v>219</v>
       </c>
@@ -7172,7 +7168,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="247" spans="1:8" s="6" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:8" s="6" customFormat="1" ht="14.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="6" t="s">
         <v>220</v>
       </c>
@@ -7187,7 +7183,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" t="s">
         <v>221</v>
       </c>
@@ -7201,7 +7197,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" t="s">
         <v>222</v>
       </c>
@@ -7213,7 +7209,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" t="s">
         <v>223</v>
       </c>
@@ -7225,7 +7221,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" t="s">
         <v>224</v>
       </c>
@@ -7237,7 +7233,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="252" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:8" s="12" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A252" s="12" t="s">
         <v>225</v>
       </c>
@@ -7249,7 +7245,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="253" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:8" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" t="s">
         <v>226</v>
       </c>
@@ -7269,7 +7265,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" t="s">
         <v>227</v>
       </c>
@@ -7287,7 +7283,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" t="s">
         <v>228</v>
       </c>
@@ -7299,7 +7295,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" t="s">
         <v>229</v>
       </c>
@@ -7320,7 +7316,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" t="s">
         <v>230</v>
       </c>
@@ -7332,7 +7328,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" t="s">
         <v>231</v>
       </c>
@@ -7344,7 +7340,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" t="s">
         <v>232</v>
       </c>
@@ -7356,7 +7352,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" t="s">
         <v>233</v>
       </c>
@@ -7377,7 +7373,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="261" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="6" t="s">
         <v>234</v>
       </c>
@@ -7395,7 +7391,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="262" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" t="s">
         <v>235</v>
       </c>
@@ -7423,7 +7419,7 @@
       <c r="J262" s="19"/>
       <c r="K262" s="19"/>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" t="s">
         <v>236</v>
       </c>
@@ -7444,7 +7440,7 @@
       <c r="J263" s="19"/>
       <c r="K263" s="19"/>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" t="s">
         <v>237</v>
       </c>
@@ -7458,7 +7454,7 @@
       <c r="F264" t="s">
         <v>360</v>
       </c>
-      <c r="G264" s="29" t="s">
+      <c r="G264" t="s">
         <v>803</v>
       </c>
       <c r="H264" t="s">
@@ -7468,7 +7464,7 @@
       <c r="J264" s="19"/>
       <c r="K264" s="19"/>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" t="s">
         <v>238</v>
       </c>
@@ -7486,7 +7482,7 @@
       <c r="J265" s="19"/>
       <c r="K265" s="19"/>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" t="s">
         <v>239</v>
       </c>
@@ -7504,7 +7500,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" t="s">
         <v>240</v>
       </c>
@@ -7516,7 +7512,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" t="s">
         <v>241</v>
       </c>
@@ -7528,7 +7524,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" t="s">
         <v>242</v>
       </c>
@@ -7540,7 +7536,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" t="s">
         <v>243</v>
       </c>
@@ -7558,7 +7554,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" t="s">
         <v>244</v>
       </c>
@@ -7576,7 +7572,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" t="s">
         <v>245</v>
       </c>
@@ -7594,7 +7590,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" t="s">
         <v>246</v>
       </c>
@@ -7615,7 +7611,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" t="s">
         <v>247</v>
       </c>
@@ -7627,7 +7623,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" t="s">
         <v>248</v>
       </c>
@@ -7648,7 +7644,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" t="s">
         <v>249</v>
       </c>
@@ -7660,7 +7656,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" t="s">
         <v>250</v>
       </c>
@@ -7672,7 +7668,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="278" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="6" t="s">
         <v>251</v>
       </c>
@@ -7684,7 +7680,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="279" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="6" t="s">
         <v>252</v>
       </c>
@@ -7707,7 +7703,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" t="s">
         <v>253</v>
       </c>
@@ -7727,7 +7723,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" t="s">
         <v>254</v>
       </c>
@@ -7745,7 +7741,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" t="s">
         <v>255</v>
       </c>
@@ -7757,7 +7753,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" t="s">
         <v>256</v>
       </c>
@@ -7778,7 +7774,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" t="s">
         <v>257</v>
       </c>
@@ -7790,7 +7786,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" t="s">
         <v>258</v>
       </c>
@@ -7802,7 +7798,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" t="s">
         <v>259</v>
       </c>
@@ -7814,7 +7810,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="287" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="6" t="s">
         <v>260</v>
       </c>
@@ -7832,7 +7828,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" t="s">
         <v>261</v>
       </c>
@@ -7855,7 +7851,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" t="s">
         <v>262</v>
       </c>
@@ -7873,7 +7869,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" t="s">
         <v>263</v>
       </c>
@@ -7894,7 +7890,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" t="s">
         <v>264</v>
       </c>
@@ -7909,7 +7905,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" t="s">
         <v>265</v>
       </c>
@@ -7927,7 +7923,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" t="s">
         <v>266</v>
       </c>
@@ -7939,7 +7935,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" t="s">
         <v>267</v>
       </c>
@@ -7951,7 +7947,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" t="s">
         <v>268</v>
       </c>
@@ -7963,7 +7959,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" t="s">
         <v>269</v>
       </c>
@@ -7981,7 +7977,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" t="s">
         <v>270</v>
       </c>
@@ -7999,7 +7995,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" t="s">
         <v>271</v>
       </c>
@@ -8017,7 +8013,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" t="s">
         <v>272</v>
       </c>
@@ -8029,7 +8025,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" t="s">
         <v>273</v>
       </c>
@@ -8050,7 +8046,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" t="s">
         <v>274</v>
       </c>
@@ -8062,7 +8058,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" t="s">
         <v>275</v>
       </c>
@@ -8074,7 +8070,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" t="s">
         <v>276</v>
       </c>
@@ -8086,7 +8082,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="304" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" s="6" t="s">
         <v>277</v>
       </c>
@@ -8107,7 +8103,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="305" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" t="s">
         <v>278</v>
       </c>
@@ -8121,11 +8117,11 @@
         <v>648</v>
       </c>
     </row>
-    <row r="306" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" t="s">
         <v>279</v>
       </c>
-      <c r="C306" s="30"/>
+      <c r="C306" s="25"/>
       <c r="E306" t="s">
         <v>357</v>
       </c>
@@ -8133,11 +8129,11 @@
         <v>649</v>
       </c>
     </row>
-    <row r="307" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" t="s">
         <v>280</v>
       </c>
-      <c r="C307" s="30"/>
+      <c r="C307" s="25"/>
       <c r="E307" t="s">
         <v>357</v>
       </c>
@@ -8145,11 +8141,11 @@
         <v>650</v>
       </c>
     </row>
-    <row r="308" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" t="s">
         <v>281</v>
       </c>
-      <c r="C308" s="30"/>
+      <c r="C308" s="25"/>
       <c r="E308" t="s">
         <v>357</v>
       </c>
@@ -8157,7 +8153,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="309" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" s="6" t="s">
         <v>282</v>
       </c>
@@ -8169,11 +8165,11 @@
         <v>365</v>
       </c>
     </row>
-    <row r="310" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" t="s">
         <v>283</v>
       </c>
-      <c r="C310" s="30" t="s">
+      <c r="C310" s="25" t="s">
         <v>555</v>
       </c>
       <c r="D310" t="s">
@@ -8189,11 +8185,11 @@
         <v>612</v>
       </c>
     </row>
-    <row r="311" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" t="s">
         <v>284</v>
       </c>
-      <c r="C311" s="30"/>
+      <c r="C311" s="25"/>
       <c r="D311" t="s">
         <v>705</v>
       </c>
@@ -8207,11 +8203,11 @@
         <v>612</v>
       </c>
     </row>
-    <row r="312" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" t="s">
         <v>285</v>
       </c>
-      <c r="C312" s="30"/>
+      <c r="C312" s="25"/>
       <c r="D312" t="s">
         <v>708</v>
       </c>
@@ -8225,11 +8221,11 @@
         <v>612</v>
       </c>
     </row>
-    <row r="313" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" t="s">
         <v>286</v>
       </c>
-      <c r="C313" s="30"/>
+      <c r="C313" s="25"/>
       <c r="D313" t="s">
         <v>709</v>
       </c>
@@ -8243,11 +8239,11 @@
         <v>612</v>
       </c>
     </row>
-    <row r="314" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" t="s">
         <v>287</v>
       </c>
-      <c r="C314" s="30"/>
+      <c r="C314" s="25"/>
       <c r="D314" t="s">
         <v>710</v>
       </c>
@@ -8261,7 +8257,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="315" spans="1:14" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="315" spans="1:14" s="12" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A315" s="12" t="s">
         <v>288</v>
       </c>
@@ -8279,7 +8275,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="316" spans="1:14" s="6" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:14" s="6" customFormat="1" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" s="6" t="s">
         <v>289</v>
       </c>
@@ -8299,7 +8295,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="317" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" s="6" t="s">
         <v>290</v>
       </c>
@@ -8310,7 +8306,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="318" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" t="s">
         <v>291</v>
       </c>
@@ -8340,7 +8336,7 @@
       </c>
       <c r="N318" s="21"/>
     </row>
-    <row r="319" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" t="s">
         <v>292</v>
       </c>
@@ -8364,7 +8360,7 @@
       <c r="M319" s="22"/>
       <c r="N319" s="22"/>
     </row>
-    <row r="320" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" t="s">
         <v>293</v>
       </c>
@@ -8391,7 +8387,7 @@
       <c r="M320" s="22"/>
       <c r="N320" s="22"/>
     </row>
-    <row r="321" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" t="s">
         <v>294</v>
       </c>
@@ -8409,7 +8405,7 @@
       <c r="M321" s="22"/>
       <c r="N321" s="22"/>
     </row>
-    <row r="322" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" t="s">
         <v>295</v>
       </c>
@@ -8427,7 +8423,7 @@
       <c r="M322" s="22"/>
       <c r="N322" s="22"/>
     </row>
-    <row r="323" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" t="s">
         <v>296</v>
       </c>
@@ -8445,7 +8441,7 @@
       <c r="M323" s="22"/>
       <c r="N323" s="22"/>
     </row>
-    <row r="324" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="6" t="s">
         <v>297</v>
       </c>
@@ -8463,7 +8459,7 @@
       <c r="M324" s="23"/>
       <c r="N324" s="23"/>
     </row>
-    <row r="325" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" s="17" t="s">
         <v>298</v>
       </c>
@@ -8483,7 +8479,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="326" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" t="s">
         <v>563</v>
       </c>
@@ -8507,7 +8503,7 @@
       </c>
       <c r="N326" s="21"/>
     </row>
-    <row r="327" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" t="s">
         <v>564</v>
       </c>
@@ -8527,7 +8523,7 @@
       <c r="M327" s="22"/>
       <c r="N327" s="22"/>
     </row>
-    <row r="328" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" t="s">
         <v>301</v>
       </c>
@@ -8547,7 +8543,7 @@
       <c r="M328" s="22"/>
       <c r="N328" s="22"/>
     </row>
-    <row r="329" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" t="s">
         <v>302</v>
       </c>
@@ -8567,7 +8563,7 @@
       <c r="M329" s="22"/>
       <c r="N329" s="22"/>
     </row>
-    <row r="330" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" t="s">
         <v>303</v>
       </c>
@@ -8587,7 +8583,7 @@
       <c r="M330" s="22"/>
       <c r="N330" s="22"/>
     </row>
-    <row r="331" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" t="s">
         <v>304</v>
       </c>
@@ -8611,7 +8607,7 @@
       <c r="M331" s="22"/>
       <c r="N331" s="22"/>
     </row>
-    <row r="332" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" t="s">
         <v>565</v>
       </c>
@@ -8633,7 +8629,7 @@
       <c r="M332" s="23"/>
       <c r="N332" s="23"/>
     </row>
-    <row r="333" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" s="6" t="s">
         <v>566</v>
       </c>
@@ -8653,7 +8649,7 @@
       <c r="I333" s="27"/>
       <c r="J333" s="27"/>
     </row>
-    <row r="334" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" t="s">
         <v>725</v>
       </c>
@@ -8669,7 +8665,7 @@
       <c r="I334" s="27"/>
       <c r="J334" s="27"/>
     </row>
-    <row r="335" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" t="s">
         <v>726</v>
       </c>
@@ -8683,7 +8679,7 @@
       <c r="I335" s="27"/>
       <c r="J335" s="27"/>
     </row>
-    <row r="336" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" t="s">
         <v>727</v>
       </c>
@@ -8697,7 +8693,7 @@
       <c r="I336" s="27"/>
       <c r="J336" s="27"/>
     </row>
-    <row r="337" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" t="s">
         <v>728</v>
       </c>
@@ -8711,7 +8707,7 @@
       <c r="I337" s="27"/>
       <c r="J337" s="27"/>
     </row>
-    <row r="338" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" s="6" t="s">
         <v>729</v>
       </c>
@@ -8725,7 +8721,7 @@
       <c r="I338" s="27"/>
       <c r="J338" s="27"/>
     </row>
-    <row r="339" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" t="s">
         <v>299</v>
       </c>
@@ -8754,7 +8750,7 @@
       </c>
       <c r="N339" s="21"/>
     </row>
-    <row r="340" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" t="s">
         <v>300</v>
       </c>
@@ -8779,7 +8775,7 @@
       <c r="M340" s="22"/>
       <c r="N340" s="22"/>
     </row>
-    <row r="341" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" t="s">
         <v>301</v>
       </c>
@@ -8801,7 +8797,7 @@
       <c r="M341" s="22"/>
       <c r="N341" s="22"/>
     </row>
-    <row r="342" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" t="s">
         <v>302</v>
       </c>
@@ -8821,7 +8817,7 @@
       <c r="M342" s="22"/>
       <c r="N342" s="22"/>
     </row>
-    <row r="343" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" t="s">
         <v>303</v>
       </c>
@@ -8841,7 +8837,7 @@
       <c r="M343" s="22"/>
       <c r="N343" s="22"/>
     </row>
-    <row r="344" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" t="s">
         <v>304</v>
       </c>
@@ -8861,7 +8857,7 @@
       <c r="M344" s="22"/>
       <c r="N344" s="22"/>
     </row>
-    <row r="345" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" t="s">
         <v>305</v>
       </c>
@@ -8884,7 +8880,7 @@
       <c r="M345" s="23"/>
       <c r="N345" s="23"/>
     </row>
-    <row r="346" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" s="6" t="s">
         <v>306</v>
       </c>
@@ -8905,7 +8901,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="347" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A347" t="s">
         <v>307</v>
       </c>
@@ -8919,7 +8915,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="348" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A348" t="s">
         <v>308</v>
       </c>
@@ -8931,7 +8927,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="349" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A349" t="s">
         <v>309</v>
       </c>
@@ -8943,7 +8939,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="350" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A350" t="s">
         <v>310</v>
       </c>
@@ -8955,7 +8951,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="351" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A351" s="6" t="s">
         <v>311</v>
       </c>
@@ -8967,7 +8963,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="352" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A352" t="s">
         <v>312</v>
       </c>
@@ -8997,7 +8993,7 @@
       </c>
       <c r="N352" s="21"/>
     </row>
-    <row r="353" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" t="s">
         <v>313</v>
       </c>
@@ -9021,7 +9017,7 @@
       <c r="M353" s="22"/>
       <c r="N353" s="22"/>
     </row>
-    <row r="354" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" t="s">
         <v>314</v>
       </c>
@@ -9048,7 +9044,7 @@
       <c r="M354" s="22"/>
       <c r="N354" s="22"/>
     </row>
-    <row r="355" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" t="s">
         <v>315</v>
       </c>
@@ -9069,7 +9065,7 @@
       <c r="M355" s="22"/>
       <c r="N355" s="22"/>
     </row>
-    <row r="356" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" t="s">
         <v>316</v>
       </c>
@@ -9090,7 +9086,7 @@
       <c r="M356" s="22"/>
       <c r="N356" s="22"/>
     </row>
-    <row r="357" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" t="s">
         <v>317</v>
       </c>
@@ -9111,7 +9107,7 @@
       <c r="M357" s="22"/>
       <c r="N357" s="22"/>
     </row>
-    <row r="358" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A358" s="6" t="s">
         <v>318</v>
       </c>
@@ -9132,7 +9128,7 @@
       <c r="M358" s="23"/>
       <c r="N358" s="23"/>
     </row>
-    <row r="359" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" t="s">
         <v>319</v>
       </c>
@@ -9152,7 +9148,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="360" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A360" t="s">
         <v>320</v>
       </c>
@@ -9170,7 +9166,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="361" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A361" t="s">
         <v>321</v>
       </c>
@@ -9188,7 +9184,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="362" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A362" t="s">
         <v>322</v>
       </c>
@@ -9206,7 +9202,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="363" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A363" t="s">
         <v>323</v>
       </c>
@@ -9224,7 +9220,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="364" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A364" t="s">
         <v>324</v>
       </c>
@@ -9242,7 +9238,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="365" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A365" t="s">
         <v>325</v>
       </c>
@@ -9260,7 +9256,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="366" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A366" t="s">
         <v>326</v>
       </c>
@@ -9278,7 +9274,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="367" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A367" t="s">
         <v>327</v>
       </c>
@@ -9290,7 +9286,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="368" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A368" t="s">
         <v>328</v>
       </c>
@@ -9302,7 +9298,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A369" t="s">
         <v>329</v>
       </c>
@@ -9314,7 +9310,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A370" t="s">
         <v>330</v>
       </c>
@@ -9326,7 +9322,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="371" spans="1:6" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="371" spans="1:6" s="12" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A371" s="12" t="s">
         <v>331</v>
       </c>
@@ -9338,7 +9334,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="372" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="372" spans="1:6" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="58">
     <mergeCell ref="I165:M168"/>

</xml_diff>